<commit_message>
More updates to `mSigHdp-paper-tracking.xlsx`
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415A4149-4F78-4B6F-8D89-C453FD66A6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A13B0BD7-3FBA-4424-B117-42C37A3C90EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="660" windowWidth="15810" windowHeight="13860" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="48">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -187,9 +187,6 @@
     <t>All 5 seeds</t>
   </si>
   <si>
-    <t>steve</t>
-  </si>
-  <si>
     <t>hpc-steve</t>
   </si>
   <si>
@@ -212,13 +209,16 @@
   </si>
   <si>
     <t>3) In the main text, we only included results summary on Realistic data set.</t>
+  </si>
+  <si>
+    <t>mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,14 +270,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -305,6 +299,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -354,41 +354,39 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -827,10 +825,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -861,7 +859,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,13 +871,13 @@
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -965,11 +963,21 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="D7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -978,19 +986,19 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1004,14 +1012,14 @@
       <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1027,7 +1035,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1052,7 +1060,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,13 +1073,13 @@
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
@@ -1175,20 +1183,20 @@
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>40</v>
+      <c r="D7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
@@ -1200,20 +1208,20 @@
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" s="19" t="s">
-        <v>40</v>
+      <c r="D8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
@@ -1252,7 +1260,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1268,10 +1276,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,13 +1289,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="19" t="s">
         <v>29</v>
       </c>
       <c r="D1" s="5"/>
@@ -1296,21 +1304,21 @@
       </c>
       <c r="F1" s="5"/>
       <c r="G1" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="20"/>
-      <c r="C2" s="11"/>
+      <c r="C2" s="19"/>
       <c r="E2" s="20"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1326,8 +1334,9 @@
         <v>38</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
+      <c r="G3" s="16" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -1346,161 +1355,298 @@
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
-        <v>38</v>
+      <c r="E5" s="2">
+        <v>145879</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+      <c r="G5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>200437</v>
+      </c>
       <c r="F6" s="2"/>
+      <c r="G6" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>38</v>
+      <c r="E7" s="2">
+        <v>310111</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
+      <c r="G7" s="17" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>528401</v>
+      </c>
       <c r="F8" s="2"/>
+      <c r="G8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2">
+        <v>1076753</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2">
+        <v>145879</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <v>200437</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
+        <v>310111</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
+        <v>528401</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2">
+        <v>1076753</v>
+      </c>
+      <c r="F16" s="2"/>
+      <c r="G16" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="F19" s="5"/>
+      <c r="G19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5" t="s">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>47</v>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A26:H26"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1518,7 +1664,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,10 +1677,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="20" t="s">
@@ -1545,27 +1691,27 @@
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="20"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" s="22" t="s">
+      <c r="F2" s="15" t="s">
         <v>44</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>43</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1586,8 +1732,12 @@
         <v>38</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="M3" s="2"/>
     </row>
@@ -1614,8 +1764,12 @@
         <v>38</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="F5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="M5" s="5"/>
     </row>
@@ -1640,8 +1794,12 @@
         <v>38</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="M7" s="5"/>
     </row>
@@ -1666,8 +1824,12 @@
         <v>38</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="F9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="M9" s="5"/>
     </row>
@@ -1692,8 +1854,7 @@
         <v>38</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
+      <c r="F11" s="5"/>
       <c r="H11" s="5"/>
       <c r="M11" s="5"/>
     </row>
@@ -1703,8 +1864,7 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="5"/>
+      <c r="F12" s="5"/>
       <c r="H12" s="5"/>
       <c r="M12" s="5"/>
     </row>
@@ -1718,8 +1878,7 @@
         <v>38</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
+      <c r="F13" s="5"/>
       <c r="H13" s="5"/>
       <c r="M13" s="5"/>
     </row>
@@ -1760,12 +1919,12 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1809,13 +1968,13 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -2023,13 +2182,13 @@
       <c r="D9" s="2">
         <v>145879</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="14" t="s">
+      <c r="E9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="22" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -2049,11 +2208,11 @@
       <c r="D10" s="2">
         <v>200437</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="22"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
@@ -2065,11 +2224,11 @@
       <c r="D11" s="2">
         <v>310111</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="14"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
@@ -2078,11 +2237,11 @@
       <c r="D12" s="2">
         <v>528401</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="14"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="22"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
@@ -2090,11 +2249,11 @@
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="14"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="22"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
@@ -2126,7 +2285,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2156,7 +2315,7 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2178,13 +2337,13 @@
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -2239,15 +2398,15 @@
       <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
       <c r="J3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2283,15 +2442,15 @@
       <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
+      <c r="E5" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="2" t="s">
         <v>2</v>
       </c>
@@ -2331,19 +2490,19 @@
       <c r="L7" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -2362,7 +2521,7 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated status of programs on data sets related to mSigHdp paper:
SigProfilerExtractor finished running on data sets SBS_2
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5649E79F-7FE5-4083-B96A-8AAD10A972BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CC254D-7DA4-47AD-9609-EA90273870C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10350" yWindow="1620" windowWidth="15810" windowHeight="13860" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="56">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -291,7 +291,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,12 +313,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,7 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -386,25 +380,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -413,36 +430,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -878,10 +865,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -912,7 +899,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" activeCellId="3" sqref="F3:H3 F5:H5 F7:H7 F9:H9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,29 +909,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -959,7 +946,7 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="16" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="2"/>
@@ -967,13 +954,13 @@
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="22"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -985,7 +972,7 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="16" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="2"/>
@@ -993,19 +980,19 @@
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="32" t="s">
+      <c r="F5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="22" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="22"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1016,19 +1003,19 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="22"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1040,7 +1027,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="16" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="5"/>
@@ -1048,13 +1035,13 @@
         <v>36</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="22"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1066,7 +1053,7 @@
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="5"/>
@@ -1082,7 +1069,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="25"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5">
         <v>200437</v>
@@ -1096,7 +1083,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="25"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5">
         <v>310111</v>
@@ -1110,7 +1097,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="25"/>
+      <c r="B14" s="24"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5">
         <v>528401</v>
@@ -1118,13 +1105,13 @@
       <c r="E14" s="5"/>
       <c r="F14" s="2"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="24" t="s">
-        <v>37</v>
+      <c r="H14" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="25"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5">
         <v>1076753</v>
@@ -1132,13 +1119,13 @@
       <c r="E15" s="5"/>
       <c r="F15" s="2"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="24" t="s">
-        <v>37</v>
+      <c r="H15" s="13" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="25"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1150,7 +1137,7 @@
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="25"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
         <v>36</v>
@@ -1158,7 +1145,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="2"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="23" t="s">
+      <c r="H17" s="17" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1199,12 +1186,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="B11:B17"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1218,8 +1205,8 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,32 +1216,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1272,7 +1259,7 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="16" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="2"/>
@@ -1280,16 +1267,16 @@
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="22"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1304,7 +1291,7 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="16" t="s">
         <v>54</v>
       </c>
       <c r="C5" s="2"/>
@@ -1312,13 +1299,13 @@
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="32" t="s">
+      <c r="H5" s="22" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="2"/>
@@ -1327,7 +1314,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="22"/>
+      <c r="B6" s="16"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1341,22 +1328,22 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="16"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="2"/>
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="22"/>
+      <c r="B8" s="16"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1371,7 +1358,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="16" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="5"/>
@@ -1379,16 +1366,16 @@
         <v>36</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="22"/>
+      <c r="B10" s="16"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1403,7 +1390,7 @@
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="5"/>
@@ -1422,7 +1409,7 @@
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="25"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1436,7 +1423,7 @@
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="25"/>
+      <c r="B13" s="24"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
         <v>36</v>
@@ -1451,7 +1438,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="26"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1464,7 +1451,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="26"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1476,13 +1463,13 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
+      <c r="B16" s="19"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="26"/>
+      <c r="B17" s="19"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1496,12 +1483,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B11:B13"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1512,10 +1499,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,30 +1513,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="25" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="5"/>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="26" t="s">
         <v>21</v>
       </c>
       <c r="F1" s="5"/>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="19"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="18"/>
-      <c r="E2" s="19"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="25"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
         <v>42</v>
@@ -1562,7 +1549,7 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="2"/>
@@ -1587,13 +1574,13 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="2">
-        <v>145879</v>
+      <c r="E5" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="8" t="s">
@@ -1608,47 +1595,33 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>200437</v>
-      </c>
+      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2">
-        <v>310111</v>
-      </c>
+      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2">
-        <v>528401</v>
+      <c r="E8" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>22</v>
+      <c r="G8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1656,16 +1629,8 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>1076753</v>
-      </c>
+      <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -1675,67 +1640,65 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="29" t="s">
-        <v>55</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="2" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="5"/>
-      <c r="G15" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
@@ -1746,91 +1709,51 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
-        <v>36</v>
-      </c>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
-      <c r="E19" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A21" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -1861,23 +1784,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="26" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="19"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
       <c r="J1" s="11"/>
@@ -1886,10 +1809,10 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="1"/>
       <c r="F2" s="12" t="s">
         <v>42</v>
@@ -1908,7 +1831,7 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="2"/>
@@ -2002,7 +1925,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C9" s="5"/>
@@ -2150,56 +2073,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="18" t="s">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="M2" s="1"/>
@@ -2208,7 +2131,7 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="18" t="s">
         <v>52</v>
       </c>
       <c r="C3" s="2"/>
@@ -2242,7 +2165,7 @@
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="24" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="2"/>
@@ -2270,7 +2193,7 @@
     </row>
     <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="28"/>
+      <c r="B5" s="24"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
         <v>310111</v>
@@ -2296,7 +2219,7 @@
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="28"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
         <v>528401</v>
@@ -2322,7 +2245,7 @@
     </row>
     <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="28"/>
+      <c r="B7" s="24"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
         <v>1076753</v>
@@ -2363,20 +2286,20 @@
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="29" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
-      <c r="E9" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
-      <c r="I9" s="21" t="s">
+      <c r="E9" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -2391,59 +2314,59 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="27"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="21"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="27"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="21"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="27"/>
+      <c r="B12" s="29"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="28"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="27"/>
+      <c r="B13" s="29"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="21"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="28"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
@@ -2525,56 +2448,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="18" t="s">
+      <c r="A1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="15">
         <v>500</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="J2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="L2" s="15" t="s">
         <v>19</v>
       </c>
       <c r="M2" s="1"/>
@@ -2583,7 +2506,7 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="2"/>
@@ -2593,12 +2516,12 @@
       <c r="E3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
       <c r="J3" s="2" t="s">
         <v>2</v>
       </c>
@@ -2637,12 +2560,12 @@
       <c r="E5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
+      <c r="F5" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="27"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27"/>
       <c r="J5" s="2" t="s">
         <v>2</v>
       </c>
@@ -2682,19 +2605,19 @@
       <c r="L7" s="5"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">

</xml_diff>

<commit_message>
Further update to `mSigHdp-paper-tracking.xlsx` -
In tab "SBS_2", I changed the color of SignatureAnalyzer, signeR, SigProfilerExtractor cells to purple (finished and reviewwed).
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CC254D-7DA4-47AD-9609-EA90273870C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CB7309-267A-456F-BEA8-C04BD3FABCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10350" yWindow="1620" windowWidth="15810" windowHeight="13860" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -413,11 +413,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -909,28 +909,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="26"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
@@ -1053,7 +1053,7 @@
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="5"/>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="24"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5">
         <v>200437</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="24"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5">
         <v>310111</v>
@@ -1097,7 +1097,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="24"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5">
         <v>528401</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="24"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5">
         <v>1076753</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="24"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1137,7 +1137,7 @@
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="24"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
         <v>36</v>
@@ -1216,31 +1216,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="26"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
@@ -1390,7 +1390,7 @@
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="5"/>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="24"/>
+      <c r="B12" s="25"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1423,7 +1423,7 @@
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="24"/>
+      <c r="B13" s="25"/>
       <c r="C13" s="5"/>
       <c r="D13" s="2" t="s">
         <v>36</v>
@@ -1483,12 +1483,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F1:H1"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
-    <mergeCell ref="F1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1501,8 +1501,8 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G11" activeCellId="2" sqref="G5:H5 G8:H8 G11:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,13 +1513,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>28</v>
       </c>
       <c r="D1" s="5"/>
@@ -1533,9 +1533,9 @@
       <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="25"/>
+      <c r="C2" s="24"/>
       <c r="E2" s="26"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
@@ -1583,10 +1583,10 @@
         <v>36</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1617,10 +1617,10 @@
         <v>36</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1653,10 +1653,10 @@
         <v>36</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="H11" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1784,10 +1784,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="26" t="s">
@@ -1809,8 +1809,8 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
       <c r="E2" s="1"/>
@@ -2077,13 +2077,13 @@
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -2165,7 +2165,7 @@
     </row>
     <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C4" s="2"/>
@@ -2193,7 +2193,7 @@
     </row>
     <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="24"/>
+      <c r="B5" s="25"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2">
         <v>310111</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="24"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2">
         <v>528401</v>
@@ -2245,7 +2245,7 @@
     </row>
     <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="24"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2">
         <v>1076753</v>
@@ -2430,7 +2430,7 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2452,13 +2452,13 @@
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
       <c r="J1" s="16"/>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>

</xml_diff>

<commit_message>
Filled in argument values for all programs and all runs.
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B222F00-EFC6-4A4D-A982-98432EA56F2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2ABE32-949E-4E0C-90BF-D970EC7587B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6645" yWindow="1665" windowWidth="21060" windowHeight="13860" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-300" yWindow="45" windowWidth="14190" windowHeight="13860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="84">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -217,13 +217,6 @@
     <t>mSigHdp = 1.1.7; hdpx = 0.3.4</t>
   </si>
   <si>
-    <t>signeR = 1.18.1; NMF = 0.30.1</t>
-  </si>
-  <si>
-    <t>mSigHdp = 2.0.1(2022-May-12);
-hdpx = 1.0.1</t>
-  </si>
-  <si>
     <t>mSigHdp = 2.0.1.10(master branch)
 hdpx = 1.0.3.9(master branch)</t>
   </si>
@@ -231,13 +224,315 @@
     <t>1.1.3(2021-Jun-18)</t>
   </si>
   <si>
-    <t>signeR = 1.20.0; NMF = 0.24.0</t>
-  </si>
-  <si>
     <t>non_hyper</t>
   </si>
   <si>
     <t>1) Filling colors: White - not started; Red - failed;  Green - running; Blue - Finished; Brown - Finished with large files downloaded; Violet - Finished with result revision; Black - Finished with result revision and image files (e.g., large Rdata file and python pickle files) downloaded</t>
+  </si>
+  <si>
+    <t>reference_genome="GRCh37",
+cosmic_version="3.2",
+context_type="ID",
+exome=False,
+minimum_signatures=2,
+maximum_signatures=20,
+nmf_replicates=100,
+resample=True,
+seeds=seeds,
+matrix_normalization="gmm",
+nmf_init="random",
+precision="single",
+min_nmf_iterations=1000,
+max_nmf_iterations=200000,
+nmf_test_conv=1000,
+nmf_tolerance=1e-08</t>
+  </si>
+  <si>
+    <t>mSigHdp = 2.0.1 (v2.0.1-branch, 2022-May-12);
+hdpx = 1.0.1 (v1.0.1-branch, 2022-May-12)</t>
+  </si>
+  <si>
+    <t>mSigHdp = 2.0.1.10(master branch);
+hdpx = 1.0.3.9(master branch)</t>
+  </si>
+  <si>
+    <t>min_K=10, max_K=40,
+reference_genome="GRCh37",
+cosmic_version="3.2",
+context_type="96",
+exome=False,
+minimum_signatures=10,
+maximum_signatures=40,
+nmf_replicates=100,
+resample=True,
+matrix_normalization="gmm",
+nmf_init="random",
+precision="single",
+min_nmf_iterations=1000,
+max_nmf_iterations=200000,
+nmf_test_conv=1000,
+nmf_tolerance=1e-08</t>
+  </si>
+  <si>
+    <t>reference_genome="GRCh37",
+cosmic_version="3.2",
+context_type="ID",
+exome=False,
+minimum_signatures=2,
+maximum_signatures=24,
+nmf_replicates=100,
+resample=True,
+seeds=seeds,
+matrix_normalization="gmm",
+nmf_init="random",
+precision="single",
+min_nmf_iterations=1000,
+max_nmf_iterations=200000,
+nmf_test_conv=1000,
+nmf_tolerance=1e-08</t>
+  </si>
+  <si>
+    <t>reference_genome="GRCh37",
+cosmic_version="3.2",
+context_type=="96",
+exome=False,
+minimum_signatures=2,
+maximum_signatures=62,
+nmf_replicates=100,
+resample=True,
+seeds=seeds,
+matrix_normalization="gmm",
+nmf_init="random",
+precision="single",
+min_nmf_iterations=1000,
+max_nmf_iterations=200000,
+nmf_test_conv=1000,
+nmf_tolerance=1e-08</t>
+  </si>
+  <si>
+    <t>K.guess = 22,
+multi.types = TRUE,
+burnin = 5000,
+burnin.multiplier = 6,
+post.n = 200,
+post. Space = 100,
+num.child.process = 20,
+CPU.cores = 20,
+high.confidence.prop = 0.9,
+gamma.alpha = 1,
+gamma.beta = 50</t>
+  </si>
+  <si>
+    <t>K.guess = 46,
+multi.types = TRUE,
+burnin = 5000,
+burnin.multiplier = 20,
+post.n = 200,
+post.space = 100,
+num.child.process = 20,
+CPU.cores = 20,
+high.confidence.prop = 0.9,
+gamma.alpha = 1,
+gamma.beta = 20</t>
+  </si>
+  <si>
+    <t>K.guess = 26,
+multi.types = TRUE,
+burnin= 5000,
+burnin.multiplier = 6,
+post.n= 200,
+post.space = 100,
+num.child.process = 20,
+CPU.cores = 20,
+high.confidence.prop = 0.9,
+gamma.alpha= 1,
+gamma.beta = 50</t>
+  </si>
+  <si>
+    <t>K.guess = 22,
+multi.types = TRUE,
+burnin = 5000,
+burnin.multiplier = 6,
+post.n = 200,
+post.space = 100,
+num.child.process = 20,
+CPU.cores = 20,
+high.confidence.prop = 0.9,
+gamma.alpha = 1,
+gamma.beta = 50</t>
+  </si>
+  <si>
+    <t>mSigHdp = 1.1.7; 
+hdpx = 0.3.4</t>
+  </si>
+  <si>
+    <t>K.guess = 64,
+multi.types = TRUE,
+burnin = 5000,
+burnin.multiplier = 20,
+post.n = 200,
+post.space = 100,
+num.child.process = 20,
+CPU.cores = 20,
+high.confidence.prop = 0.9,
+gamma.alpha = 1,
+gamma.beta = 20</t>
+  </si>
+  <si>
+    <t>reference_genome="GRCh37",
+cosmic_version="3.2",
+context_type=="96",
+exome=False,
+minimum_signatures=10,
+maximum_signatures=40,
+nmf_replicates=100,
+resample=True,
+seeds=seeds,
+matrix_normalization="gmm",
+nmf_init="random",
+precision="single",
+min_nmf_iterations=1000,
+max_nmf_iterations=200000,
+nmf_test_conv=1000,
+nmf_tolerance=1e-08</t>
+  </si>
+  <si>
+    <t>K_range = c(2, 62)</t>
+  </si>
+  <si>
+    <t>K_range = c(10, 40)</t>
+  </si>
+  <si>
+    <t>K_range = c(2, 24)</t>
+  </si>
+  <si>
+    <t>K_range = c(2, 20)</t>
+  </si>
+  <si>
+    <t>signeR = 1.18.1; 
+NMF = 0.30.1;
+Wrapper function SynSigRun::RunsigneR(), SynSigRun = 1.0.0</t>
+  </si>
+  <si>
+    <t>signeR = 1.20.0;
+NMF = 0.24.0;
+Wrapper function SynSigRun::RunsigneR(), SynSigRun = 1.0.0</t>
+  </si>
+  <si>
+    <t>signeR = 1.18.1;
+NMF = 0.30.1;
+Wrapper function SynSigRun::RunsigneR(), SynSigRun = 1.0.0</t>
+  </si>
+  <si>
+    <t>maxK = 26,
+tol = 1e-7</t>
+  </si>
+  <si>
+    <t>maxK = 22,
+tol = 1e-7</t>
+  </si>
+  <si>
+    <t>maxK = 64,
+tol = 1e-7</t>
+  </si>
+  <si>
+    <t>maxK = 46,
+tol = 1e-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SignatureAnalyzer
+ 2018-05-24 </t>
+  </si>
+  <si>
+    <t>Arguments for function mSigHdp::RunHdpParallel():
+K.guess = 46,
+multi.types = TRUE,
+post.burnin = 5000 * 20,
+post.n = 200,
+post.space = 100,
+post.cpiter = 3,
+num.child.process = 20,
+CPU.cores = 20,
+cos.merge = 0.9,
+min.sample = 1
+Arguments for function mSigHdp::SetupAndPosterior():
+GLOBAL.gamma.alpha = 1,
+GLOBAL.gamma.beta = 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Arguments for function mSigHdp::RunHdpParallel():
+K.guess = 46,
+multi.types = TRUE,
+post.burnin = 5000 * 20,
+post.n = 200,
+post.space = 100,
+post.cpiter = 3,
+num.child.process = 20,
+CPU.cores = 20,
+cos.merge = 0.9,
+min.sample = 1
+Arguments for function mSigHdp::SetupAndPosterior():</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GLOBAL.gamma.alpha = 1,
+GLOBAL.gamma.beta = 50</t>
+    </r>
+  </si>
+  <si>
+    <t>Arguments for function mSigHdp::RunHdpParallel():
+K.guess = 22,
+multi.types = TRUE,
+post.burnin = 5000 * 6,
+post.n = 200,
+post.space = 100,
+post.cpiter = 3,
+num.child.process = 20,
+CPU.cores = 20,
+cos.merge = 0.9,
+min.sample = 1
+Arguments for function mSigHdp::SetupAndPosterior():
+GLOBAL.gamma.alpha = 1,
+GLOBAL.gamma.beta = 50</t>
+  </si>
+  <si>
+    <t>Arguments for function mSigHdp::RunHdpParallel():
+K.guess = 22,
+multi.types = TRUE,
+post.burnin = 5000 * 20,
+post.n = 200,
+post.space = 100,
+post.cpiter = 3,
+num.child.process = 20,
+CPU.cores = 20,
+cos.merge = 0.9,
+min.sample = 1
+Arguments for function mSigHdp::SetupAndPosterior():
+GLOBAL.gamma.alpha = 1,
+GLOBAL.gamma.beta = 1</t>
   </si>
 </sst>
 </file>
@@ -297,10 +592,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -360,7 +655,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -431,6 +726,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -440,26 +747,47 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -895,10 +1223,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -928,40 +1256,41 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" activeCellId="1" sqref="C17 C11:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="26"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -972,14 +1301,16 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="23" t="s">
+        <v>62</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
@@ -998,14 +1329,16 @@
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>67</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
@@ -1029,12 +1362,16 @@
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>78</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1053,14 +1390,16 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="B9" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>69</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1079,14 +1418,16 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="43" t="s">
+        <v>80</v>
+      </c>
       <c r="D11" s="5">
         <v>145879</v>
       </c>
@@ -1097,10 +1438,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="5"/>
+    <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="40"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="5">
         <v>200437</v>
       </c>
@@ -1111,10 +1452,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="5"/>
+    <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="40"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="5">
         <v>310111</v>
       </c>
@@ -1125,10 +1466,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="5"/>
+    <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="5">
         <v>528401</v>
       </c>
@@ -1139,10 +1480,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="5"/>
+    <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="5">
         <v>1076753</v>
       </c>
@@ -1155,7 +1496,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="25"/>
+      <c r="B16" s="29"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1163,12 +1504,14 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="300" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="5"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="42" t="s">
+        <v>81</v>
+      </c>
       <c r="D17" s="5" t="s">
         <v>36</v>
       </c>
@@ -1215,13 +1558,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="B11:B17"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="A11:A15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1235,43 +1580,44 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="26"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="30"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1285,14 +1631,16 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="2"/>
+      <c r="B3" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>64</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1317,14 +1665,16 @@
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>52</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>55</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
@@ -1354,12 +1704,16 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>76</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1384,14 +1738,16 @@
       <c r="J8" s="4"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="5"/>
+      <c r="B9" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1416,14 +1772,16 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="300" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="41" t="s">
+        <v>83</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1439,7 +1797,7 @@
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="25"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1449,12 +1807,14 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="300" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="41" t="s">
+        <v>82</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1521,6 +1881,7 @@
     <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1529,217 +1890,212 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="7" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="26" t="s">
+      <c r="D1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="26" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="26"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="24"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="1"/>
+      <c r="G1" s="30"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="12" t="s">
+      <c r="E3" s="2"/>
+      <c r="F3" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="21" t="s">
+        <v>22</v>
+      </c>
       <c r="G5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
+      <c r="B8" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="G8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="G11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -1747,19 +2103,17 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -1769,26 +2123,25 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A18:G18"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1801,37 +2154,38 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="30" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
       <c r="J1" s="10"/>
@@ -1840,10 +2194,10 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="1"/>
       <c r="F2" s="11" t="s">
         <v>42</v>
@@ -1858,14 +2212,16 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="165" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>63</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
@@ -1890,14 +2246,16 @@
       <c r="H4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="240" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="23" t="s">
+        <v>59</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
@@ -1922,12 +2280,16 @@
       <c r="H6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
+      <c r="B7" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>75</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
@@ -1952,14 +2314,16 @@
       <c r="H8" s="5"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="5"/>
+        <v>73</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>70</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>36</v>
       </c>
@@ -2086,15 +2450,16 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="8" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
@@ -2108,13 +2473,13 @@
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="15"/>
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
@@ -2158,15 +2523,17 @@
       </c>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2">
+        <v>56</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="15">
         <v>145879</v>
       </c>
       <c r="E3" s="21" t="s">
@@ -2181,7 +2548,7 @@
       <c r="H3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="25" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -2194,13 +2561,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2">
+    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33"/>
+      <c r="B4" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="15">
         <v>200437</v>
       </c>
       <c r="E4" s="21" t="s">
@@ -2215,18 +2582,18 @@
       <c r="H4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="25" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="3"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2">
+    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="15">
         <v>310111</v>
       </c>
       <c r="E5" s="21" t="s">
@@ -2241,18 +2608,18 @@
       <c r="H5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="25" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="3"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2">
+    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="15">
         <v>528401</v>
       </c>
       <c r="E6" s="21" t="s">
@@ -2267,18 +2634,18 @@
       <c r="H6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="25" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="3"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2">
+    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="15">
         <v>1076753</v>
       </c>
       <c r="E7" s="21" t="s">
@@ -2293,7 +2660,7 @@
       <c r="H7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="25" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="2"/>
@@ -2304,7 +2671,7 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="D8" s="15"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
@@ -2313,23 +2680,25 @@
       <c r="K8" s="3"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2">
+      <c r="C9" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="15">
         <v>145879</v>
       </c>
-      <c r="E9" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
+      <c r="E9" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
       <c r="I9" s="32" t="s">
         <v>22</v>
       </c>
@@ -2343,60 +2712,64 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2">
+    <row r="10" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="15">
         <v>200437</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
       <c r="I10" s="32"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="28"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2">
+    <row r="11" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="15">
         <v>310111</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
       <c r="I11" s="32"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
-      <c r="D12" s="2">
+    <row r="12" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="15">
         <v>528401</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
       <c r="I12" s="32"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
-      <c r="D13" s="2">
+    <row r="13" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="15">
         <v>1076753</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
       <c r="I13" s="32"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
@@ -2415,7 +2788,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2438,12 +2811,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A9:A13"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="E9:H13"/>
     <mergeCell ref="I9:I13"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="C9:C13"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -2463,14 +2840,15 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:I3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="4" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="8" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" customWidth="1"/>
@@ -2485,13 +2863,13 @@
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="14"/>
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
@@ -2526,7 +2904,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K2" s="13" t="s">
         <v>0</v>
@@ -2539,26 +2917,28 @@
       </c>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>61</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
       <c r="J3" s="22" t="s">
         <v>45</v>
       </c>
@@ -2573,7 +2953,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -2587,27 +2967,29 @@
       <c r="L4" s="3"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:14" ht="255" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="23" t="s">
+        <v>55</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="29" t="s">
+      <c r="E5" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="24" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -2651,20 +3033,20 @@
       <c r="M7" s="5"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="27"/>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">

</xml_diff>

<commit_message>
Updated running status recorded in `mSigHdp-paper-tracking.xlsx`:
On "indel_2/Noiseless", NR_hdp failed to run with 3 seeds when setting gamma.beta = 50
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746682DC-3D52-4C64-8F03-F51655C9AB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FFDC3C-341C-41B7-A303-A9D110AB9978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="1620" windowWidth="14190" windowHeight="13860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2925" yWindow="1245" windowWidth="14190" windowHeight="13860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="86">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -630,7 +630,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +673,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -687,7 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -707,9 +713,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -776,14 +779,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -806,8 +806,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -815,13 +818,13 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1258,10 +1261,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -1291,8 +1294,8 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,29 +1306,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="36"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="34"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1340,23 +1343,23 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>62</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="15"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1368,29 +1371,29 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>67</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="21" t="s">
+      <c r="F5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="20" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="15"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1401,23 +1404,23 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="15"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1429,7 +1432,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>74</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1439,13 +1442,13 @@
         <v>36</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="15"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1453,14 +1456,14 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
+    <row r="11" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="35" t="s">
         <v>80</v>
       </c>
       <c r="D11" s="5">
@@ -1469,69 +1472,69 @@
       <c r="E11" s="5"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="38"/>
+      <c r="H11" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="5">
         <v>200437</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="2"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="38"/>
+      <c r="H12" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="5">
         <v>310111</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="2"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="38"/>
+      <c r="H13" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="5">
         <v>528401</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="2"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="38"/>
+      <c r="H14" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="37"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="5">
         <v>1076753</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="2"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="12" t="s">
+      <c r="H15" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="35"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1539,12 +1542,12 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="300" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="270" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="29" t="s">
+      <c r="B17" s="33"/>
+      <c r="C17" s="28" t="s">
         <v>81</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -1553,7 +1556,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="2"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="16" t="s">
+      <c r="H17" s="15" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1615,7 +1618,7 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
@@ -1627,32 +1630,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="36"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="34"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1670,26 +1673,26 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="15"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1704,23 +1707,23 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="20" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="2"/>
@@ -1729,7 +1732,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
-      <c r="B6" s="15"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1743,26 +1746,26 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>76</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
       <c r="I7" s="2"/>
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="15"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1777,7 +1780,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>72</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -1787,16 +1790,16 @@
         <v>36</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="15"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -1807,14 +1810,14 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="300" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="270" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="27" t="s">
         <v>85</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1823,7 +1826,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="8" t="s">
         <v>37</v>
       </c>
       <c r="I11" s="2"/>
@@ -1832,7 +1835,7 @@
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="35"/>
+      <c r="B12" s="33"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1842,19 +1845,19 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="300" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="270" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="28" t="s">
+      <c r="B13" s="33"/>
+      <c r="C13" s="27" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="H13" s="9" t="s">
+      <c r="H13" s="8" t="s">
         <v>37</v>
       </c>
       <c r="I13" s="2"/>
@@ -1863,7 +1866,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="18"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -1876,7 +1879,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="18"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -1888,13 +1891,13 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
+      <c r="B16" s="17"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="17"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1927,8 +1930,8 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1940,29 +1943,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="34" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="36"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="36"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>42</v>
@@ -1975,17 +1978,17 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="11" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1999,20 +2002,20 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="2"/>
@@ -2035,20 +2038,20 @@
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="22" t="s">
         <v>77</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="21" t="s">
+      <c r="F8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="21" t="s">
+      <c r="G8" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2070,7 +2073,7 @@
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -2080,10 +2083,10 @@
         <v>36</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="20" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2140,13 +2143,13 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -2189,8 +2192,8 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2204,40 +2207,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="34" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="10" t="s">
         <v>41</v>
       </c>
       <c r="H2" s="1"/>
@@ -2251,20 +2254,20 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>63</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="21" t="s">
         <v>45</v>
       </c>
       <c r="H3" s="2"/>
@@ -2276,8 +2279,8 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="2"/>
       <c r="M4" s="2"/>
     </row>
@@ -2288,17 +2291,17 @@
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="21" t="s">
+      <c r="F5" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="23" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="5"/>
@@ -2310,8 +2313,8 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="4"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="5"/>
       <c r="M6" s="5"/>
     </row>
@@ -2319,20 +2322,20 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="22" t="s">
         <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="23" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="5"/>
@@ -2344,8 +2347,8 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="4"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="5"/>
       <c r="M8" s="5"/>
     </row>
@@ -2353,7 +2356,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>73</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -2363,10 +2366,10 @@
         <v>36</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="23" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="5"/>
@@ -2378,125 +2381,121 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="5"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+    <row r="11" spans="1:13" ht="270" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="5">
-        <v>145879</v>
+      <c r="D11" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="25" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="5">
-        <v>200437</v>
-      </c>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="F12" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>23</v>
-      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="29"/>
       <c r="H12" s="5"/>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="40"/>
+    <row r="13" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" s="39" t="s">
+        <v>83</v>
+      </c>
       <c r="D13" s="5">
-        <v>310111</v>
+        <v>145879</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="25" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="41"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="40"/>
+    <row r="14" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="40"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="39"/>
       <c r="D14" s="5">
-        <v>528401</v>
+        <v>200437</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="30" t="s">
+      <c r="F14" s="38"/>
+      <c r="G14" s="25" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="40"/>
+    <row r="15" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="39"/>
       <c r="D15" s="5">
-        <v>1076753</v>
+        <v>310111</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="30" t="s">
+      <c r="F15" s="38"/>
+      <c r="G15" s="44" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+    <row r="16" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="40"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="5">
+        <v>528401</v>
+      </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="31"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="44" t="s">
+        <v>23</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13" ht="270" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>36</v>
+    <row r="17" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="40"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="5">
+        <v>1076753</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="32" t="s">
+      <c r="F17" s="38"/>
+      <c r="G17" s="44" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="5"/>
@@ -2534,7 +2533,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -2548,10 +2547,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="A11:A15"/>
+  <mergeCells count="9">
+    <mergeCell ref="F13:F17"/>
     <mergeCell ref="B11:B17"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="A13:A17"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="D1:D2"/>
@@ -2559,6 +2559,7 @@
     <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2569,8 +2570,8 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,86 +2589,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="34" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
     </row>
     <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="14">
         <v>145879</v>
       </c>
-      <c r="E3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="25" t="s">
+      <c r="E3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="24" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -2681,27 +2682,27 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="41"/>
-      <c r="B4" s="35" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="15">
+      <c r="C4" s="42"/>
+      <c r="D4" s="14">
         <v>200437</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="25" t="s">
+      <c r="E4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="24" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="2"/>
@@ -2709,25 +2710,25 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41"/>
-      <c r="B5" s="35"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="15">
+      <c r="A5" s="40"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="14">
         <v>310111</v>
       </c>
-      <c r="E5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="25" t="s">
+      <c r="E5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="24" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="2"/>
@@ -2735,25 +2736,25 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="15">
+      <c r="A6" s="40"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="14">
         <v>528401</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="25" t="s">
+      <c r="E6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="24" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="2"/>
@@ -2761,25 +2762,25 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="15">
+      <c r="A7" s="40"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="14">
         <v>1076753</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="21" t="s">
+      <c r="E7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="24" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="2"/>
@@ -2790,7 +2791,7 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="15"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
@@ -2800,25 +2801,25 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="14">
         <v>145879</v>
       </c>
-      <c r="E9" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="43" t="s">
+      <c r="E9" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="38" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -2832,64 +2833,64 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="15">
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="14">
         <v>200437</v>
       </c>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="43"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="15">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="14">
         <v>310111</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="43"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="15">
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="14">
         <v>528401</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="38"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="15">
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="14">
         <v>1076753</v>
       </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="38"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
@@ -2959,7 +2960,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A9" sqref="A9:L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2978,87 +2979,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="34" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="13">
         <v>500</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="G2" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="165" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="22" t="s">
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="45" t="s">
+      <c r="F3" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="22" t="s">
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="21" t="s">
         <v>45</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -3072,7 +3073,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="15"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -3087,28 +3088,28 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="255" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="22" t="s">
         <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="24" t="s">
+      <c r="E5" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="23" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -3152,20 +3153,20 @@
       <c r="M7" s="5"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">

</xml_diff>

<commit_message>
Added two sheets to show overall progress of benchmarking and evaluation.
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FFDC3C-341C-41B7-A303-A9D110AB9978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C76F17-EDFD-455B-B750-890C8796C4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="1245" windowWidth="14190" windowHeight="13860" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="1290" windowWidth="14190" windowHeight="13860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
-    <sheet name="SBS" sheetId="11" r:id="rId2"/>
-    <sheet name="indel" sheetId="10" r:id="rId3"/>
-    <sheet name="SBS_2" sheetId="8" r:id="rId4"/>
-    <sheet name="indel_2" sheetId="9" r:id="rId5"/>
-    <sheet name="SBS_down_samp" sheetId="1" r:id="rId6"/>
-    <sheet name="indel_down_samp" sheetId="4" r:id="rId7"/>
+    <sheet name="SBS_general" sheetId="12" r:id="rId2"/>
+    <sheet name="Indel_general" sheetId="13" r:id="rId3"/>
+    <sheet name="SBS" sheetId="11" r:id="rId4"/>
+    <sheet name="indel" sheetId="10" r:id="rId5"/>
+    <sheet name="SBS_2" sheetId="8" r:id="rId6"/>
+    <sheet name="indel_2" sheetId="9" r:id="rId7"/>
+    <sheet name="SBS_down_samp" sheetId="1" r:id="rId8"/>
+    <sheet name="indel_down_samp" sheetId="4" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="116">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -566,17 +568,116 @@
 GLOBAL.gamma.alpha = 1,
 GLOBAL.gamma.beta = 1</t>
   </si>
+  <si>
+    <t>Benchmarking mSigHdp in the original submission and proposed additional benchmarking </t>
+  </si>
+  <si>
+    <t>  </t>
+  </si>
+  <si>
+    <t> = benchmarking in the original submission </t>
+  </si>
+  <si>
+    <t>= additional benchmarking in revision </t>
+  </si>
+  <si>
+    <t>SBS  data sets </t>
+  </si>
+  <si>
+    <t>Synthetic data set 1 </t>
+  </si>
+  <si>
+    <t>Synthetic data set 2 </t>
+  </si>
+  <si>
+    <t>Noise </t>
+  </si>
+  <si>
+    <t>Approach </t>
+  </si>
+  <si>
+    <t>None </t>
+  </si>
+  <si>
+    <t>Moderate </t>
+  </si>
+  <si>
+    <t>Realistic </t>
+  </si>
+  <si>
+    <t>mSigHdp no downsampling </t>
+  </si>
+  <si>
+    <t>original submission </t>
+  </si>
+  <si>
+    <t>done </t>
+  </si>
+  <si>
+    <t>SigProfilerExtractor </t>
+  </si>
+  <si>
+    <t>SignatureAnalyzer </t>
+  </si>
+  <si>
+    <t>signeR </t>
+  </si>
+  <si>
+    <t>Original hdp with programming errors corrected </t>
+  </si>
+  <si>
+    <t>gamma.beta = 1</t>
+  </si>
+  <si>
+    <t>Running
+Takes 14 days already</t>
+  </si>
+  <si>
+    <t>Pending for available resources</t>
+  </si>
+  <si>
+    <t>gamma.beta = 20</t>
+  </si>
+  <si>
+    <t>mSigHdp 10k downsampling </t>
+  </si>
+  <si>
+    <t>Not yet runned</t>
+  </si>
+  <si>
+    <t>mSigHdp 5k downsampling </t>
+  </si>
+  <si>
+    <t>mSigHdp 3k downsampling </t>
+  </si>
+  <si>
+    <t>Indel data sets </t>
+  </si>
+  <si>
+    <t>gamma.beta = 50</t>
+  </si>
+  <si>
+    <t>Some runs failed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -629,8 +730,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -679,8 +799,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8EA9DB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -688,56 +832,185 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -746,58 +1019,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -806,30 +1082,107 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="常规 2" xfId="2" xr:uid="{4DBD74BB-9B12-4298-9AA6-0A807FEE0790}"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1131,12 +1484,12 @@
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -1144,7 +1497,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1164,7 +1517,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>2022</v>
       </c>
@@ -1184,7 +1537,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>2022</v>
       </c>
@@ -1204,7 +1557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>25</v>
@@ -1216,7 +1569,7 @@
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>26</v>
@@ -1228,7 +1581,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
         <v>27</v>
@@ -1240,7 +1593,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>27</v>
@@ -1252,7 +1605,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1260,15 +1613,15 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
+    <row r="10" spans="1:6">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1288,6 +1641,506 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52971DA9-35F9-431D-99EC-B8057B18CDFC}">
+  <dimension ref="A1:F18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="46"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5" customHeight="1">
+      <c r="A1" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:6" ht="25.5" customHeight="1">
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+    </row>
+    <row r="4" spans="1:6" ht="25.5" customHeight="1">
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="51" t="s">
+        <v>90</v>
+      </c>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+    </row>
+    <row r="7" spans="1:6" ht="26.25" thickBot="1">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="54"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A9" s="55" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="C9" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" s="53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="51.75" thickBot="1">
+      <c r="A10" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="55"/>
+      <c r="C10" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="57"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="39" thickBot="1">
+      <c r="A11" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="55"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="26.25" thickBot="1">
+      <c r="A12" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="55"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A13" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="55"/>
+      <c r="C13" s="63"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="64.5" customHeight="1" thickBot="1">
+      <c r="A14" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
+      <c r="E14" s="67" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="67" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="51.75" thickBot="1">
+      <c r="A15" s="66"/>
+      <c r="B15" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="68" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="51.75" thickBot="1">
+      <c r="A16" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" s="55"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="F16" s="69" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="51.75" thickBot="1">
+      <c r="A17" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="55"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="69" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="51.75" thickBot="1">
+      <c r="A18" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="B18" s="55"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="70" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C10:E13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A16AE307-4AD6-4677-ADDD-934D34217471}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="46"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="25.5" customHeight="1">
+      <c r="A1" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+    </row>
+    <row r="3" spans="1:6" ht="25.5" customHeight="1">
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+    </row>
+    <row r="4" spans="1:6" ht="25.5" customHeight="1">
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="51" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+    </row>
+    <row r="8" spans="1:6" ht="26.25" thickBot="1">
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="47"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="53" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="51.75" thickBot="1">
+      <c r="A11" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="39" thickBot="1">
+      <c r="A12" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="55"/>
+      <c r="C12" s="60"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="26.25" thickBot="1">
+      <c r="A13" s="55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="55"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1">
+      <c r="A14" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="55"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="59" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="64.5" customHeight="1" thickBot="1">
+      <c r="A15" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="47"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="F15" s="69"/>
+    </row>
+    <row r="16" spans="1:6" ht="26.25" thickBot="1">
+      <c r="A16" s="66"/>
+      <c r="B16" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="71" t="s">
+        <v>115</v>
+      </c>
+      <c r="F16" s="69"/>
+    </row>
+    <row r="17" spans="1:6" ht="51.75" thickBot="1">
+      <c r="A17" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="F17" s="69"/>
+    </row>
+    <row r="18" spans="1:6" ht="51.75" thickBot="1">
+      <c r="A18" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" s="55"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="F18" s="69"/>
+    </row>
+    <row r="19" spans="1:6" ht="51.75" thickBot="1">
+      <c r="A19" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="55"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="70"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="C11:E14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14DFF80A-C422-4360-9D1E-94068848F4B1}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1298,37 +2151,37 @@
       <selection activeCell="B11" sqref="B11:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="34"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="35"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1339,7 +2192,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="165">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1357,7 +2210,7 @@
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2"/>
       <c r="B4" s="14"/>
       <c r="C4" s="2"/>
@@ -1367,7 +2220,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="240">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1391,7 +2244,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2"/>
       <c r="B6" s="14"/>
       <c r="C6" s="2"/>
@@ -1400,7 +2253,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1418,7 +2271,7 @@
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" s="2"/>
       <c r="B8" s="14"/>
       <c r="C8" s="2"/>
@@ -1428,7 +2281,7 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="75">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1446,7 +2299,7 @@
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="5"/>
       <c r="B10" s="14"/>
       <c r="C10" s="5"/>
@@ -1456,14 +2309,14 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="37" t="s">
+    <row r="11" spans="1:8" ht="54" customHeight="1">
+      <c r="A11" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="36" t="s">
         <v>80</v>
       </c>
       <c r="D11" s="5">
@@ -1476,10 +2329,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="36"/>
+    <row r="12" spans="1:8" ht="54" customHeight="1">
+      <c r="A12" s="38"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="37"/>
       <c r="D12" s="5">
         <v>200437</v>
       </c>
@@ -1490,10 +2343,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="37"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="36"/>
+    <row r="13" spans="1:8" ht="54" customHeight="1">
+      <c r="A13" s="38"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="37"/>
       <c r="D13" s="5">
         <v>310111</v>
       </c>
@@ -1504,10 +2357,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="36"/>
+    <row r="14" spans="1:8" ht="54" customHeight="1">
+      <c r="A14" s="38"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="5">
         <v>528401</v>
       </c>
@@ -1518,10 +2371,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="37"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="36"/>
+    <row r="15" spans="1:8" ht="54" customHeight="1">
+      <c r="A15" s="38"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="37"/>
       <c r="D15" s="5">
         <v>1076753</v>
       </c>
@@ -1532,9 +2385,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="5"/>
-      <c r="B16" s="33"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -1542,11 +2395,11 @@
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="270" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="270" customHeight="1">
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="33"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="28" t="s">
         <v>81</v>
       </c>
@@ -1560,7 +2413,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1570,7 +2423,7 @@
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1580,17 +2433,17 @@
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="5" t="s">
         <v>31</v>
       </c>
@@ -1611,7 +2464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A9EF94-C3F0-491E-B97E-7A2B5FFF7AB0}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1622,40 +2475,40 @@
       <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="34"/>
+    <row r="2" spans="1:11">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="35"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1669,7 +2522,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="165">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1690,7 +2543,7 @@
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4" s="2"/>
       <c r="B4" s="14"/>
       <c r="C4" s="2"/>
@@ -1703,7 +2556,7 @@
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="240">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1730,7 +2583,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6" s="2"/>
       <c r="B6" s="14"/>
       <c r="C6" s="2"/>
@@ -1742,7 +2595,7 @@
       <c r="J6" s="4"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="30">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -1763,7 +2616,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8" s="2"/>
       <c r="B8" s="14"/>
       <c r="C8" s="2"/>
@@ -1776,7 +2629,7 @@
       <c r="J8" s="4"/>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="75">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -1797,7 +2650,7 @@
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10" s="5"/>
       <c r="B10" s="14"/>
       <c r="C10" s="5"/>
@@ -1810,11 +2663,11 @@
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
     </row>
-    <row r="11" spans="1:11" ht="270" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="270" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="27" t="s">
@@ -1833,9 +2686,9 @@
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
     </row>
-    <row r="12" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="33"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1845,11 +2698,11 @@
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
     </row>
-    <row r="13" spans="1:11" ht="270" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="270" customHeight="1">
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="33"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="27" t="s">
         <v>82</v>
       </c>
@@ -1864,7 +2717,7 @@
       <c r="J13" s="5"/>
       <c r="K13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14" s="5"/>
       <c r="B14" s="17"/>
       <c r="C14" s="5"/>
@@ -1877,7 +2730,7 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15" s="5"/>
       <c r="B15" s="17"/>
       <c r="C15" s="5"/>
@@ -1890,21 +2743,21 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="B16" s="17"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
       <c r="B17" s="17"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
         <v>31</v>
       </c>
@@ -1923,7 +2776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA50912E-27FE-44B5-A047-41F12E48181B}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -1934,7 +2787,7 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
@@ -1942,30 +2795,30 @@
     <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:8" ht="49.5" customHeight="1">
+      <c r="A1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="35" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="34"/>
+      <c r="G1" s="35"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="33"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>42</v>
@@ -1974,7 +2827,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="165">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -1992,13 +2845,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="240" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="240">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -2020,21 +2873,21 @@
       </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -2055,21 +2908,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="75">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -2090,14 +2943,14 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
         <v>29</v>
       </c>
@@ -2108,14 +2961,14 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
@@ -2126,14 +2979,14 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2142,16 +2995,16 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7">
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
         <v>32</v>
       </c>
@@ -2162,12 +3015,12 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -2185,18 +3038,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B3DE763-45BF-4630-996D-9B80B26D1A4B}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
@@ -2206,24 +3059,24 @@
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:13" ht="46.5" customHeight="1">
+      <c r="A1" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="35" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="34"/>
+      <c r="G1" s="35"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -2231,11 +3084,11 @@
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
     </row>
-    <row r="2" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
+    <row r="2" spans="1:13" ht="30.75" customHeight="1">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="1"/>
       <c r="F2" s="10" t="s">
         <v>42</v>
@@ -2250,7 +3103,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="165">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -2273,7 +3126,7 @@
       <c r="H3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2284,7 +3137,7 @@
       <c r="H4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="240" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="240">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -2307,7 +3160,7 @@
       <c r="H5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2318,7 +3171,7 @@
       <c r="H6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="30">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2341,7 +3194,7 @@
       <c r="H7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2352,7 +3205,7 @@
       <c r="H8" s="5"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="90">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
@@ -2375,7 +3228,7 @@
       <c r="H9" s="5"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -2386,11 +3239,11 @@
       <c r="H10" s="5"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="270" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="270" customHeight="1">
       <c r="A11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="34" t="s">
         <v>46</v>
       </c>
       <c r="C11" s="27" t="s">
@@ -2409,9 +3262,9 @@
       <c r="H11" s="5"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13">
       <c r="A12" s="5"/>
-      <c r="B12" s="33"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -2420,19 +3273,19 @@
       <c r="H12" s="5"/>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
+    <row r="13" spans="1:13" ht="54" customHeight="1">
+      <c r="A13" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="33"/>
-      <c r="C13" s="39" t="s">
+      <c r="B13" s="34"/>
+      <c r="C13" s="40" t="s">
         <v>83</v>
       </c>
       <c r="D13" s="5">
         <v>145879</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="38" t="s">
+      <c r="F13" s="39" t="s">
         <v>23</v>
       </c>
       <c r="G13" s="25" t="s">
@@ -2441,67 +3294,67 @@
       <c r="H13" s="5"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="33"/>
-      <c r="C14" s="39"/>
+    <row r="14" spans="1:13" ht="54" customHeight="1">
+      <c r="A14" s="41"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="40"/>
       <c r="D14" s="5">
         <v>200437</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="38"/>
+      <c r="F14" s="39"/>
       <c r="G14" s="25" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="5"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="39"/>
+    <row r="15" spans="1:13" ht="54" customHeight="1">
+      <c r="A15" s="41"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="40"/>
       <c r="D15" s="5">
         <v>310111</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="44" t="s">
+      <c r="F15" s="39"/>
+      <c r="G15" s="31" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="5"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="39"/>
+    <row r="16" spans="1:13" ht="54" customHeight="1">
+      <c r="A16" s="41"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="40"/>
       <c r="D16" s="5">
         <v>528401</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="44" t="s">
+      <c r="F16" s="39"/>
+      <c r="G16" s="31" t="s">
         <v>23</v>
       </c>
       <c r="H16" s="5"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="39"/>
+    <row r="17" spans="1:13" ht="54" customHeight="1">
+      <c r="A17" s="41"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="40"/>
       <c r="D17" s="5">
         <v>1076753</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="44" t="s">
+      <c r="F17" s="39"/>
+      <c r="G17" s="31" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="5"/>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -2516,7 +3369,7 @@
       <c r="L18" s="5"/>
       <c r="M18" s="5"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -2531,17 +3384,17 @@
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13">
       <c r="A21" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13">
       <c r="A22" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -2563,7 +3416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2574,7 +3427,7 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
@@ -2588,23 +3441,23 @@
     <col min="13" max="13" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
       <c r="J1" s="14"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
     </row>
-    <row r="2" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="45">
       <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
@@ -2643,14 +3496,14 @@
       </c>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+    <row r="3" spans="1:13" ht="60" customHeight="1">
+      <c r="A3" s="41" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="37" t="s">
         <v>62</v>
       </c>
       <c r="D3" s="14">
@@ -2681,12 +3534,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="33" t="s">
+    <row r="4" spans="1:13" ht="30" customHeight="1">
+      <c r="A4" s="41"/>
+      <c r="B4" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="14">
         <v>200437</v>
       </c>
@@ -2709,10 +3562,10 @@
       <c r="K4" s="3"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="42"/>
+    <row r="5" spans="1:13" ht="30" customHeight="1">
+      <c r="A5" s="41"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="14">
         <v>310111</v>
       </c>
@@ -2735,10 +3588,10 @@
       <c r="K5" s="3"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="42"/>
+    <row r="6" spans="1:13" ht="30" customHeight="1">
+      <c r="A6" s="41"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="14">
         <v>528401</v>
       </c>
@@ -2761,10 +3614,10 @@
       <c r="K6" s="3"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="42"/>
+    <row r="7" spans="1:13" ht="30" customHeight="1">
+      <c r="A7" s="41"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="14">
         <v>1076753</v>
       </c>
@@ -2787,7 +3640,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -2800,26 +3653,26 @@
       <c r="K8" s="3"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+    <row r="9" spans="1:13" ht="48" customHeight="1">
+      <c r="A9" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="37" t="s">
         <v>58</v>
       </c>
       <c r="D9" s="14">
         <v>145879</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="38" t="s">
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="39" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -2832,81 +3685,81 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="42"/>
+    <row r="10" spans="1:13" ht="48" customHeight="1">
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="14">
         <v>200437</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="38"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="42"/>
+    <row r="11" spans="1:13" ht="48" customHeight="1">
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="14">
         <v>310111</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="38"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="42"/>
+    <row r="12" spans="1:13" ht="48" customHeight="1">
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="14">
         <v>528401</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="38"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="39"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="42"/>
+    <row r="13" spans="1:13" ht="48" customHeight="1">
+      <c r="A13" s="41"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="14">
         <v>1076753</v>
       </c>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="38"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="39"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13">
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13">
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13">
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17" s="5" t="s">
         <v>54</v>
       </c>
@@ -2920,12 +3773,12 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -2942,7 +3795,7 @@
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="C9:C13"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
   </hyperlinks>
@@ -2952,7 +3805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CCBB4E0-5F89-431B-A9E8-4B03CB92E69C}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -2963,7 +3816,7 @@
       <selection activeCell="A9" sqref="A9:L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" customWidth="1"/>
@@ -2978,24 +3831,24 @@
     <col min="14" max="14" width="31.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="14"/>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
       <c r="J1" s="13"/>
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
     </row>
-    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="45">
       <c r="A2" s="13" t="s">
         <v>4</v>
       </c>
@@ -3037,7 +3890,7 @@
       </c>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="165">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
@@ -3053,12 +3906,12 @@
       <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
       <c r="J3" s="21" t="s">
         <v>45</v>
       </c>
@@ -3072,7 +3925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="A4" s="14"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -3087,7 +3940,7 @@
       <c r="L4" s="3"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="5" spans="1:14" ht="255" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="255" customHeight="1">
       <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
@@ -3103,12 +3956,12 @@
       <c r="E5" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
       <c r="J5" s="23" t="s">
         <v>22</v>
       </c>
@@ -3122,7 +3975,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -3137,7 +3990,7 @@
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -3152,23 +4005,23 @@
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+    <row r="9" spans="1:14">
+      <c r="A9" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -3184,12 +4037,12 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Added "NR_hdp_gb_50" to result summary of "indel_2".
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E485196F-5D91-410D-88BA-2628331F48E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717AB852-B8BF-4E85-9081-C790958F07F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -1192,9 +1192,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1405,6 +1402,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1841,10 +1841,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="51"/>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -1874,7 +1874,7 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1882,171 +1882,171 @@
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="5" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" style="26" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="25" customWidth="1"/>
     <col min="11" max="11" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="70" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="14"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="13"/>
     </row>
     <row r="2" spans="1:11" ht="45">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="35.1" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="50" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="50" t="s">
+      <c r="E3" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="29"/>
-      <c r="G3" s="50" t="s">
+      <c r="F3" s="28"/>
+      <c r="G3" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="H3" s="50" t="s">
+      <c r="H3" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="I3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="82" t="s">
+      <c r="J3" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="75" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="35.1" customHeight="1">
-      <c r="A4" s="76"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="51"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="50" t="s">
+      <c r="F4" s="28"/>
+      <c r="G4" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="H4" s="29"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="82"/>
-      <c r="K4" s="76"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="81"/>
+      <c r="K4" s="75"/>
     </row>
     <row r="5" spans="1:11" ht="35.1" customHeight="1">
-      <c r="A5" s="76"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="51"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="50" t="s">
+      <c r="F5" s="28"/>
+      <c r="G5" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="76"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="76"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="75"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="75"/>
     </row>
     <row r="6" spans="1:11" ht="35.1" customHeight="1">
-      <c r="A6" s="76"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="51"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="F6" s="29"/>
-      <c r="G6" s="50" t="s">
+      <c r="F6" s="28"/>
+      <c r="G6" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="H6" s="29"/>
-      <c r="I6" s="76"/>
-      <c r="J6" s="82"/>
-      <c r="K6" s="76"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="75"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="75"/>
     </row>
     <row r="7" spans="1:11" ht="35.1" customHeight="1">
-      <c r="A7" s="76"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="51"/>
+      <c r="A7" s="75"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="50" t="s">
+      <c r="E7" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="50" t="s">
+      <c r="F7" s="28"/>
+      <c r="G7" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="H7" s="29"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="76"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="81"/>
+      <c r="K7" s="75"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2055,22 +2055,22 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="45"/>
+      <c r="J8" s="44"/>
       <c r="K8" s="2"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
@@ -2084,7 +2084,7 @@
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="17"/>
+      <c r="J11" s="16"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
@@ -2123,12 +2123,12 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="51"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5"/>
@@ -2183,68 +2183,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="70" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:13" ht="45">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>19</v>
       </c>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="50" t="s">
         <v>63</v>
       </c>
       <c r="D3" s="2">
@@ -2265,20 +2265,20 @@
       <c r="I3" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="J3" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="82" t="s">
+      <c r="K3" s="81" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="L3" s="75" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A4" s="76"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="51"/>
+      <c r="A4" s="75"/>
+      <c r="B4" s="70"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
@@ -2297,14 +2297,14 @@
       <c r="I4" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="76"/>
-      <c r="K4" s="82"/>
-      <c r="L4" s="76"/>
+      <c r="J4" s="75"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="75"/>
     </row>
     <row r="5" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A5" s="76"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="51"/>
+      <c r="A5" s="75"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
@@ -2323,14 +2323,14 @@
       <c r="I5" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J5" s="76"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="76"/>
+      <c r="J5" s="75"/>
+      <c r="K5" s="81"/>
+      <c r="L5" s="75"/>
     </row>
     <row r="6" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A6" s="76"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="51"/>
+      <c r="A6" s="75"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
@@ -2349,14 +2349,14 @@
       <c r="I6" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J6" s="76"/>
-      <c r="K6" s="82"/>
-      <c r="L6" s="76"/>
+      <c r="J6" s="75"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="75"/>
     </row>
     <row r="7" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A7" s="76"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="51"/>
+      <c r="A7" s="75"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
@@ -2375,12 +2375,12 @@
       <c r="I7" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J7" s="76"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="76"/>
+      <c r="J7" s="75"/>
+      <c r="K7" s="81"/>
+      <c r="L7" s="75"/>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="14"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2390,7 +2390,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="45"/>
+      <c r="K8" s="44"/>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:13">
@@ -2408,19 +2408,19 @@
       <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="51" t="s">
+      <c r="A10" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="51"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="51"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="51"/>
-      <c r="K10" s="51"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="5" t="s">
@@ -2476,336 +2476,336 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="32"/>
+    <col min="1" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="49" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="44"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
     </row>
     <row r="5" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="48" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
+      <c r="M5" s="43"/>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="63" t="s">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="64" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="66" t="s">
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="G8" s="66"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="65" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65" t="s">
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="G9" s="65"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="36" t="s">
+      <c r="B10" s="36"/>
+      <c r="C10" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="E10" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="36" t="s">
+      <c r="G10" s="35" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51.75" thickBot="1">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="53" t="s">
+      <c r="B11" s="36"/>
+      <c r="C11" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="40" t="s">
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="38" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="39" thickBot="1">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="56"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="38" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="26.25" thickBot="1">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="38" t="s">
+      <c r="B13" s="36"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="38" t="s">
+      <c r="B14" s="36"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="39" t="s">
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="G15" s="40" t="s">
+      <c r="G15" s="39" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="51.75" thickBot="1">
-      <c r="A16" s="52"/>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="51"/>
+      <c r="B16" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="38" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="40" t="s">
+      <c r="G16" s="39" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A17" s="52" t="s">
+      <c r="A17" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="38" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="G17" s="40" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A18" s="52"/>
-      <c r="B18" s="37" t="s">
+      <c r="A18" s="51"/>
+      <c r="B18" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="38" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="40" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A19" s="52"/>
-      <c r="B19" s="37" t="s">
+      <c r="A19" s="51"/>
+      <c r="B19" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="38" t="s">
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="41" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A20" s="52"/>
-      <c r="B20" s="37" t="s">
+      <c r="A20" s="51"/>
+      <c r="B20" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="38" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="39" thickBot="1">
-      <c r="A21" s="52" t="s">
+      <c r="A21" s="51" t="s">
         <v>123</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="39" thickBot="1">
-      <c r="A22" s="52"/>
-      <c r="B22" s="37" t="s">
+      <c r="A22" s="51"/>
+      <c r="B22" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="39" thickBot="1">
-      <c r="A23" s="52"/>
-      <c r="B23" s="37" t="s">
+      <c r="A23" s="51"/>
+      <c r="B23" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39" thickBot="1">
-      <c r="A24" s="52"/>
-      <c r="B24" s="37" t="s">
+      <c r="A24" s="51"/>
+      <c r="B24" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="37" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2837,375 +2837,380 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="32"/>
+    <col min="1" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
     </row>
     <row r="2" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A2" s="43"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
     </row>
     <row r="4" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="49" t="s">
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="47" t="s">
+      <c r="I4" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="48" t="s">
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="47" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="43"/>
+      <c r="L5" s="43"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
     </row>
     <row r="8" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="63" t="s">
+      <c r="A8" s="32"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="64" t="s">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64" t="s">
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="G9" s="64"/>
+      <c r="G9" s="63"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="65" t="s">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65" t="s">
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="G10" s="65"/>
+      <c r="G10" s="64"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="36" t="s">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="35" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="51.75" thickBot="1">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="53" t="s">
+      <c r="B12" s="36"/>
+      <c r="C12" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="54"/>
-      <c r="E12" s="55"/>
-      <c r="F12" s="38" t="s">
+      <c r="D12" s="53"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="39" thickBot="1">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="56"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="38" t="s">
+      <c r="B13" s="36"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="26.25" thickBot="1">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="58"/>
-      <c r="F14" s="38" t="s">
+      <c r="B14" s="36"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="37"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="38" t="s">
+      <c r="B15" s="36"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A16" s="52" t="s">
+      <c r="A16" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="38" t="s">
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="26.25" thickBot="1">
-      <c r="A17" s="52"/>
-      <c r="B17" s="37" t="s">
+      <c r="A17" s="51"/>
+      <c r="B17" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="38" t="s">
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="F17" s="46" t="s">
+      <c r="F17" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="37" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="39" thickBot="1">
-      <c r="A18" s="52" t="s">
+      <c r="A18" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="38" t="s">
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="33"/>
-      <c r="G18" s="67" t="s">
+      <c r="F18" s="32"/>
+      <c r="G18" s="66" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="39" thickBot="1">
-      <c r="A19" s="52"/>
-      <c r="B19" s="37" t="s">
+      <c r="A19" s="51"/>
+      <c r="B19" s="36" t="s">
         <v>121</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="38" t="s">
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="F19" s="33"/>
-      <c r="G19" s="68"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="67"/>
     </row>
     <row r="20" spans="1:7" ht="39" thickBot="1">
-      <c r="A20" s="52"/>
-      <c r="B20" s="37" t="s">
+      <c r="A20" s="51"/>
+      <c r="B20" s="36" t="s">
         <v>122</v>
       </c>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-      <c r="E20" s="38" t="s">
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="F20" s="33"/>
-      <c r="G20" s="68"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="67"/>
     </row>
     <row r="21" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A21" s="52"/>
-      <c r="B21" s="37" t="s">
+      <c r="A21" s="51"/>
+      <c r="B21" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G21" s="68"/>
+      <c r="G21" s="67"/>
     </row>
     <row r="22" spans="1:7" ht="90" thickBot="1">
-      <c r="A22" s="52"/>
-      <c r="B22" s="37" t="s">
+      <c r="A22" s="51"/>
+      <c r="B22" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E22" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G22" s="69"/>
+      <c r="G22" s="68"/>
     </row>
     <row r="23" spans="1:7" ht="39" thickBot="1">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="E23" s="38" t="s">
+      <c r="E23" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G23" s="67" t="s">
+      <c r="G23" s="66" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39" thickBot="1">
-      <c r="A24" s="52"/>
-      <c r="B24" s="37" t="s">
+      <c r="A24" s="51"/>
+      <c r="B24" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E24" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G24" s="68"/>
+      <c r="G24" s="67"/>
     </row>
     <row r="25" spans="1:7" ht="39" thickBot="1">
-      <c r="A25" s="52"/>
-      <c r="B25" s="37" t="s">
+      <c r="A25" s="51"/>
+      <c r="B25" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="E25" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G25" s="68"/>
+      <c r="G25" s="67"/>
     </row>
     <row r="26" spans="1:7" ht="39" thickBot="1">
-      <c r="A26" s="52"/>
-      <c r="B26" s="37" t="s">
+      <c r="A26" s="51"/>
+      <c r="B26" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="E26" s="38" t="s">
+      <c r="E26" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="68"/>
+      <c r="G26" s="67"/>
     </row>
     <row r="27" spans="1:7" ht="90" thickBot="1">
-      <c r="A27" s="52"/>
-      <c r="B27" s="37" t="s">
+      <c r="A27" s="51"/>
+      <c r="B27" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="E27" s="38" t="s">
+      <c r="E27" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="G27" s="69"/>
+      <c r="G27" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="G23:G27"/>
     <mergeCell ref="G18:G22"/>
@@ -3213,11 +3218,6 @@
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="C12:E15"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3231,8 +3231,8 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3243,29 +3243,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="72"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="71"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -3280,23 +3280,23 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>62</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2"/>
-      <c r="B4" s="14"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -3308,29 +3308,29 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>67</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="19" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="2"/>
-      <c r="B6" s="14"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -3341,23 +3341,23 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="2"/>
-      <c r="B8" s="14"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -3369,7 +3369,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>74</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -3379,13 +3379,13 @@
         <v>36</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="5"/>
-      <c r="B10" s="14"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -3394,13 +3394,13 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="54" customHeight="1">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="72" t="s">
         <v>80</v>
       </c>
       <c r="D11" s="5">
@@ -3409,69 +3409,69 @@
       <c r="E11" s="5"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="82" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="54" customHeight="1">
-      <c r="A12" s="75"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="74"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="5">
         <v>200437</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="2"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="82" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="54" customHeight="1">
-      <c r="A13" s="75"/>
-      <c r="B13" s="71"/>
-      <c r="C13" s="74"/>
+      <c r="A13" s="74"/>
+      <c r="B13" s="70"/>
+      <c r="C13" s="73"/>
       <c r="D13" s="5">
         <v>310111</v>
       </c>
       <c r="E13" s="5"/>
       <c r="F13" s="2"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="82" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="54" customHeight="1">
-      <c r="A14" s="75"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="74"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="73"/>
       <c r="D14" s="5">
         <v>528401</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="2"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="82" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="54" customHeight="1">
-      <c r="A15" s="75"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="74"/>
+      <c r="A15" s="74"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="73"/>
       <c r="D15" s="5">
         <v>1076753</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="2"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="11" t="s">
+      <c r="H15" s="82" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="5"/>
-      <c r="B16" s="71"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
@@ -3483,8 +3483,8 @@
       <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="71"/>
-      <c r="C17" s="28" t="s">
+      <c r="B17" s="70"/>
+      <c r="C17" s="27" t="s">
         <v>81</v>
       </c>
       <c r="D17" s="5" t="s">
@@ -3493,7 +3493,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="2"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3555,7 +3555,7 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:B13"/>
     </sheetView>
   </sheetViews>
@@ -3567,32 +3567,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="69" t="s">
         <v>48</v>
       </c>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="72"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="71"/>
       <c r="F2" s="1" t="s">
         <v>41</v>
       </c>
@@ -3610,26 +3610,26 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>64</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2"/>
-      <c r="B4" s="14"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -3644,23 +3644,23 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="19" t="s">
         <v>22</v>
       </c>
       <c r="I5" s="2"/>
@@ -3669,7 +3669,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="2"/>
-      <c r="B6" s="14"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -3683,26 +3683,26 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>76</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
       <c r="I7" s="2"/>
       <c r="J7" s="4"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="2"/>
-      <c r="B8" s="14"/>
+      <c r="B8" s="13"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -3717,7 +3717,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>72</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -3727,16 +3727,16 @@
         <v>36</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="20"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="5"/>
-      <c r="B10" s="14"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -3751,10 +3751,10 @@
       <c r="A11" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>85</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -3772,7 +3772,7 @@
     </row>
     <row r="12" spans="1:11" ht="30" customHeight="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="71"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -3786,8 +3786,8 @@
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="27" t="s">
+      <c r="B13" s="70"/>
+      <c r="C13" s="26" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -3803,7 +3803,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="5"/>
-      <c r="B14" s="17"/>
+      <c r="B14" s="16"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
@@ -3816,7 +3816,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="5"/>
-      <c r="B15" s="17"/>
+      <c r="B15" s="16"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
@@ -3828,13 +3828,13 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="B16" s="17"/>
+      <c r="B16" s="16"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="16"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
@@ -3867,7 +3867,7 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -3886,86 +3886,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="70" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
     </row>
     <row r="2" spans="1:13" ht="45">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>19</v>
       </c>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="60" customHeight="1">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="D3" s="14">
+      <c r="D3" s="13">
         <v>145879</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="23" t="s">
         <v>23</v>
       </c>
       <c r="J3" s="2" t="s">
@@ -3979,27 +3979,27 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" customHeight="1">
-      <c r="A4" s="76"/>
-      <c r="B4" s="71" t="s">
+      <c r="A4" s="75"/>
+      <c r="B4" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="79"/>
-      <c r="D4" s="14">
+      <c r="C4" s="78"/>
+      <c r="D4" s="13">
         <v>200437</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="23" t="s">
         <v>22</v>
       </c>
       <c r="J4" s="2"/>
@@ -4007,25 +4007,25 @@
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="30" customHeight="1">
-      <c r="A5" s="76"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="14">
+      <c r="A5" s="75"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="13">
         <v>310111</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="23" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="2"/>
@@ -4033,25 +4033,25 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:13" ht="30" customHeight="1">
-      <c r="A6" s="76"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="14">
+      <c r="A6" s="75"/>
+      <c r="B6" s="70"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="13">
         <v>528401</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="23" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="2"/>
@@ -4059,25 +4059,25 @@
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="30" customHeight="1">
-      <c r="A7" s="76"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="79"/>
-      <c r="D7" s="14">
+      <c r="A7" s="75"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="13">
         <v>1076753</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="23" t="s">
         <v>23</v>
       </c>
       <c r="J7" s="2"/>
@@ -4088,7 +4088,7 @@
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="14"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
@@ -4098,25 +4098,25 @@
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:13" ht="48" customHeight="1">
-      <c r="A9" s="76" t="s">
+      <c r="A9" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="76" t="s">
+      <c r="B9" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="13">
         <v>145879</v>
       </c>
-      <c r="E9" s="77" t="s">
+      <c r="E9" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="77"/>
-      <c r="G9" s="77"/>
-      <c r="H9" s="77"/>
-      <c r="I9" s="78" t="s">
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="77" t="s">
         <v>22</v>
       </c>
       <c r="J9" s="2" t="s">
@@ -4130,64 +4130,64 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="48" customHeight="1">
-      <c r="A10" s="76"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="79"/>
-      <c r="D10" s="14">
+      <c r="A10" s="75"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="13">
         <v>200437</v>
       </c>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="78"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="77"/>
       <c r="J10" s="2"/>
       <c r="K10" s="4"/>
       <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="48" customHeight="1">
-      <c r="A11" s="76"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="79"/>
-      <c r="D11" s="14">
+      <c r="A11" s="75"/>
+      <c r="B11" s="75"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="13">
         <v>310111</v>
       </c>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="78"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
       <c r="J11" s="2"/>
       <c r="K11" s="4"/>
       <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="48" customHeight="1">
-      <c r="A12" s="76"/>
-      <c r="B12" s="76"/>
-      <c r="C12" s="79"/>
-      <c r="D12" s="14">
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="13">
         <v>528401</v>
       </c>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
-      <c r="H12" s="77"/>
-      <c r="I12" s="78"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="77"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="48" customHeight="1">
-      <c r="A13" s="76"/>
-      <c r="B13" s="76"/>
-      <c r="C13" s="79"/>
-      <c r="D13" s="14">
+      <c r="A13" s="75"/>
+      <c r="B13" s="75"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="13">
         <v>1076753</v>
       </c>
-      <c r="E13" s="77"/>
-      <c r="F13" s="77"/>
-      <c r="G13" s="77"/>
-      <c r="H13" s="77"/>
-      <c r="I13" s="78"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="76"/>
+      <c r="H13" s="76"/>
+      <c r="I13" s="77"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
@@ -4256,7 +4256,7 @@
   </sheetPr>
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
@@ -4276,72 +4276,72 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="70" t="s">
+      <c r="A1" s="13"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:14" ht="45">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>500</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="12" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="165">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>61</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -4350,13 +4350,13 @@
       <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="80" t="s">
+      <c r="F3" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="80"/>
-      <c r="H3" s="80"/>
-      <c r="I3" s="80"/>
-      <c r="J3" s="21" t="s">
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="20" t="s">
         <v>45</v>
       </c>
       <c r="K3" s="2" t="s">
@@ -4370,7 +4370,7 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="14"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -4385,28 +4385,28 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="255" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="77" t="s">
+      <c r="F5" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="23" t="s">
+      <c r="G5" s="76"/>
+      <c r="H5" s="76"/>
+      <c r="I5" s="76"/>
+      <c r="J5" s="22" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="2" t="s">
@@ -4450,20 +4450,20 @@
       <c r="M7" s="5"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="A9" s="51" t="s">
+      <c r="A9" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="51"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="51"/>
-      <c r="L9" s="51"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="5" t="s">
@@ -4513,8 +4513,8 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4526,29 +4526,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="49.5" customHeight="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="71" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="71" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="72"/>
+      <c r="G1" s="71"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="70"/>
-      <c r="B2" s="72"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="72"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="71"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>42</v>
@@ -4561,17 +4561,17 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="25" t="s">
         <v>66</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="82" t="s">
         <v>45</v>
       </c>
     </row>
@@ -4585,20 +4585,20 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="25" t="s">
         <v>60</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="2"/>
@@ -4621,20 +4621,20 @@
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>77</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4656,7 +4656,7 @@
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -4666,10 +4666,10 @@
         <v>36</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4726,13 +4726,13 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="51"/>
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="50"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
@@ -4775,8 +4775,8 @@
   </sheetPr>
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4790,23 +4790,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" customHeight="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="71" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="71" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="72"/>
+      <c r="G1" s="71"/>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
@@ -4815,10 +4815,10 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" customHeight="1">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="A2" s="69"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
       <c r="E2" s="1"/>
       <c r="F2" s="10" t="s">
         <v>42</v>
@@ -4837,20 +4837,20 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>63</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="20" t="s">
         <v>45</v>
       </c>
       <c r="H3" s="2"/>
@@ -4862,8 +4862,8 @@
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="30"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="2"/>
       <c r="M4" s="2"/>
     </row>
@@ -4874,17 +4874,17 @@
       <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>59</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="5"/>
@@ -4896,8 +4896,8 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="30"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="29"/>
       <c r="H6" s="5"/>
       <c r="M6" s="5"/>
     </row>
@@ -4905,20 +4905,20 @@
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>75</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="22" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="5"/>
@@ -4930,8 +4930,8 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="30"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="29"/>
       <c r="H8" s="5"/>
       <c r="M8" s="5"/>
     </row>
@@ -4939,7 +4939,7 @@
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>73</v>
       </c>
       <c r="C9" s="5" t="s">
@@ -4949,10 +4949,10 @@
         <v>36</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="23" t="s">
+      <c r="G9" s="22" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="5"/>
@@ -4964,29 +4964,29 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
       <c r="H10" s="5"/>
       <c r="M10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="270" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>84</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>36</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="20" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="5"/>
@@ -4994,91 +4994,91 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="5"/>
-      <c r="B12" s="71"/>
+      <c r="B12" s="70"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="29"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="5"/>
       <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="54" customHeight="1">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="71"/>
-      <c r="C13" s="81" t="s">
+      <c r="B13" s="70"/>
+      <c r="C13" s="80" t="s">
         <v>83</v>
       </c>
       <c r="D13" s="5">
         <v>145879</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="78" t="s">
+      <c r="F13" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="24" t="s">
         <v>23</v>
       </c>
       <c r="H13" s="5"/>
       <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="54" customHeight="1">
-      <c r="A14" s="76"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="81"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="70"/>
+      <c r="C14" s="80"/>
       <c r="D14" s="5">
         <v>200437</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="25" t="s">
+      <c r="F14" s="79"/>
+      <c r="G14" s="24" t="s">
         <v>23</v>
       </c>
       <c r="H14" s="5"/>
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="54" customHeight="1">
-      <c r="A15" s="76"/>
-      <c r="B15" s="71"/>
-      <c r="C15" s="81"/>
+      <c r="A15" s="75"/>
+      <c r="B15" s="70"/>
+      <c r="C15" s="80"/>
       <c r="D15" s="5">
         <v>310111</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="31" t="s">
+      <c r="F15" s="79"/>
+      <c r="G15" s="30" t="s">
         <v>23</v>
       </c>
       <c r="H15" s="5"/>
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="54" customHeight="1">
-      <c r="A16" s="76"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="81"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="70"/>
+      <c r="C16" s="80"/>
       <c r="D16" s="5">
         <v>528401</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="31" t="s">
+      <c r="F16" s="79"/>
+      <c r="G16" s="30" t="s">
         <v>23</v>
       </c>
       <c r="H16" s="5"/>
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" ht="54" customHeight="1">
-      <c r="A17" s="76"/>
-      <c r="B17" s="71"/>
-      <c r="C17" s="81"/>
+      <c r="A17" s="75"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="80"/>
       <c r="D17" s="5">
         <v>1076753</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="31" t="s">
+      <c r="F17" s="79"/>
+      <c r="G17" s="30" t="s">
         <v>23</v>
       </c>
       <c r="H17" s="5"/>

</xml_diff>

<commit_message>
Updates to mSigHdp-paper-tracking.xlsx - now NR_hdp_gb_20 jobs have started running on SBS_2/Realistic
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E00D9F0-AC06-4122-9BFA-2239324B9914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5593DD0-BF47-44E1-B5D6-FCCDAC71A026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="2010" windowWidth="17490" windowHeight="13860" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="134">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -492,6 +492,341 @@
 Arguments for function mSigHdp::SetupAndPosterior():
 GLOBAL.gamma.alpha = 1,
 GLOBAL.gamma.beta = 1</t>
+  </si>
+  <si>
+    <t>Arguments for function mSigHdp::RunHdpParallel():
+K.guess = 22,
+multi.types = TRUE,
+post.burnin = 5000 * 6,
+post.n = 200,
+post.space = 100,
+post.cpiter = 3,
+num.child.process = 20,
+CPU.cores = 20,
+cos.merge = 0.9,
+min.sample = 1
+Arguments for function mSigHdp::SetupAndPosterior():
+GLOBAL.gamma.alpha = 1,
+GLOBAL.gamma.beta = 50</t>
+  </si>
+  <si>
+    <t>Arguments for function mSigHdp::RunHdpParallel():
+K.guess = 26,
+multi.types = TRUE,
+post.burnin = 5000 * 6,
+post.n = 200,
+post.space = 100,
+post.cpiter = 3,
+num.child.process = 20,
+CPU.cores = 20,
+cos.merge = 0.9,
+min.sample = 1
+Arguments for function mSigHdp::SetupAndPosterior():
+GLOBAL.gamma.alpha = 1,
+GLOBAL.gamma.beta = 50</t>
+  </si>
+  <si>
+    <t>Arguments for function mSigHdp::RunHdpParallel():
+K.guess = 26,
+multi.types = TRUE,
+post.burnin = 5000 * 6,
+post.n = 200,
+post.space = 100,
+post.cpiter = 3,
+num.child.process = 20,
+CPU.cores = 20,
+cos.merge = 0.9,
+min.sample = 1
+Arguments for function mSigHdp::SetupAndPosterior():
+GLOBAL.gamma.alpha = 1,
+GLOBAL.gamma.beta = 1</t>
+  </si>
+  <si>
+    <t>Arguments for function mSigHdp::RunHdpParallel():
+K.guess = 22,
+multi.types = TRUE,
+post.burnin = 5000 * 6,
+post.n = 200,
+post.space = 100,
+post.cpiter = 3,
+num.child.process = 20,
+CPU.cores = 20,
+cos.merge = 0.9,
+min.sample = 1
+Arguments for function mSigHdp::SetupAndPosterior():
+GLOBAL.gamma.alpha = 1,
+GLOBAL.gamma.beta = 1</t>
+  </si>
+  <si>
+    <t>Benchmarking mSigHdp in the original submission and proposed additional benchmarking </t>
+  </si>
+  <si>
+    <t>  </t>
+  </si>
+  <si>
+    <t> = benchmarking in the original submission </t>
+  </si>
+  <si>
+    <t>= additional benchmarking in revision </t>
+  </si>
+  <si>
+    <t>SBS  data sets </t>
+  </si>
+  <si>
+    <t>Synthetic data set 1 </t>
+  </si>
+  <si>
+    <t>Synthetic data set 2 </t>
+  </si>
+  <si>
+    <t>Noise </t>
+  </si>
+  <si>
+    <t>Approach </t>
+  </si>
+  <si>
+    <t>None </t>
+  </si>
+  <si>
+    <t>Moderate </t>
+  </si>
+  <si>
+    <t>Realistic </t>
+  </si>
+  <si>
+    <t>mSigHdp no downsampling </t>
+  </si>
+  <si>
+    <t>original submission </t>
+  </si>
+  <si>
+    <t>done </t>
+  </si>
+  <si>
+    <t>SigProfilerExtractor </t>
+  </si>
+  <si>
+    <t>SignatureAnalyzer </t>
+  </si>
+  <si>
+    <t>signeR </t>
+  </si>
+  <si>
+    <t>Original hdp with programming errors corrected </t>
+  </si>
+  <si>
+    <t>gamma.beta = 1</t>
+  </si>
+  <si>
+    <t>Pending for available resources</t>
+  </si>
+  <si>
+    <t>gamma.beta = 20</t>
+  </si>
+  <si>
+    <t>Not yet runned</t>
+  </si>
+  <si>
+    <t>Indel data sets </t>
+  </si>
+  <si>
+    <t>gamma.beta = 50</t>
+  </si>
+  <si>
+    <t>Some runs failed</t>
+  </si>
+  <si>
+    <t>hpc-long</t>
+  </si>
+  <si>
+    <t>hpc-super</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Running on monster2</t>
+  </si>
+  <si>
+    <t>Running
+on minimonster</t>
+  </si>
+  <si>
+    <t> = additional benchmarking running</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = additional benchmarking done</t>
+  </si>
+  <si>
+    <t>Running on HPC-cluster, queue "long"</t>
+  </si>
+  <si>
+    <t>10k downsampling</t>
+  </si>
+  <si>
+    <t>5k downsampling</t>
+  </si>
+  <si>
+    <t>3k downsampling</t>
+  </si>
+  <si>
+    <r>
+      <t>SigPro</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1k downsampling </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"non-hyper" - removed all spectra with &gt;10k mutations</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1k downsampling</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SigProfilerExtractor</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <t>Running on HPC-cluster, queue "super"</t>
+  </si>
+  <si>
+    <r>
+      <t>10k downsampling</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5k downsampling</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3k downsampling</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> = Data sets not included in Prof Steve's revision plan</t>
+    </r>
+  </si>
+  <si>
+    <t>Arguments for function mSigHdp::RunHdpParallel():
+K.guess = 64,
+multi.types = TRUE,
+post.burnin = 5000 * 20,
+post.n = 200,
+post.space = 100,
+post.cpiter = 3,
+num.child.process = 20,
+CPU.cores = 20,
+cos.merge = 0.9,
+min.sample = 1
+Arguments for function mSigHdp::SetupAndPosterior():
+GLOBAL.gamma.alpha = 1,
+GLOBAL.gamma.beta = 20</t>
   </si>
   <si>
     <r>
@@ -533,326 +868,7 @@
         <scheme val="minor"/>
       </rPr>
       <t>GLOBAL.gamma.alpha = 1,
-GLOBAL.gamma.beta = 50</t>
-    </r>
-  </si>
-  <si>
-    <t>Arguments for function mSigHdp::RunHdpParallel():
-K.guess = 22,
-multi.types = TRUE,
-post.burnin = 5000 * 6,
-post.n = 200,
-post.space = 100,
-post.cpiter = 3,
-num.child.process = 20,
-CPU.cores = 20,
-cos.merge = 0.9,
-min.sample = 1
-Arguments for function mSigHdp::SetupAndPosterior():
-GLOBAL.gamma.alpha = 1,
-GLOBAL.gamma.beta = 50</t>
-  </si>
-  <si>
-    <t>Arguments for function mSigHdp::RunHdpParallel():
-K.guess = 26,
-multi.types = TRUE,
-post.burnin = 5000 * 6,
-post.n = 200,
-post.space = 100,
-post.cpiter = 3,
-num.child.process = 20,
-CPU.cores = 20,
-cos.merge = 0.9,
-min.sample = 1
-Arguments for function mSigHdp::SetupAndPosterior():
-GLOBAL.gamma.alpha = 1,
-GLOBAL.gamma.beta = 50</t>
-  </si>
-  <si>
-    <t>Arguments for function mSigHdp::RunHdpParallel():
-K.guess = 26,
-multi.types = TRUE,
-post.burnin = 5000 * 6,
-post.n = 200,
-post.space = 100,
-post.cpiter = 3,
-num.child.process = 20,
-CPU.cores = 20,
-cos.merge = 0.9,
-min.sample = 1
-Arguments for function mSigHdp::SetupAndPosterior():
-GLOBAL.gamma.alpha = 1,
-GLOBAL.gamma.beta = 1</t>
-  </si>
-  <si>
-    <t>Arguments for function mSigHdp::RunHdpParallel():
-K.guess = 22,
-multi.types = TRUE,
-post.burnin = 5000 * 6,
-post.n = 200,
-post.space = 100,
-post.cpiter = 3,
-num.child.process = 20,
-CPU.cores = 20,
-cos.merge = 0.9,
-min.sample = 1
-Arguments for function mSigHdp::SetupAndPosterior():
-GLOBAL.gamma.alpha = 1,
-GLOBAL.gamma.beta = 1</t>
-  </si>
-  <si>
-    <t>Benchmarking mSigHdp in the original submission and proposed additional benchmarking </t>
-  </si>
-  <si>
-    <t>  </t>
-  </si>
-  <si>
-    <t> = benchmarking in the original submission </t>
-  </si>
-  <si>
-    <t>= additional benchmarking in revision </t>
-  </si>
-  <si>
-    <t>SBS  data sets </t>
-  </si>
-  <si>
-    <t>Synthetic data set 1 </t>
-  </si>
-  <si>
-    <t>Synthetic data set 2 </t>
-  </si>
-  <si>
-    <t>Noise </t>
-  </si>
-  <si>
-    <t>Approach </t>
-  </si>
-  <si>
-    <t>None </t>
-  </si>
-  <si>
-    <t>Moderate </t>
-  </si>
-  <si>
-    <t>Realistic </t>
-  </si>
-  <si>
-    <t>mSigHdp no downsampling </t>
-  </si>
-  <si>
-    <t>original submission </t>
-  </si>
-  <si>
-    <t>done </t>
-  </si>
-  <si>
-    <t>SigProfilerExtractor </t>
-  </si>
-  <si>
-    <t>SignatureAnalyzer </t>
-  </si>
-  <si>
-    <t>signeR </t>
-  </si>
-  <si>
-    <t>Original hdp with programming errors corrected </t>
-  </si>
-  <si>
-    <t>gamma.beta = 1</t>
-  </si>
-  <si>
-    <t>Pending for available resources</t>
-  </si>
-  <si>
-    <t>gamma.beta = 20</t>
-  </si>
-  <si>
-    <t>Not yet runned</t>
-  </si>
-  <si>
-    <t>Indel data sets </t>
-  </si>
-  <si>
-    <t>gamma.beta = 50</t>
-  </si>
-  <si>
-    <t>Some runs failed</t>
-  </si>
-  <si>
-    <t>hpc-long</t>
-  </si>
-  <si>
-    <t>hpc-super</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>Running on monster2</t>
-  </si>
-  <si>
-    <t>Running
-on minimonster</t>
-  </si>
-  <si>
-    <t> = additional benchmarking running</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> = additional benchmarking done</t>
-  </si>
-  <si>
-    <t>Running on HPC-cluster, queue "long"</t>
-  </si>
-  <si>
-    <t>10k downsampling</t>
-  </si>
-  <si>
-    <t>5k downsampling</t>
-  </si>
-  <si>
-    <t>3k downsampling</t>
-  </si>
-  <si>
-    <r>
-      <t>SigPro</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1k downsampling </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>"non-hyper" - removed all spectra with &gt;10k mutations</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1k downsampling</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>SigProfilerExtractor</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Running on HPC-cluster, queue "super"</t>
-  </si>
-  <si>
-    <r>
-      <t>10k downsampling</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>5k downsampling</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3k downsampling</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> = Data sets not included in Prof Steve's revision plan</t>
+GLOBAL.gamma.beta = 20</t>
     </r>
   </si>
 </sst>
@@ -1443,7 +1459,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2006,16 +2022,16 @@
         <v>145879</v>
       </c>
       <c r="E3" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F3" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I3" s="78" t="s">
         <v>2</v>
@@ -2035,16 +2051,16 @@
         <v>200437</v>
       </c>
       <c r="E4" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F4" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I4" s="78"/>
       <c r="J4" s="84"/>
@@ -2058,16 +2074,16 @@
         <v>310111</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F5" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G5" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H5" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I5" s="78"/>
       <c r="J5" s="84"/>
@@ -2081,16 +2097,16 @@
         <v>528401</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F6" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H6" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I6" s="78"/>
       <c r="J6" s="84"/>
@@ -2104,16 +2120,16 @@
         <v>1076753</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F7" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G7" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H7" s="51" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I7" s="78"/>
       <c r="J7" s="84"/>
@@ -2327,19 +2343,19 @@
         <v>145879</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J3" s="78" t="s">
         <v>2</v>
@@ -2359,19 +2375,19 @@
         <v>200437</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J4" s="78"/>
       <c r="K4" s="84"/>
@@ -2385,19 +2401,19 @@
         <v>310111</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J5" s="78"/>
       <c r="K5" s="84"/>
@@ -2411,19 +2427,19 @@
         <v>528401</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J6" s="78"/>
       <c r="K6" s="84"/>
@@ -2437,19 +2453,19 @@
         <v>1076753</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J7" s="78"/>
       <c r="K7" s="84"/>
@@ -2557,7 +2573,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" customHeight="1">
       <c r="A1" s="64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -2577,7 +2593,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -2588,10 +2604,10 @@
     </row>
     <row r="4" spans="1:13" ht="25.5" customHeight="1">
       <c r="A4" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="44" t="s">
         <v>87</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>88</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="44"/>
@@ -2599,10 +2615,10 @@
       <c r="F4" s="44"/>
       <c r="G4" s="41"/>
       <c r="H4" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" s="41"/>
       <c r="K4" s="41"/>
@@ -2611,10 +2627,10 @@
     </row>
     <row r="5" spans="1:13" ht="25.5" customHeight="1">
       <c r="A5" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
@@ -2622,10 +2638,10 @@
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
       <c r="H5" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J5" s="41"/>
       <c r="K5" s="41"/>
@@ -2646,7 +2662,7 @@
       <c r="A7" s="30"/>
       <c r="B7" s="30"/>
       <c r="C7" s="65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D7" s="65"/>
       <c r="E7" s="65"/>
@@ -2657,12 +2673,12 @@
       <c r="A8" s="30"/>
       <c r="B8" s="30"/>
       <c r="C8" s="66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" s="66"/>
       <c r="E8" s="66"/>
       <c r="F8" s="68" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G8" s="68"/>
     </row>
@@ -2670,126 +2686,126 @@
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D9" s="67"/>
       <c r="E9" s="67"/>
       <c r="F9" s="67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="67"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1">
       <c r="A10" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D10" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="33" t="s">
+      <c r="E10" s="33" t="s">
         <v>96</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>97</v>
       </c>
       <c r="F10" s="33" t="s">
         <v>41</v>
       </c>
       <c r="G10" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51.75" thickBot="1">
       <c r="A11" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D11" s="56"/>
       <c r="E11" s="57"/>
       <c r="F11" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="39" thickBot="1">
       <c r="A12" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="58"/>
       <c r="D12" s="59"/>
       <c r="E12" s="60"/>
       <c r="F12" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="26.25" thickBot="1">
       <c r="A13" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="58"/>
       <c r="D13" s="59"/>
       <c r="E13" s="60"/>
       <c r="F13" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1">
       <c r="A14" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="61"/>
       <c r="D14" s="62"/>
       <c r="E14" s="63"/>
       <c r="F14" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="64.5" customHeight="1" thickBot="1">
       <c r="A15" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="34" t="s">
         <v>104</v>
-      </c>
-      <c r="B15" s="34" t="s">
-        <v>105</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="30"/>
       <c r="E15" s="36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="51.75" thickBot="1">
       <c r="A16" s="54"/>
       <c r="B16" s="34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
       <c r="E16" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
@@ -2797,92 +2813,92 @@
         <v>10</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
       <c r="E17" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G17" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
       <c r="A18" s="54"/>
       <c r="B18" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
       <c r="E18" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G18" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
       <c r="A19" s="54"/>
       <c r="B19" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G19" s="39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
       <c r="A20" s="54"/>
       <c r="B20" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
       <c r="E20" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="39" thickBot="1">
       <c r="A21" s="54" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="39" thickBot="1">
       <c r="A22" s="54"/>
       <c r="B22" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="39" thickBot="1">
       <c r="A23" s="54"/>
       <c r="B23" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39" thickBot="1">
       <c r="A24" s="54"/>
       <c r="B24" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -2918,7 +2934,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="25.5" customHeight="1">
       <c r="A1" s="64" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B1" s="64"/>
       <c r="C1" s="64"/>
@@ -2938,7 +2954,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -2949,10 +2965,10 @@
     </row>
     <row r="4" spans="1:12" ht="25.5" customHeight="1">
       <c r="A4" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="44" t="s">
         <v>87</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>88</v>
       </c>
       <c r="C4" s="44"/>
       <c r="D4" s="44"/>
@@ -2960,10 +2976,10 @@
       <c r="F4" s="44"/>
       <c r="G4" s="41"/>
       <c r="H4" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I4" s="44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J4" s="41"/>
       <c r="K4" s="41"/>
@@ -2971,10 +2987,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1">
       <c r="A5" s="32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
@@ -2982,10 +2998,10 @@
       <c r="F5" s="41"/>
       <c r="G5" s="41"/>
       <c r="H5" s="45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I5" s="44" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J5" s="41"/>
       <c r="K5" s="41"/>
@@ -3013,7 +3029,7 @@
       <c r="A8" s="30"/>
       <c r="B8" s="30"/>
       <c r="C8" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D8" s="65"/>
       <c r="E8" s="65"/>
@@ -3024,12 +3040,12 @@
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" s="66"/>
       <c r="E9" s="66"/>
       <c r="F9" s="66" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G9" s="66"/>
     </row>
@@ -3037,12 +3053,12 @@
       <c r="A10" s="30"/>
       <c r="B10" s="30"/>
       <c r="C10" s="67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D10" s="67"/>
       <c r="E10" s="67"/>
       <c r="F10" s="67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G10" s="67"/>
     </row>
@@ -3050,117 +3066,117 @@
       <c r="A11" s="30"/>
       <c r="B11" s="30"/>
       <c r="C11" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="E11" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="33" t="s">
-        <v>97</v>
-      </c>
       <c r="F11" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="51.75" thickBot="1">
       <c r="A12" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="34"/>
       <c r="C12" s="55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D12" s="56"/>
       <c r="E12" s="57"/>
       <c r="F12" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="39" thickBot="1">
       <c r="A13" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B13" s="34"/>
       <c r="C13" s="58"/>
       <c r="D13" s="59"/>
       <c r="E13" s="60"/>
       <c r="F13" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="26.25" thickBot="1">
       <c r="A14" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B14" s="34"/>
       <c r="C14" s="58"/>
       <c r="D14" s="59"/>
       <c r="E14" s="60"/>
       <c r="F14" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1">
       <c r="A15" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" s="34"/>
       <c r="C15" s="61"/>
       <c r="D15" s="62"/>
       <c r="E15" s="63"/>
       <c r="F15" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G15" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="64.5" customHeight="1" thickBot="1">
       <c r="A16" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B16" s="34" t="s">
         <v>104</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>105</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
       <c r="E16" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="26.25" thickBot="1">
       <c r="A17" s="54"/>
       <c r="B17" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
       <c r="E17" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F17" s="43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G17" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="39" thickBot="1">
@@ -3168,27 +3184,27 @@
         <v>10</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
       <c r="E18" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F18" s="30"/>
       <c r="G18" s="69" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="39" thickBot="1">
       <c r="A19" s="54"/>
       <c r="B19" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F19" s="30"/>
       <c r="G19" s="70"/>
@@ -3196,12 +3212,12 @@
     <row r="20" spans="1:7" ht="39" thickBot="1">
       <c r="A20" s="54"/>
       <c r="B20" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
       <c r="E20" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" s="30"/>
       <c r="G20" s="70"/>
@@ -3209,84 +3225,79 @@
     <row r="21" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
       <c r="A21" s="54"/>
       <c r="B21" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G21" s="70"/>
     </row>
     <row r="22" spans="1:7" ht="90" thickBot="1">
       <c r="A22" s="54"/>
       <c r="B22" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G22" s="71"/>
     </row>
     <row r="23" spans="1:7" ht="39" thickBot="1">
       <c r="A23" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="G23" s="69" t="s">
         <v>127</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>100</v>
-      </c>
-      <c r="G23" s="69" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39" thickBot="1">
       <c r="A24" s="54"/>
       <c r="B24" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G24" s="70"/>
     </row>
     <row r="25" spans="1:7" ht="39" thickBot="1">
       <c r="A25" s="54"/>
       <c r="B25" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E25" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G25" s="70"/>
     </row>
     <row r="26" spans="1:7" ht="39" thickBot="1">
       <c r="A26" s="54"/>
       <c r="B26" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E26" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G26" s="70"/>
     </row>
     <row r="27" spans="1:7" ht="90" thickBot="1">
       <c r="A27" s="54"/>
       <c r="B27" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E27" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G27" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:G10"/>
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="G23:G27"/>
     <mergeCell ref="G18:G22"/>
@@ -3294,6 +3305,11 @@
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="C12:E15"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3307,8 +3323,8 @@
   </sheetPr>
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3557,11 +3573,11 @@
     </row>
     <row r="17" spans="1:8" ht="270" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B17" s="73"/>
       <c r="C17" s="25" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>36</v>
@@ -3831,7 +3847,7 @@
         <v>46</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>36</v>
@@ -3864,7 +3880,7 @@
       </c>
       <c r="B13" s="73"/>
       <c r="C13" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>36</v>
@@ -3943,8 +3959,8 @@
   </sheetPr>
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4333,7 +4349,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4587,10 +4603,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4601,7 +4617,7 @@
     <col min="6" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="49.5" customHeight="1">
+    <row r="1" spans="1:14" ht="49.5" customHeight="1">
       <c r="A1" s="72" t="s">
         <v>4</v>
       </c>
@@ -4620,7 +4636,7 @@
       </c>
       <c r="G1" s="74"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:14">
       <c r="A2" s="72"/>
       <c r="B2" s="74"/>
       <c r="C2" s="72"/>
@@ -4633,7 +4649,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="36" customHeight="1">
+    <row r="3" spans="1:14" ht="36" customHeight="1">
       <c r="A3" s="78" t="s">
         <v>10</v>
       </c>
@@ -4647,14 +4663,11 @@
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="85" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="36" customHeight="1">
+    </row>
+    <row r="4" spans="1:14" ht="36" customHeight="1">
       <c r="A4" s="78"/>
       <c r="B4" s="73"/>
       <c r="C4" s="53"/>
@@ -4662,14 +4675,11 @@
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="36" customHeight="1">
+    </row>
+    <row r="5" spans="1:14" ht="36" customHeight="1">
       <c r="A5" s="78"/>
       <c r="B5" s="73"/>
       <c r="C5" s="53"/>
@@ -4677,14 +4687,11 @@
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="85" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="36" customHeight="1">
+    </row>
+    <row r="6" spans="1:14" ht="36" customHeight="1">
       <c r="A6" s="78"/>
       <c r="B6" s="73"/>
       <c r="C6" s="53"/>
@@ -4692,14 +4699,11 @@
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="36" customHeight="1">
+    </row>
+    <row r="7" spans="1:14" ht="36" customHeight="1">
       <c r="A7" s="78"/>
       <c r="B7" s="73"/>
       <c r="C7" s="53"/>
@@ -4707,20 +4711,17 @@
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="21" t="s">
+      <c r="F7" s="85" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="85" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="240">
+    <row r="9" spans="1:14" ht="240">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -4742,21 +4743,21 @@
       </c>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:14">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:14">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="30">
+    <row r="12" spans="1:14" ht="30">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -4777,21 +4778,21 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:14">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:14">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="75">
+    <row r="15" spans="1:14" ht="75" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>26</v>
       </c>
@@ -4812,15 +4813,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:14">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="5" t="s">
+      <c r="N16" s="14"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="5"/>
@@ -4829,75 +4831,137 @@
         <v>36</v>
       </c>
       <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="N17" s="14"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="N18" s="14"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="5"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="N19" s="14"/>
+    </row>
+    <row r="20" spans="1:14" ht="54" customHeight="1">
+      <c r="A20" s="78" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="83" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="75" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="5">
+        <v>145879</v>
+      </c>
       <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="G20" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="14"/>
+    </row>
+    <row r="21" spans="1:14" ht="54" customHeight="1">
+      <c r="A21" s="78"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="5">
+        <v>200437</v>
+      </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="53"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="53"/>
-      <c r="E22" s="53"/>
-      <c r="F22" s="53"/>
-      <c r="G22" s="53"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="5" t="s">
+      <c r="G21" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="14"/>
+    </row>
+    <row r="22" spans="1:14" ht="54" customHeight="1">
+      <c r="A22" s="78"/>
+      <c r="B22" s="83"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="5">
+        <v>310111</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="G22" s="47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="54" customHeight="1">
+      <c r="A23" s="78"/>
+      <c r="B23" s="83"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="5">
+        <v>528401</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="G23" s="47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="54" customHeight="1">
+      <c r="A24" s="78"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="5">
+        <v>1076753</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="G24" s="47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="53"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="53"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" t="s">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
+    <row r="29" spans="1:14">
+      <c r="A29" t="s">
         <v>44</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="A20:A24"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A26:G26"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -4905,8 +4969,10 @@
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
+    <mergeCell ref="C20:C24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5119,7 +5185,7 @@
         <v>46</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>36</v>
@@ -5151,7 +5217,7 @@
       </c>
       <c r="B13" s="73"/>
       <c r="C13" s="83" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D13" s="5">
         <v>145879</v>

</xml_diff>

<commit_message>
Started to run signeR for indel_set1/Realistic, on HPC-cluster
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFEB8528-953C-4C04-8ACA-899E9D1AA02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF799D9-8BD5-464B-86FA-AC378EA08931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="1080" windowWidth="15375" windowHeight="12855" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2010" yWindow="1005" windowWidth="15375" windowHeight="12855" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="221">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -454,11 +454,6 @@
   </si>
   <si>
     <t>K_range = c(2, 20)</t>
-  </si>
-  <si>
-    <t>signeR = 1.18.1; 
-NMF = 0.30.1;
-Wrapper function SynSigRun::RunsigneR(), SynSigRun = 1.0.0</t>
   </si>
   <si>
     <t>signeR = 1.20.0;
@@ -1319,6 +1314,61 @@
   <si>
     <t>m2 (e0240162)
 &lt;192035&gt;</t>
+  </si>
+  <si>
+    <t>mm (wuyang)
+&lt;2209953&gt;</t>
+  </si>
+  <si>
+    <t>mm (wuyang)
+&lt;2210233&gt;</t>
+  </si>
+  <si>
+    <t>mm (wuyang)
+&lt;2210393&gt;</t>
+  </si>
+  <si>
+    <t>mm (wuyang)
+&lt;2210553&gt;</t>
+  </si>
+  <si>
+    <t>mm (wuyang)
+&lt;2210713&gt;</t>
+  </si>
+  <si>
+    <t>m2 (e0240162)
+&lt;231643&gt;</t>
+  </si>
+  <si>
+    <t>HPC
+&lt;115237&gt;
+(wuyang)</t>
+  </si>
+  <si>
+    <t>HPC
+&lt;115238&gt;
+(wuyang)</t>
+  </si>
+  <si>
+    <t>HPC
+&lt;115239&gt;
+(wuyang)</t>
+  </si>
+  <si>
+    <t>HPC
+&lt;115240&gt;
+(wuyang)</t>
+  </si>
+  <si>
+    <t>HPC
+&lt;115241&gt;
+(wuyang)</t>
+  </si>
+  <si>
+    <t>signeR = 1.20.0; 
+NMF = 0.24.0;
+Wrapper function SynSigRun::RunsigneR(), SynSigRun = 1.0.0
+(Version for rerun)</t>
   </si>
 </sst>
 </file>
@@ -1439,7 +1489,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1449,12 +1499,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1670,7 +1714,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1717,7 +1761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1732,38 +1776,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1775,48 +1819,45 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1826,7 +1867,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1838,10 +1879,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1853,31 +1894,31 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1895,13 +1936,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1931,18 +1975,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1952,10 +1996,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2441,10 +2482,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="60"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -2537,8 +2578,8 @@
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>190</v>
+      <c r="B3" s="53" t="s">
+        <v>189</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>52</v>
@@ -2547,11 +2588,11 @@
         <v>35</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="G3" s="48" t="s">
-        <v>136</v>
+      <c r="F3" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>135</v>
       </c>
       <c r="H3" s="2"/>
       <c r="M3" s="2"/>
@@ -2571,8 +2612,8 @@
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="54" t="s">
-        <v>193</v>
+      <c r="B5" s="53" t="s">
+        <v>192</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>48</v>
@@ -2581,10 +2622,10 @@
         <v>35</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="48" t="s">
         <v>22</v>
       </c>
       <c r="H5" s="5"/>
@@ -2606,19 +2647,19 @@
         <v>25</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="47" t="s">
+      <c r="F7" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="55" t="s">
+      <c r="G7" s="54" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="5"/>
@@ -2640,7 +2681,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>58</v>
@@ -2649,10 +2690,10 @@
         <v>35</v>
       </c>
       <c r="E9" s="5"/>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="55" t="s">
+      <c r="G9" s="54" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="5"/>
@@ -2677,17 +2718,17 @@
         <v>43</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="5"/>
-      <c r="F11" s="48" t="s">
-        <v>123</v>
-      </c>
-      <c r="G11" s="49" t="s">
-        <v>123</v>
+      <c r="F11" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="48" t="s">
+        <v>122</v>
       </c>
       <c r="H11" s="10"/>
       <c r="M11" s="5"/>
@@ -2705,7 +2746,7 @@
         <v>39</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M12" s="5"/>
     </row>
@@ -2715,17 +2756,17 @@
       </c>
       <c r="B13" s="80"/>
       <c r="C13" s="93" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="5">
         <v>145879</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="89" t="s">
-        <v>123</v>
-      </c>
-      <c r="G13" s="44" t="s">
-        <v>128</v>
+      <c r="F13" s="88" t="s">
+        <v>122</v>
+      </c>
+      <c r="G13" s="43" t="s">
+        <v>127</v>
       </c>
       <c r="H13" s="16" t="s">
         <v>23</v>
@@ -2740,9 +2781,9 @@
         <v>200437</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="44" t="s">
-        <v>128</v>
+      <c r="F14" s="88"/>
+      <c r="G14" s="43" t="s">
+        <v>127</v>
       </c>
       <c r="H14" s="16" t="s">
         <v>23</v>
@@ -2757,9 +2798,9 @@
         <v>310111</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="89"/>
-      <c r="G15" s="45" t="s">
-        <v>133</v>
+      <c r="F15" s="88"/>
+      <c r="G15" s="44" t="s">
+        <v>132</v>
       </c>
       <c r="H15" s="21" t="s">
         <v>23</v>
@@ -2774,9 +2815,9 @@
         <v>528401</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="45" t="s">
-        <v>133</v>
+      <c r="F16" s="88"/>
+      <c r="G16" s="44" t="s">
+        <v>132</v>
       </c>
       <c r="H16" s="21" t="s">
         <v>23</v>
@@ -2791,9 +2832,9 @@
         <v>1076753</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="45" t="s">
-        <v>133</v>
+      <c r="F17" s="88"/>
+      <c r="G17" s="44" t="s">
+        <v>132</v>
       </c>
       <c r="H17" s="21" t="s">
         <v>23</v>
@@ -2831,15 +2872,15 @@
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" ht="105" customHeight="1">
-      <c r="A20" s="60" t="s">
-        <v>135</v>
-      </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
+      <c r="A20" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="59"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
@@ -2934,10 +2975,10 @@
         <v>7</v>
       </c>
       <c r="H2" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>125</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>0</v>
@@ -2954,28 +2995,28 @@
         <v>10</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="59" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="I3" s="91" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="42" t="s">
         <v>126</v>
+      </c>
+      <c r="I3" s="89" t="s">
+        <v>125</v>
       </c>
       <c r="J3" s="85" t="s">
         <v>2</v>
@@ -2990,20 +3031,20 @@
     <row r="4" spans="1:12" ht="35.1" customHeight="1">
       <c r="A4" s="85"/>
       <c r="B4" s="80"/>
-      <c r="C4" s="60"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="I4" s="91"/>
+        <v>98</v>
+      </c>
+      <c r="I4" s="89"/>
       <c r="J4" s="85"/>
       <c r="K4" s="94"/>
       <c r="L4" s="85"/>
@@ -3011,20 +3052,20 @@
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
       <c r="A5" s="85"/>
       <c r="B5" s="80"/>
-      <c r="C5" s="60"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="I5" s="91"/>
+        <v>98</v>
+      </c>
+      <c r="I5" s="89"/>
       <c r="J5" s="85"/>
       <c r="K5" s="94"/>
       <c r="L5" s="85"/>
@@ -3032,20 +3073,20 @@
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
       <c r="A6" s="85"/>
       <c r="B6" s="80"/>
-      <c r="C6" s="60"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G6" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="I6" s="91"/>
+        <v>98</v>
+      </c>
+      <c r="I6" s="89"/>
       <c r="J6" s="85"/>
       <c r="K6" s="94"/>
       <c r="L6" s="85"/>
@@ -3053,20 +3094,20 @@
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
       <c r="A7" s="85"/>
       <c r="B7" s="80"/>
-      <c r="C7" s="60"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>99</v>
-      </c>
-      <c r="I7" s="91"/>
+        <v>98</v>
+      </c>
+      <c r="I7" s="89"/>
       <c r="J7" s="85"/>
       <c r="K7" s="94"/>
       <c r="L7" s="85"/>
@@ -3086,30 +3127,30 @@
       <c r="L8" s="2"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
     </row>
     <row r="11" spans="1:12" ht="75" customHeight="1">
-      <c r="A11" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
+      <c r="A11" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3152,12 +3193,12 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="60"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
+      <c r="A19" s="59"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5"/>
@@ -3274,28 +3315,28 @@
         <v>10</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="59" t="s">
         <v>52</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="89" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="89" t="s">
-        <v>128</v>
-      </c>
-      <c r="G3" s="89" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="89" t="s">
-        <v>128</v>
+      <c r="E3" s="88" t="s">
+        <v>127</v>
+      </c>
+      <c r="F3" s="88" t="s">
+        <v>127</v>
+      </c>
+      <c r="G3" s="88" t="s">
+        <v>127</v>
+      </c>
+      <c r="H3" s="88" t="s">
+        <v>127</v>
       </c>
       <c r="I3" s="95" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J3" s="85" t="s">
         <v>2</v>
@@ -3310,14 +3351,14 @@
     <row r="4" spans="1:13" ht="35.1" customHeight="1">
       <c r="A4" s="85"/>
       <c r="B4" s="80"/>
-      <c r="C4" s="60"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
+      <c r="E4" s="88"/>
+      <c r="F4" s="88"/>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
       <c r="I4" s="95"/>
       <c r="J4" s="85"/>
       <c r="K4" s="94"/>
@@ -3326,14 +3367,14 @@
     <row r="5" spans="1:13" ht="35.1" customHeight="1">
       <c r="A5" s="85"/>
       <c r="B5" s="80"/>
-      <c r="C5" s="60"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
       <c r="I5" s="95"/>
       <c r="J5" s="85"/>
       <c r="K5" s="94"/>
@@ -3342,14 +3383,14 @@
     <row r="6" spans="1:13" ht="35.1" customHeight="1">
       <c r="A6" s="85"/>
       <c r="B6" s="80"/>
-      <c r="C6" s="60"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="89"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
       <c r="I6" s="95"/>
       <c r="J6" s="85"/>
       <c r="K6" s="94"/>
@@ -3358,14 +3399,14 @@
     <row r="7" spans="1:13" ht="35.1" customHeight="1">
       <c r="A7" s="85"/>
       <c r="B7" s="80"/>
-      <c r="C7" s="60"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
       <c r="I7" s="95"/>
       <c r="J7" s="85"/>
       <c r="K7" s="94"/>
@@ -3400,30 +3441,30 @@
       <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="59"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
     </row>
     <row r="11" spans="1:13" ht="99.95" customHeight="1">
-      <c r="A11" s="60" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="60"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="60"/>
+      <c r="A11" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" s="59"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3478,15 +3519,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A1" s="71" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
+      <c r="A1" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" customHeight="1">
       <c r="A2" s="33"/>
@@ -3499,7 +3540,7 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -3510,10 +3551,10 @@
     </row>
     <row r="4" spans="1:13" ht="25.5" customHeight="1">
       <c r="A4" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="37" t="s">
         <v>74</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>75</v>
       </c>
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
@@ -3521,10 +3562,10 @@
       <c r="F4" s="37"/>
       <c r="G4" s="34"/>
       <c r="H4" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J4" s="34"/>
       <c r="K4" s="34"/>
@@ -3533,10 +3574,10 @@
     </row>
     <row r="5" spans="1:13" ht="25.5" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -3544,10 +3585,10 @@
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
       <c r="H5" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
@@ -3567,244 +3608,244 @@
     <row r="7" spans="1:13" ht="15.75" thickBot="1">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="72" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
+      <c r="C7" s="71" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="75" t="s">
-        <v>79</v>
-      </c>
-      <c r="G8" s="75"/>
+      <c r="G8" s="74"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="74" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" s="74"/>
+      <c r="C9" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="73"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1">
       <c r="A10" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="E10" s="26" t="s">
         <v>83</v>
-      </c>
-      <c r="E10" s="26" t="s">
-        <v>84</v>
       </c>
       <c r="F10" s="26" t="s">
         <v>39</v>
       </c>
       <c r="G10" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="51.75" thickBot="1">
       <c r="A11" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="27"/>
+      <c r="C11" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="27"/>
-      <c r="C11" s="62" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="63"/>
       <c r="F11" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="39" thickBot="1">
       <c r="A12" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="27"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="66"/>
-      <c r="E12" s="67"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="65"/>
+      <c r="E12" s="66"/>
       <c r="F12" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="26.25" thickBot="1">
       <c r="A13" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="27"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="67"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="66"/>
       <c r="F13" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" thickBot="1">
       <c r="A14" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="64.5" customHeight="1" thickBot="1">
+      <c r="A15" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G14" s="28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A15" s="61" t="s">
+      <c r="B15" s="27" t="s">
         <v>91</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>92</v>
       </c>
       <c r="C15" s="23"/>
       <c r="D15" s="23"/>
       <c r="E15" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G15" s="30" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="51.75" thickBot="1">
+      <c r="A16" s="60"/>
+      <c r="B16" s="27" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="51.75" thickBot="1">
-      <c r="A16" s="61"/>
-      <c r="B16" s="27" t="s">
-        <v>94</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="60" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A18" s="61"/>
+      <c r="A18" s="60"/>
       <c r="B18" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A19" s="61"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G19" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A20" s="61"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="39" thickBot="1">
-      <c r="A21" s="61" t="s">
-        <v>109</v>
+      <c r="A21" s="60" t="s">
+        <v>108</v>
       </c>
       <c r="B21" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="39" thickBot="1">
+      <c r="A22" s="60"/>
+      <c r="B22" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="E21" s="28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="39" thickBot="1">
-      <c r="A22" s="61"/>
-      <c r="B22" s="27" t="s">
+      <c r="E22" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="39" thickBot="1">
+      <c r="A23" s="60"/>
+      <c r="B23" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="39" thickBot="1">
-      <c r="A23" s="61"/>
-      <c r="B23" s="27" t="s">
-        <v>117</v>
-      </c>
       <c r="E23" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39" thickBot="1">
-      <c r="A24" s="61"/>
+      <c r="A24" s="60"/>
       <c r="B24" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E24" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3839,15 +3880,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A1" s="71" t="s">
-        <v>73</v>
-      </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
+      <c r="A1" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:12" ht="25.5" customHeight="1">
       <c r="A2" s="33"/>
@@ -3860,7 +3901,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="37" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -3871,10 +3912,10 @@
     </row>
     <row r="4" spans="1:12" ht="25.5" customHeight="1">
       <c r="A4" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="37" t="s">
         <v>74</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>75</v>
       </c>
       <c r="C4" s="37"/>
       <c r="D4" s="37"/>
@@ -3882,10 +3923,10 @@
       <c r="F4" s="37"/>
       <c r="G4" s="34"/>
       <c r="H4" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I4" s="37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J4" s="34"/>
       <c r="K4" s="34"/>
@@ -3893,10 +3934,10 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" customHeight="1">
       <c r="A5" s="25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -3904,10 +3945,10 @@
       <c r="F5" s="34"/>
       <c r="G5" s="34"/>
       <c r="H5" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J5" s="34"/>
       <c r="K5" s="34"/>
@@ -3934,273 +3975,273 @@
     <row r="8" spans="1:12" ht="15.75" thickBot="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="72" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
+      <c r="C8" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="72" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="G9" s="73"/>
+      <c r="G9" s="72"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
-      <c r="C10" s="74" t="s">
-        <v>80</v>
-      </c>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74" t="s">
-        <v>80</v>
-      </c>
-      <c r="G10" s="74"/>
+      <c r="C10" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="73"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="E11" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="26" t="s">
-        <v>84</v>
-      </c>
       <c r="F11" s="26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="51.75" thickBot="1">
       <c r="A12" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="62" t="s">
+      <c r="D12" s="62"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="28" t="s">
-        <v>87</v>
-      </c>
       <c r="G12" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="39" thickBot="1">
       <c r="A13" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B13" s="27"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="67"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="66"/>
       <c r="F13" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="26.25" thickBot="1">
       <c r="A14" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="27"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="67"/>
+      <c r="C14" s="64"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="66"/>
       <c r="F14" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1">
       <c r="A15" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="64.5" customHeight="1" thickBot="1">
+      <c r="A16" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G15" s="28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A16" s="61" t="s">
+      <c r="B16" s="27" t="s">
         <v>91</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>92</v>
       </c>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="26.25" thickBot="1">
-      <c r="A17" s="61"/>
+      <c r="A17" s="60"/>
       <c r="B17" s="27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
       <c r="E17" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="39" thickBot="1">
-      <c r="A18" s="61" t="s">
+      <c r="A18" s="60" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18" s="23"/>
       <c r="D18" s="23"/>
       <c r="E18" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F18" s="23"/>
-      <c r="G18" s="76" t="s">
-        <v>105</v>
+      <c r="G18" s="75" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="39" thickBot="1">
-      <c r="A19" s="61"/>
+      <c r="A19" s="60"/>
       <c r="B19" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C19" s="23"/>
       <c r="D19" s="23"/>
       <c r="E19" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F19" s="23"/>
-      <c r="G19" s="77"/>
+      <c r="G19" s="76"/>
     </row>
     <row r="20" spans="1:7" ht="39" thickBot="1">
-      <c r="A20" s="61"/>
+      <c r="A20" s="60"/>
       <c r="B20" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
       <c r="E20" s="28" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F20" s="23"/>
-      <c r="G20" s="77"/>
+      <c r="G20" s="76"/>
     </row>
     <row r="21" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A21" s="61"/>
+      <c r="A21" s="60"/>
       <c r="B21" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="76"/>
+    </row>
+    <row r="22" spans="1:7" ht="90" thickBot="1">
+      <c r="A22" s="60"/>
+      <c r="B22" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="E21" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" s="77"/>
-    </row>
-    <row r="22" spans="1:7" ht="90" thickBot="1">
-      <c r="A22" s="61"/>
-      <c r="B22" s="27" t="s">
+      <c r="E22" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="77"/>
+    </row>
+    <row r="23" spans="1:7" ht="39" thickBot="1">
+      <c r="A23" s="60" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="75" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="39" thickBot="1">
+      <c r="A24" s="60"/>
+      <c r="B24" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="76"/>
+    </row>
+    <row r="25" spans="1:7" ht="39" thickBot="1">
+      <c r="A25" s="60"/>
+      <c r="B25" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="76"/>
+    </row>
+    <row r="26" spans="1:7" ht="39" thickBot="1">
+      <c r="A26" s="60"/>
+      <c r="B26" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="E22" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G22" s="78"/>
-    </row>
-    <row r="23" spans="1:7" ht="39" thickBot="1">
-      <c r="A23" s="61" t="s">
-        <v>113</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="E23" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="76" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="39" thickBot="1">
-      <c r="A24" s="61"/>
-      <c r="B24" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G24" s="77"/>
-    </row>
-    <row r="25" spans="1:7" ht="39" thickBot="1">
-      <c r="A25" s="61"/>
-      <c r="B25" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E25" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="77"/>
-    </row>
-    <row r="26" spans="1:7" ht="39" thickBot="1">
-      <c r="A26" s="61"/>
-      <c r="B26" s="27" t="s">
-        <v>112</v>
-      </c>
       <c r="E26" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G26" s="77"/>
+        <v>86</v>
+      </c>
+      <c r="G26" s="76"/>
     </row>
     <row r="27" spans="1:7" ht="90" thickBot="1">
-      <c r="A27" s="61"/>
+      <c r="A27" s="60"/>
       <c r="B27" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="G27" s="78"/>
+        <v>86</v>
+      </c>
+      <c r="G27" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4229,8 +4270,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23:B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4238,8 +4279,8 @@
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
-    <col min="6" max="8" width="10.7109375" style="52" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="52" customWidth="1"/>
+    <col min="6" max="8" width="10.7109375" style="51" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" style="51" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4276,7 +4317,7 @@
         <v>40</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="36" customHeight="1">
@@ -4284,7 +4325,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C3" s="87" t="s">
         <v>51</v>
@@ -4293,13 +4334,13 @@
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="88" t="s">
-        <v>194</v>
-      </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="58" t="s">
-        <v>137</v>
+      <c r="F3" s="78" t="s">
+        <v>209</v>
+      </c>
+      <c r="G3" s="78"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="57" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36" customHeight="1">
@@ -4310,13 +4351,13 @@
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="88" t="s">
-        <v>195</v>
-      </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="58" t="s">
-        <v>136</v>
+      <c r="F4" s="78" t="s">
+        <v>210</v>
+      </c>
+      <c r="G4" s="78"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="57" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="36" customHeight="1">
@@ -4327,13 +4368,13 @@
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="88" t="s">
-        <v>196</v>
-      </c>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="58" t="s">
-        <v>130</v>
+      <c r="F5" s="78" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5" s="78"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="57" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1">
@@ -4344,13 +4385,13 @@
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="88" t="s">
-        <v>197</v>
-      </c>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="58" t="s">
-        <v>136</v>
+      <c r="F6" s="78" t="s">
+        <v>212</v>
+      </c>
+      <c r="G6" s="78"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="57" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36" customHeight="1">
@@ -4361,13 +4402,13 @@
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="88" t="s">
-        <v>198</v>
-      </c>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="58" t="s">
-        <v>130</v>
+      <c r="F7" s="78" t="s">
+        <v>213</v>
+      </c>
+      <c r="G7" s="78"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="57" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -4379,82 +4420,82 @@
     </row>
     <row r="9" spans="1:9" ht="36" customHeight="1">
       <c r="A9" s="85" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>190</v>
-      </c>
-      <c r="C9" s="60" t="s">
-        <v>121</v>
+        <v>189</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>120</v>
       </c>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="89" t="s">
-        <v>140</v>
-      </c>
-      <c r="G9" s="89" t="s">
-        <v>140</v>
-      </c>
-      <c r="H9" s="57" t="s">
-        <v>130</v>
+      <c r="F9" s="88" t="s">
+        <v>139</v>
+      </c>
+      <c r="G9" s="88" t="s">
+        <v>139</v>
+      </c>
+      <c r="H9" s="56" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="36" customHeight="1">
       <c r="A10" s="85"/>
       <c r="B10" s="86"/>
-      <c r="C10" s="60"/>
+      <c r="C10" s="59"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="48" t="s">
-        <v>130</v>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="47" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="36" customHeight="1">
       <c r="A11" s="85"/>
       <c r="B11" s="86"/>
-      <c r="C11" s="60"/>
+      <c r="C11" s="59"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="48" t="s">
-        <v>130</v>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="47" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="36" customHeight="1">
       <c r="A12" s="85"/>
       <c r="B12" s="86"/>
-      <c r="C12" s="60"/>
+      <c r="C12" s="59"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="89"/>
-      <c r="H12" s="48" t="s">
-        <v>130</v>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="47" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="36" customHeight="1">
       <c r="A13" s="85"/>
       <c r="B13" s="86"/>
-      <c r="C13" s="60"/>
+      <c r="C13" s="59"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="48" t="s">
-        <v>130</v>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="47" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -4463,16 +4504,16 @@
       <c r="C14" s="15"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
     </row>
     <row r="15" spans="1:9" ht="54" customHeight="1">
       <c r="A15" s="85" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="80" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C15" s="87" t="s">
         <v>55</v>
@@ -4482,12 +4523,12 @@
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="88" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G15" s="88"/>
       <c r="H15" s="88"/>
-      <c r="I15" s="91" t="s">
-        <v>130</v>
+      <c r="I15" s="89" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="54" customHeight="1">
@@ -4499,11 +4540,11 @@
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="88" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G16" s="88"/>
       <c r="H16" s="88"/>
-      <c r="I16" s="91"/>
+      <c r="I16" s="89"/>
     </row>
     <row r="17" spans="1:9" ht="54" customHeight="1">
       <c r="A17" s="85"/>
@@ -4514,11 +4555,11 @@
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="88" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G17" s="88"/>
       <c r="H17" s="88"/>
-      <c r="I17" s="91"/>
+      <c r="I17" s="89"/>
     </row>
     <row r="18" spans="1:9" ht="54" customHeight="1">
       <c r="A18" s="85"/>
@@ -4529,11 +4570,11 @@
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="88" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G18" s="88"/>
       <c r="H18" s="88"/>
-      <c r="I18" s="91"/>
+      <c r="I18" s="89"/>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1">
       <c r="A19" s="85"/>
@@ -4544,11 +4585,11 @@
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="88" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G19" s="88"/>
       <c r="H19" s="88"/>
-      <c r="I19" s="91"/>
+      <c r="I19" s="89"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2"/>
@@ -4564,26 +4605,26 @@
         <v>25</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="G21" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="H21" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="I21" s="44" t="s">
-        <v>136</v>
+      <c r="F21" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G21" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="I21" s="43" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -4600,8 +4641,8 @@
       <c r="A23" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="96" t="s">
-        <v>62</v>
+      <c r="B23" s="90" t="s">
+        <v>61</v>
       </c>
       <c r="C23" s="85" t="s">
         <v>57</v>
@@ -4612,14 +4653,14 @@
       <c r="E23" s="5"/>
       <c r="F23"/>
       <c r="G23"/>
-      <c r="H23" s="53" t="s">
-        <v>208</v>
+      <c r="H23" s="43" t="s">
+        <v>207</v>
       </c>
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9" ht="45">
       <c r="A24" s="85"/>
-      <c r="B24" s="96"/>
+      <c r="B24" s="90"/>
       <c r="C24" s="85"/>
       <c r="D24" s="5">
         <v>200437</v>
@@ -4627,14 +4668,14 @@
       <c r="E24" s="5"/>
       <c r="F24"/>
       <c r="G24"/>
-      <c r="H24" s="53" t="s">
-        <v>209</v>
+      <c r="H24" s="43" t="s">
+        <v>208</v>
       </c>
       <c r="I24"/>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" ht="45" customHeight="1">
       <c r="A25" s="85"/>
-      <c r="B25" s="96"/>
+      <c r="B25" s="90"/>
       <c r="C25" s="85"/>
       <c r="D25" s="5">
         <v>310111</v>
@@ -4642,12 +4683,14 @@
       <c r="E25" s="5"/>
       <c r="F25"/>
       <c r="G25"/>
-      <c r="H25"/>
+      <c r="H25" s="43" t="s">
+        <v>214</v>
+      </c>
       <c r="I25"/>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" ht="45" customHeight="1">
       <c r="A26" s="85"/>
-      <c r="B26" s="96"/>
+      <c r="B26" s="90"/>
       <c r="C26" s="85"/>
       <c r="D26" s="5">
         <v>528401</v>
@@ -4655,12 +4698,14 @@
       <c r="E26" s="5"/>
       <c r="F26"/>
       <c r="G26"/>
-      <c r="H26"/>
+      <c r="H26" s="78" t="s">
+        <v>214</v>
+      </c>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="85"/>
-      <c r="B27" s="96"/>
+      <c r="B27" s="90"/>
       <c r="C27" s="85"/>
       <c r="D27" s="5">
         <v>1076753</v>
@@ -4668,7 +4713,7 @@
       <c r="E27" s="5"/>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27"/>
+      <c r="H27" s="78"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
@@ -4689,7 +4734,7 @@
         <v>43</v>
       </c>
       <c r="C29" s="82" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D29" s="5">
         <v>145879</v>
@@ -4697,8 +4742,8 @@
       <c r="E29" s="5"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="48" t="s">
-        <v>164</v>
+      <c r="H29" s="47" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="54" customHeight="1">
@@ -4711,8 +4756,8 @@
       <c r="E30" s="5"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="48" t="s">
-        <v>165</v>
+      <c r="H30" s="47" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="54" customHeight="1">
@@ -4725,8 +4770,8 @@
       <c r="E31" s="5"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
-      <c r="H31" s="48" t="s">
-        <v>166</v>
+      <c r="H31" s="47" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="54" customHeight="1">
@@ -4739,8 +4784,8 @@
       <c r="E32" s="5"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
-      <c r="H32" s="48" t="s">
-        <v>167</v>
+      <c r="H32" s="47" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="54" customHeight="1">
@@ -4753,8 +4798,8 @@
       <c r="E33" s="5"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
-      <c r="H33" s="48" t="s">
-        <v>168</v>
+      <c r="H33" s="47" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -4773,7 +4818,7 @@
       </c>
       <c r="B35" s="80"/>
       <c r="C35" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>35</v>
@@ -4781,8 +4826,8 @@
       <c r="E35" s="5"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="48" t="s">
-        <v>131</v>
+      <c r="H35" s="47" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -4806,14 +4851,14 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" ht="94.5" customHeight="1">
-      <c r="A38" s="60" t="s">
-        <v>189</v>
-      </c>
-      <c r="B38" s="60"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
-      <c r="F38" s="60"/>
+      <c r="A38" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="59"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
@@ -4827,11 +4872,11 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="35">
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="C23:C27"/>
@@ -4846,11 +4891,12 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="F9:F13"/>
     <mergeCell ref="G9:G13"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H26:H27"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="B29:B35"/>
@@ -4905,7 +4951,7 @@
         <v>21</v>
       </c>
       <c r="F1" s="81" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G1" s="79"/>
       <c r="H1" s="79"/>
@@ -4913,7 +4959,7 @@
       <c r="J1" s="79"/>
       <c r="K1" s="79"/>
       <c r="M1" s="81" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="N1" s="79"/>
       <c r="O1" s="79"/>
@@ -4965,148 +5011,148 @@
     </row>
     <row r="3" spans="1:18" ht="68.25" customHeight="1">
       <c r="A3" s="85" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>121</v>
+        <v>189</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>120</v>
       </c>
       <c r="D3" s="10">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="G3" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="G3" s="44" t="s">
+      <c r="H3" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="H3" s="44" t="s">
+      <c r="I3" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="I3" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="J3" s="44" t="s">
-        <v>160</v>
-      </c>
-      <c r="K3" s="88" t="s">
-        <v>170</v>
-      </c>
-      <c r="M3" s="88" t="s">
+      <c r="J3" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="K3" s="91" t="s">
+        <v>169</v>
+      </c>
+      <c r="M3" s="91" t="s">
+        <v>178</v>
+      </c>
+      <c r="N3" s="91" t="s">
+        <v>176</v>
+      </c>
+      <c r="O3" s="91" t="s">
+        <v>177</v>
+      </c>
+      <c r="P3" s="91" t="s">
         <v>179</v>
       </c>
-      <c r="N3" s="88" t="s">
-        <v>177</v>
-      </c>
-      <c r="O3" s="88" t="s">
-        <v>178</v>
-      </c>
-      <c r="P3" s="88" t="s">
+      <c r="Q3" s="91" t="s">
         <v>180</v>
       </c>
-      <c r="Q3" s="88" t="s">
+      <c r="R3" s="91" t="s">
         <v>181</v>
-      </c>
-      <c r="R3" s="88" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
       <c r="A4" s="85"/>
       <c r="B4" s="86"/>
-      <c r="C4" s="60"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="88" t="s">
-        <v>163</v>
-      </c>
-      <c r="G4" s="88" t="s">
-        <v>174</v>
-      </c>
-      <c r="H4" s="88" t="s">
+      <c r="F4" s="91" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" s="91" t="s">
+        <v>173</v>
+      </c>
+      <c r="H4" s="91" t="s">
+        <v>170</v>
+      </c>
+      <c r="I4" s="91" t="s">
         <v>171</v>
       </c>
-      <c r="I4" s="88" t="s">
+      <c r="J4" s="91" t="s">
         <v>172</v>
       </c>
-      <c r="J4" s="88" t="s">
-        <v>173</v>
-      </c>
-      <c r="K4" s="88"/>
-      <c r="M4" s="88"/>
-      <c r="N4" s="88"/>
-      <c r="O4" s="88"/>
-      <c r="P4" s="88"/>
-      <c r="Q4" s="88"/>
-      <c r="R4" s="88"/>
+      <c r="K4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
+      <c r="O4" s="91"/>
+      <c r="P4" s="91"/>
+      <c r="Q4" s="91"/>
+      <c r="R4" s="91"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
       <c r="A5" s="85"/>
       <c r="B5" s="86"/>
-      <c r="C5" s="60"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-      <c r="M5" s="88"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
-      <c r="Q5" s="88"/>
-      <c r="R5" s="88"/>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
+      <c r="O5" s="91"/>
+      <c r="P5" s="91"/>
+      <c r="Q5" s="91"/>
+      <c r="R5" s="91"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
       <c r="A6" s="85"/>
       <c r="B6" s="86"/>
-      <c r="C6" s="60"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="88"/>
-      <c r="J6" s="88"/>
-      <c r="K6" s="88"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="88"/>
-      <c r="R6" s="88"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="91"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
       <c r="A7" s="85"/>
       <c r="B7" s="86"/>
-      <c r="C7" s="60"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="88"/>
-      <c r="J7" s="88"/>
-      <c r="K7" s="88"/>
-      <c r="M7" s="88"/>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="88"/>
+      <c r="F7" s="91"/>
+      <c r="G7" s="91"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="M7" s="91"/>
+      <c r="N7" s="91"/>
+      <c r="O7" s="91"/>
+      <c r="P7" s="91"/>
+      <c r="Q7" s="91"/>
+      <c r="R7" s="91"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2"/>
@@ -5121,7 +5167,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="80" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="87" t="s">
         <v>55</v>
@@ -5130,41 +5176,41 @@
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="89" t="s">
+      <c r="F9" s="88" t="s">
+        <v>145</v>
+      </c>
+      <c r="G9" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="G9" s="89" t="s">
+      <c r="H9" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="89" t="s">
-        <v>148</v>
-      </c>
-      <c r="I9" s="89" t="s">
+      <c r="I9" s="88" t="s">
+        <v>160</v>
+      </c>
+      <c r="J9" s="88" t="s">
         <v>161</v>
       </c>
-      <c r="J9" s="89" t="s">
-        <v>162</v>
-      </c>
-      <c r="K9" s="89" t="s">
-        <v>169</v>
-      </c>
-      <c r="M9" s="89" t="s">
+      <c r="K9" s="88" t="s">
+        <v>168</v>
+      </c>
+      <c r="M9" s="88" t="s">
+        <v>182</v>
+      </c>
+      <c r="N9" s="88" t="s">
         <v>183</v>
       </c>
-      <c r="N9" s="89" t="s">
+      <c r="O9" s="88" t="s">
         <v>184</v>
       </c>
-      <c r="O9" s="89" t="s">
+      <c r="P9" s="88" t="s">
         <v>185</v>
       </c>
-      <c r="P9" s="89" t="s">
+      <c r="Q9" s="88" t="s">
         <v>186</v>
       </c>
-      <c r="Q9" s="89" t="s">
+      <c r="R9" s="88" t="s">
         <v>187</v>
-      </c>
-      <c r="R9" s="89" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
@@ -5175,18 +5221,18 @@
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="89"/>
-      <c r="I10" s="89"/>
-      <c r="J10" s="89"/>
-      <c r="K10" s="89"/>
-      <c r="M10" s="89"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
-      <c r="P10" s="89"/>
-      <c r="Q10" s="89"/>
-      <c r="R10" s="89"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="88"/>
+      <c r="M10" s="88"/>
+      <c r="N10" s="88"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="88"/>
+      <c r="Q10" s="88"/>
+      <c r="R10" s="88"/>
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
       <c r="A11" s="85"/>
@@ -5196,18 +5242,18 @@
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="89"/>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="89"/>
-      <c r="M11" s="89"/>
-      <c r="N11" s="89"/>
-      <c r="O11" s="89"/>
-      <c r="P11" s="89"/>
-      <c r="Q11" s="89"/>
-      <c r="R11" s="89"/>
+      <c r="F11" s="88"/>
+      <c r="G11" s="88"/>
+      <c r="H11" s="88"/>
+      <c r="I11" s="88"/>
+      <c r="J11" s="88"/>
+      <c r="K11" s="88"/>
+      <c r="M11" s="88"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="88"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="88"/>
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
       <c r="A12" s="85"/>
@@ -5217,18 +5263,18 @@
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="89"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="89"/>
-      <c r="M12" s="89"/>
-      <c r="N12" s="89"/>
-      <c r="O12" s="89"/>
-      <c r="P12" s="89"/>
-      <c r="Q12" s="89"/>
-      <c r="R12" s="89"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="88"/>
+      <c r="H12" s="88"/>
+      <c r="I12" s="88"/>
+      <c r="J12" s="88"/>
+      <c r="K12" s="88"/>
+      <c r="M12" s="88"/>
+      <c r="N12" s="88"/>
+      <c r="O12" s="88"/>
+      <c r="P12" s="88"/>
+      <c r="Q12" s="88"/>
+      <c r="R12" s="88"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
       <c r="A13" s="85"/>
@@ -5238,18 +5284,18 @@
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="89"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="89"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
-      <c r="M13" s="89"/>
-      <c r="N13" s="89"/>
-      <c r="O13" s="89"/>
-      <c r="P13" s="89"/>
-      <c r="Q13" s="89"/>
-      <c r="R13" s="89"/>
+      <c r="F13" s="88"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="88"/>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="88"/>
+      <c r="M13" s="88"/>
+      <c r="N13" s="88"/>
+      <c r="O13" s="88"/>
+      <c r="P13" s="88"/>
+      <c r="Q13" s="88"/>
+      <c r="R13" s="88"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="5"/>
@@ -5262,14 +5308,14 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:18" ht="94.5" customHeight="1">
-      <c r="A15" s="60" t="s">
-        <v>189</v>
-      </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="60"/>
-      <c r="F15" s="60"/>
+      <c r="A15" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
@@ -5332,10 +5378,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5391,20 +5437,20 @@
         <v>10</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>199</v>
-      </c>
-      <c r="C3" s="60" t="s">
+        <v>198</v>
+      </c>
+      <c r="C3" s="59" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="90" t="s">
-        <v>203</v>
-      </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
+      <c r="F3" s="88" t="s">
+        <v>202</v>
+      </c>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
@@ -5412,16 +5458,16 @@
     <row r="4" spans="1:15" ht="45" customHeight="1">
       <c r="A4" s="85"/>
       <c r="B4" s="80"/>
-      <c r="C4" s="60"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="90" t="s">
-        <v>204</v>
-      </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
+      <c r="F4" s="88" t="s">
+        <v>203</v>
+      </c>
+      <c r="G4" s="88"/>
+      <c r="H4" s="88"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
@@ -5429,16 +5475,16 @@
     <row r="5" spans="1:15" ht="45" customHeight="1">
       <c r="A5" s="85"/>
       <c r="B5" s="80"/>
-      <c r="C5" s="60"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="90" t="s">
-        <v>205</v>
-      </c>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
+      <c r="F5" s="88" t="s">
+        <v>204</v>
+      </c>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
@@ -5446,16 +5492,16 @@
     <row r="6" spans="1:15" ht="45" customHeight="1">
       <c r="A6" s="85"/>
       <c r="B6" s="80"/>
-      <c r="C6" s="60"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="90" t="s">
-        <v>206</v>
-      </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90"/>
+      <c r="F6" s="88" t="s">
+        <v>205</v>
+      </c>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
@@ -5463,16 +5509,16 @@
     <row r="7" spans="1:15" ht="45" customHeight="1">
       <c r="A7" s="85"/>
       <c r="B7" s="80"/>
-      <c r="C7" s="60"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="90" t="s">
-        <v>207</v>
-      </c>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
+      <c r="F7" s="88" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
@@ -5494,8 +5540,8 @@
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="59" t="s">
-        <v>201</v>
+      <c r="B9" s="58" t="s">
+        <v>200</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>47</v>
@@ -5504,11 +5550,11 @@
         <v>35</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="90" t="s">
-        <v>200</v>
-      </c>
-      <c r="G9" s="90"/>
-      <c r="H9" s="90"/>
+      <c r="F9" s="88" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
@@ -5523,35 +5569,35 @@
       <c r="I10" s="2"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
-      <c r="O10" s="59"/>
+      <c r="O10" s="58"/>
     </row>
     <row r="11" spans="1:15" ht="30">
       <c r="A11" s="10" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="G11" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="H11" s="48" t="s">
-        <v>130</v>
+      <c r="F11" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G11" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>129</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
-      <c r="O11" s="59"/>
+      <c r="O11" s="58"/>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="10"/>
@@ -5565,145 +5611,191 @@
       <c r="I12" s="2"/>
       <c r="J12" s="4"/>
       <c r="K12" s="5"/>
-      <c r="O12" s="59"/>
-    </row>
-    <row r="13" spans="1:15" ht="75">
-      <c r="A13" s="10" t="s">
+      <c r="O12" s="58"/>
+    </row>
+    <row r="13" spans="1:15" ht="60" customHeight="1">
+      <c r="A13" s="85" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="56" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="80" t="s">
+        <v>220</v>
+      </c>
+      <c r="C13" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>35</v>
+      <c r="D13" s="2">
+        <v>145879</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="G13" s="42" t="s">
-        <v>136</v>
-      </c>
-      <c r="H13" s="48" t="s">
-        <v>130</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="O13" s="59"/>
-    </row>
-    <row r="14" spans="1:15">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="H13" s="42" t="s">
+        <v>215</v>
+      </c>
+      <c r="O13" s="58"/>
+    </row>
+    <row r="14" spans="1:15" ht="60" customHeight="1">
+      <c r="A14" s="85"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="2">
+        <v>200437</v>
+      </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-    </row>
-    <row r="15" spans="1:15" ht="270" customHeight="1">
-      <c r="A15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="80" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>35</v>
+      <c r="H14" s="42" t="s">
+        <v>216</v>
+      </c>
+      <c r="O14" s="58"/>
+    </row>
+    <row r="15" spans="1:15" ht="60" customHeight="1">
+      <c r="A15" s="85"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="2">
+        <v>310111</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-    </row>
-    <row r="16" spans="1:15" ht="30" customHeight="1">
-      <c r="A16" s="10"/>
+      <c r="H15" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="O15" s="58"/>
+    </row>
+    <row r="16" spans="1:15" ht="60" customHeight="1">
+      <c r="A16" s="85"/>
       <c r="B16" s="80"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="2">
+        <v>528401</v>
+      </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-    </row>
-    <row r="17" spans="1:11" ht="270" customHeight="1">
-      <c r="A17" s="10" t="s">
-        <v>32</v>
-      </c>
+      <c r="H16" s="42" t="s">
+        <v>218</v>
+      </c>
+      <c r="O16" s="58"/>
+    </row>
+    <row r="17" spans="1:15" ht="60" customHeight="1">
+      <c r="A17" s="85"/>
       <c r="B17" s="80"/>
-      <c r="C17" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>35</v>
+      <c r="C17" s="84"/>
+      <c r="D17" s="2">
+        <v>1076753</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="H17" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="I17" s="2"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="5"/>
-      <c r="B18" s="12"/>
+      <c r="H17" s="42" t="s">
+        <v>219</v>
+      </c>
+      <c r="O17" s="58"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="10"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
     </row>
-    <row r="19" spans="1:11" ht="75" customHeight="1">
-      <c r="A19" s="60" t="s">
-        <v>189</v>
-      </c>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
+    <row r="19" spans="1:15" ht="270" customHeight="1">
+      <c r="A19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="80" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="H19" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="I19" s="2"/>
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
+    <row r="20" spans="1:15" ht="30" customHeight="1">
+      <c r="A20" s="10"/>
+      <c r="B20" s="80"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:15" ht="270" customHeight="1">
+      <c r="A21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="80"/>
+      <c r="C21" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="H21" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="5"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" ht="75" customHeight="1">
+      <c r="A23" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="5" t="s">
+    <row r="25" spans="1:15">
+      <c r="A25" s="5" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A19:F19"/>
+  <mergeCells count="19">
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="A23:F23"/>
     <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B19:B21"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
@@ -5793,8 +5885,8 @@
       <c r="I2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="50" t="s">
-        <v>139</v>
+      <c r="J2" s="49" t="s">
+        <v>138</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>0</v>
@@ -5811,8 +5903,8 @@
       <c r="A3" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="56" t="s">
-        <v>191</v>
+      <c r="B3" s="55" t="s">
+        <v>190</v>
       </c>
       <c r="C3" s="83" t="s">
         <v>51</v>
@@ -5820,20 +5912,20 @@
       <c r="D3" s="10">
         <v>145879</v>
       </c>
-      <c r="E3" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="H3" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="I3" s="49" t="s">
-        <v>132</v>
+      <c r="E3" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="H3" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>131</v>
       </c>
       <c r="J3" s="41"/>
       <c r="K3" s="2" t="s">
@@ -5849,26 +5941,26 @@
     <row r="4" spans="1:14" ht="30" customHeight="1">
       <c r="A4" s="85"/>
       <c r="B4" s="80" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="92"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
-      <c r="E4" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F4" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="G4" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="H4" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="I4" s="49" t="s">
-        <v>130</v>
+      <c r="E4" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="H4" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="I4" s="48" t="s">
+        <v>129</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -5882,20 +5974,20 @@
       <c r="D5" s="10">
         <v>310111</v>
       </c>
-      <c r="E5" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="H5" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="I5" s="49" t="s">
-        <v>130</v>
+      <c r="E5" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="I5" s="48" t="s">
+        <v>129</v>
       </c>
       <c r="J5" s="41"/>
       <c r="K5" s="2"/>
@@ -5909,20 +6001,20 @@
       <c r="D6" s="10">
         <v>528401</v>
       </c>
-      <c r="E6" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F6" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="H6" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="I6" s="49" t="s">
-        <v>130</v>
+      <c r="E6" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" s="48" t="s">
+        <v>129</v>
       </c>
       <c r="J6" s="41"/>
       <c r="K6" s="2"/>
@@ -5936,20 +6028,20 @@
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
-      <c r="E7" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="F7" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="H7" s="46" t="s">
-        <v>132</v>
-      </c>
-      <c r="I7" s="49" t="s">
-        <v>132</v>
+      <c r="E7" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" s="48" t="s">
+        <v>131</v>
       </c>
       <c r="J7" s="41"/>
       <c r="K7" s="2"/>
@@ -5961,14 +6053,14 @@
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:14" ht="90" customHeight="1">
-      <c r="A9" s="60" t="s">
-        <v>189</v>
-      </c>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
+      <c r="A9" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -6090,8 +6182,8 @@
       <c r="A3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="54" t="s">
-        <v>190</v>
+      <c r="B3" s="53" t="s">
+        <v>189</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>50</v>
@@ -6099,23 +6191,23 @@
       <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="G3" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="I3" s="48" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" s="49" t="s">
-        <v>136</v>
+      <c r="E3" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="I3" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="48" t="s">
+        <v>135</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>2</v>
@@ -6143,30 +6235,30 @@
       <c r="M4" s="2"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
     </row>
     <row r="7" spans="1:14" ht="90" customHeight="1">
-      <c r="A7" s="60" t="s">
-        <v>189</v>
-      </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
+      <c r="A7" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="59"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -6205,8 +6297,8 @@
   </sheetPr>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6255,65 +6347,65 @@
         <v>10</v>
       </c>
       <c r="B3" s="80" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="60" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="59" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="48" t="s">
-        <v>136</v>
+      <c r="F3" s="47" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="36" customHeight="1">
       <c r="A4" s="85"/>
       <c r="B4" s="80"/>
-      <c r="C4" s="60"/>
+      <c r="C4" s="59"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="48" t="s">
-        <v>136</v>
+      <c r="F4" s="47" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="36" customHeight="1">
       <c r="A5" s="85"/>
       <c r="B5" s="80"/>
-      <c r="C5" s="60"/>
+      <c r="C5" s="59"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="48" t="s">
-        <v>136</v>
+      <c r="F5" s="47" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="36" customHeight="1">
       <c r="A6" s="85"/>
       <c r="B6" s="80"/>
-      <c r="C6" s="60"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="48" t="s">
-        <v>136</v>
+      <c r="F6" s="47" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="36" customHeight="1">
       <c r="A7" s="85"/>
       <c r="B7" s="80"/>
-      <c r="C7" s="60"/>
+      <c r="C7" s="59"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="48" t="s">
-        <v>136</v>
+      <c r="F7" s="47" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -6326,8 +6418,8 @@
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="54" t="s">
-        <v>193</v>
+      <c r="B9" s="53" t="s">
+        <v>192</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>49</v>
@@ -6336,7 +6428,7 @@
         <v>35</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="46" t="s">
         <v>22</v>
       </c>
       <c r="G9" s="2"/>
@@ -6361,19 +6453,19 @@
         <v>25</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>35</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="47" t="s">
+      <c r="F12" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="48" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6396,7 +6488,7 @@
         <v>26</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>56</v>
@@ -6405,10 +6497,10 @@
         <v>35</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="49" t="s">
+      <c r="G15" s="48" t="s">
         <v>23</v>
       </c>
     </row>
@@ -6428,14 +6520,14 @@
         <v>43</v>
       </c>
       <c r="C17" s="82" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D17" s="5">
         <v>145879</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="53" t="s">
-        <v>159</v>
+      <c r="F17" s="52" t="s">
+        <v>158</v>
       </c>
       <c r="N17" s="12"/>
     </row>
@@ -6447,8 +6539,8 @@
         <v>200437</v>
       </c>
       <c r="E18" s="5"/>
-      <c r="F18" s="53" t="s">
-        <v>155</v>
+      <c r="F18" s="52" t="s">
+        <v>154</v>
       </c>
       <c r="N18" s="12"/>
     </row>
@@ -6460,8 +6552,8 @@
         <v>310111</v>
       </c>
       <c r="E19" s="5"/>
-      <c r="F19" s="53" t="s">
-        <v>156</v>
+      <c r="F19" s="52" t="s">
+        <v>155</v>
       </c>
       <c r="N19" s="12"/>
     </row>
@@ -6473,8 +6565,8 @@
         <v>528401</v>
       </c>
       <c r="E20" s="5"/>
-      <c r="F20" s="53" t="s">
-        <v>157</v>
+      <c r="F20" s="52" t="s">
+        <v>156</v>
       </c>
       <c r="N20" s="12"/>
     </row>
@@ -6486,8 +6578,8 @@
         <v>1076753</v>
       </c>
       <c r="E21" s="5"/>
-      <c r="F21" s="53" t="s">
-        <v>158</v>
+      <c r="F21" s="52" t="s">
+        <v>157</v>
       </c>
       <c r="N21" s="12"/>
     </row>
@@ -6507,14 +6599,14 @@
         <v>43</v>
       </c>
       <c r="C23" s="82" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D23" s="5">
         <v>145879</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="44" t="s">
-        <v>151</v>
+      <c r="F23" s="43" t="s">
+        <v>150</v>
       </c>
       <c r="N23" s="12"/>
     </row>
@@ -6526,8 +6618,8 @@
         <v>200437</v>
       </c>
       <c r="E24" s="5"/>
-      <c r="F24" s="44" t="s">
-        <v>152</v>
+      <c r="F24" s="43" t="s">
+        <v>151</v>
       </c>
       <c r="N24" s="12"/>
     </row>
@@ -6539,8 +6631,8 @@
         <v>310111</v>
       </c>
       <c r="E25" s="5"/>
-      <c r="F25" s="44" t="s">
-        <v>153</v>
+      <c r="F25" s="43" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="54" customHeight="1">
@@ -6551,8 +6643,8 @@
         <v>528401</v>
       </c>
       <c r="E26" s="5"/>
-      <c r="F26" s="44" t="s">
-        <v>154</v>
+      <c r="F26" s="43" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="54" customHeight="1">
@@ -6563,8 +6655,8 @@
         <v>1076753</v>
       </c>
       <c r="E27" s="5"/>
-      <c r="F27" s="44" t="s">
-        <v>150</v>
+      <c r="F27" s="43" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -6577,15 +6669,15 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:14" ht="99.95" customHeight="1">
-      <c r="A29" s="60" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="60"/>
+      <c r="A29" s="59" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="59"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">

</xml_diff>

<commit_message>
Starts to re-run mSigHdp_ds_*k on SBS_set1/Realistic.
Previous results were from a legacy version of mSigHdp.
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF799D9-8BD5-464B-86FA-AC378EA08931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F658FFD-99F0-4485-9071-E82A19926DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="1005" windowWidth="15375" windowHeight="12855" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2010" yWindow="1005" windowWidth="15375" windowHeight="12855" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="222">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -1228,11 +1228,6 @@
 hdpx = 1.0.5</t>
   </si>
   <si>
-    <t>mSigHdp = 2.0.1 (v2.0.1-branch, 2022-May-12);
-hdpx = 1.0.1 (v1.0.1-branch, 2022-May-12)
-Needs rerun</t>
-  </si>
-  <si>
     <t>4) Bolded red text indicates the run needs to be re-executed.</t>
   </si>
   <si>
@@ -1369,6 +1364,16 @@
 NMF = 0.24.0;
 Wrapper function SynSigRun::RunsigneR(), SynSigRun = 1.0.0
 (Version for rerun)</t>
+  </si>
+  <si>
+    <t>mSigHdp = 2.1.0;
+hdpx = 1.0.5
+(Version used in rerun)</t>
+  </si>
+  <si>
+    <t>HPC
+&lt;115386&gt;
+(wuyang)</t>
   </si>
 </sst>
 </file>
@@ -1714,7 +1719,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1875,12 +1880,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2482,10 +2481,10 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="59"/>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
+      <c r="A10" s="57"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
@@ -2531,23 +2530,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" customHeight="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="79" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="81"/>
+      <c r="G1" s="79"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -2556,10 +2555,10 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" customHeight="1">
-      <c r="A2" s="79"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
       <c r="E2" s="1"/>
       <c r="F2" s="8" t="s">
         <v>40</v>
@@ -2613,7 +2612,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="53" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>48</v>
@@ -2714,7 +2713,7 @@
       <c r="A11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="78" t="s">
         <v>43</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -2735,7 +2734,7 @@
     </row>
     <row r="12" spans="1:13" ht="30">
       <c r="A12" s="5"/>
-      <c r="B12" s="80"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -2751,18 +2750,18 @@
       <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="54" customHeight="1">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="93" t="s">
+      <c r="B13" s="78"/>
+      <c r="C13" s="91" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="5">
         <v>145879</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="88" t="s">
+      <c r="F13" s="86" t="s">
         <v>122</v>
       </c>
       <c r="G13" s="43" t="s">
@@ -2774,14 +2773,14 @@
       <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="54" customHeight="1">
-      <c r="A14" s="85"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="93"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="91"/>
       <c r="D14" s="5">
         <v>200437</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="88"/>
+      <c r="F14" s="86"/>
       <c r="G14" s="43" t="s">
         <v>127</v>
       </c>
@@ -2791,14 +2790,14 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="54" customHeight="1">
-      <c r="A15" s="85"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="93"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="91"/>
       <c r="D15" s="5">
         <v>310111</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="88"/>
+      <c r="F15" s="86"/>
       <c r="G15" s="44" t="s">
         <v>132</v>
       </c>
@@ -2808,14 +2807,14 @@
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="54" customHeight="1">
-      <c r="A16" s="85"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="93"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="91"/>
       <c r="D16" s="5">
         <v>528401</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="88"/>
+      <c r="F16" s="86"/>
       <c r="G16" s="44" t="s">
         <v>132</v>
       </c>
@@ -2825,14 +2824,14 @@
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" ht="54" customHeight="1">
-      <c r="A17" s="85"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="93"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="91"/>
       <c r="D17" s="5">
         <v>1076753</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="88"/>
+      <c r="F17" s="86"/>
       <c r="G17" s="44" t="s">
         <v>132</v>
       </c>
@@ -2872,15 +2871,15 @@
       <c r="M19" s="5"/>
     </row>
     <row r="20" spans="1:13" ht="105" customHeight="1">
-      <c r="A20" s="59" t="s">
+      <c r="A20" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="59"/>
-      <c r="C20" s="59"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
+      <c r="B20" s="57"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
@@ -2941,13 +2940,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
       <c r="J1" s="10"/>
       <c r="K1" s="11"/>
       <c r="L1" s="10"/>
@@ -2991,13 +2990,13 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="57" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="2">
@@ -3015,23 +3014,23 @@
       <c r="H3" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="I3" s="89" t="s">
+      <c r="I3" s="87" t="s">
         <v>125</v>
       </c>
-      <c r="J3" s="85" t="s">
+      <c r="J3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="94" t="s">
+      <c r="K3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="85" t="s">
+      <c r="L3" s="83" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A4" s="85"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="59"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
@@ -3044,15 +3043,15 @@
       <c r="G4" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="89"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="85"/>
+      <c r="I4" s="87"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="83"/>
     </row>
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A5" s="85"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="59"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
@@ -3065,15 +3064,15 @@
       <c r="G5" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I5" s="89"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="85"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="83"/>
     </row>
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="59"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
@@ -3086,15 +3085,15 @@
       <c r="G6" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I6" s="89"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="85"/>
+      <c r="I6" s="87"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="83"/>
     </row>
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A7" s="85"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="59"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
@@ -3107,10 +3106,10 @@
       <c r="G7" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I7" s="89"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="85"/>
+      <c r="I7" s="87"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="83"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -3127,30 +3126,30 @@
       <c r="L8" s="2"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
     </row>
     <row r="11" spans="1:12" ht="75" customHeight="1">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3193,12 +3192,12 @@
       <c r="F18" s="5"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="59"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="59"/>
-      <c r="F19" s="59"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="5"/>
@@ -3260,13 +3259,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -3311,106 +3310,106 @@
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="57" t="s">
         <v>52</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="88" t="s">
+      <c r="G3" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="88" t="s">
+      <c r="H3" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="I3" s="95" t="s">
+      <c r="I3" s="93" t="s">
         <v>127</v>
       </c>
-      <c r="J3" s="85" t="s">
+      <c r="J3" s="83" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="94" t="s">
+      <c r="K3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="85" t="s">
+      <c r="L3" s="83" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A4" s="85"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="59"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="85"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="85"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="93"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="83"/>
     </row>
     <row r="5" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A5" s="85"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="59"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="85"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="93"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="83"/>
     </row>
     <row r="6" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="59"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="88"/>
-      <c r="F6" s="88"/>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="85"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="83"/>
     </row>
     <row r="7" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A7" s="85"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="59"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="85"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="83"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="10"/>
@@ -3441,30 +3440,30 @@
       <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="59"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="59"/>
-      <c r="G10" s="59"/>
-      <c r="H10" s="59"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="59"/>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="57"/>
+      <c r="K10" s="57"/>
     </row>
     <row r="11" spans="1:13" ht="99.95" customHeight="1">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -3519,15 +3518,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="25.5" customHeight="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" customHeight="1">
       <c r="A2" s="33"/>
@@ -3608,39 +3607,39 @@
     <row r="7" spans="1:13" ht="15.75" thickBot="1">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="74" t="s">
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="74"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="73" t="s">
+      <c r="C9" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73" t="s">
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="73"/>
+      <c r="G9" s="71"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1">
       <c r="A10" s="27" t="s">
@@ -3668,11 +3667,11 @@
         <v>84</v>
       </c>
       <c r="B11" s="27"/>
-      <c r="C11" s="61" t="s">
+      <c r="C11" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D11" s="62"/>
-      <c r="E11" s="63"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="61"/>
       <c r="F11" s="30" t="s">
         <v>92</v>
       </c>
@@ -3685,9 +3684,9 @@
         <v>87</v>
       </c>
       <c r="B12" s="27"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="66"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="64"/>
       <c r="F12" s="28" t="s">
         <v>86</v>
       </c>
@@ -3700,9 +3699,9 @@
         <v>88</v>
       </c>
       <c r="B13" s="27"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="66"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
       <c r="F13" s="28" t="s">
         <v>86</v>
       </c>
@@ -3715,9 +3714,9 @@
         <v>89</v>
       </c>
       <c r="B14" s="27"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="69"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="28" t="s">
         <v>86</v>
       </c>
@@ -3726,7 +3725,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="58" t="s">
         <v>90</v>
       </c>
       <c r="B15" s="27" t="s">
@@ -3742,7 +3741,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="51.75" thickBot="1">
-      <c r="A16" s="60"/>
+      <c r="A16" s="58"/>
       <c r="B16" s="27" t="s">
         <v>93</v>
       </c>
@@ -3756,7 +3755,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A17" s="60" t="s">
+      <c r="A17" s="58" t="s">
         <v>10</v>
       </c>
       <c r="B17" s="27" t="s">
@@ -3772,7 +3771,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A18" s="60"/>
+      <c r="A18" s="58"/>
       <c r="B18" s="27" t="s">
         <v>106</v>
       </c>
@@ -3786,7 +3785,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A19" s="60"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="27" t="s">
         <v>107</v>
       </c>
@@ -3800,7 +3799,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A20" s="60"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="27" t="s">
         <v>111</v>
       </c>
@@ -3811,7 +3810,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="39" thickBot="1">
-      <c r="A21" s="60" t="s">
+      <c r="A21" s="58" t="s">
         <v>108</v>
       </c>
       <c r="B21" s="27" t="s">
@@ -3822,7 +3821,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="39" thickBot="1">
-      <c r="A22" s="60"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="27" t="s">
         <v>115</v>
       </c>
@@ -3831,7 +3830,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="39" thickBot="1">
-      <c r="A23" s="60"/>
+      <c r="A23" s="58"/>
       <c r="B23" s="27" t="s">
         <v>116</v>
       </c>
@@ -3840,7 +3839,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="39" thickBot="1">
-      <c r="A24" s="60"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="27" t="s">
         <v>111</v>
       </c>
@@ -3880,15 +3879,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.5" customHeight="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:12" ht="25.5" customHeight="1">
       <c r="A2" s="33"/>
@@ -3975,39 +3974,39 @@
     <row r="8" spans="1:12" ht="15.75" thickBot="1">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
-      <c r="C8" s="71" t="s">
+      <c r="C8" s="69" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="70" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72" t="s">
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="72"/>
+      <c r="G9" s="70"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
-      <c r="C10" s="73" t="s">
+      <c r="C10" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73" t="s">
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" thickBot="1">
       <c r="A11" s="23"/>
@@ -4033,11 +4032,11 @@
         <v>84</v>
       </c>
       <c r="B12" s="27"/>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="63"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="28" t="s">
         <v>86</v>
       </c>
@@ -4050,9 +4049,9 @@
         <v>87</v>
       </c>
       <c r="B13" s="27"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="66"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
       <c r="F13" s="28" t="s">
         <v>86</v>
       </c>
@@ -4065,9 +4064,9 @@
         <v>88</v>
       </c>
       <c r="B14" s="27"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="66"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="64"/>
       <c r="F14" s="28" t="s">
         <v>86</v>
       </c>
@@ -4080,9 +4079,9 @@
         <v>89</v>
       </c>
       <c r="B15" s="27"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="69"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="28" t="s">
         <v>86</v>
       </c>
@@ -4091,7 +4090,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A16" s="60" t="s">
+      <c r="A16" s="58" t="s">
         <v>90</v>
       </c>
       <c r="B16" s="27" t="s">
@@ -4110,7 +4109,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="26.25" thickBot="1">
-      <c r="A17" s="60"/>
+      <c r="A17" s="58"/>
       <c r="B17" s="27" t="s">
         <v>96</v>
       </c>
@@ -4127,7 +4126,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="39" thickBot="1">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="58" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="27" t="s">
@@ -4139,12 +4138,12 @@
         <v>86</v>
       </c>
       <c r="F18" s="23"/>
-      <c r="G18" s="75" t="s">
+      <c r="G18" s="73" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="39" thickBot="1">
-      <c r="A19" s="60"/>
+      <c r="A19" s="58"/>
       <c r="B19" s="27" t="s">
         <v>106</v>
       </c>
@@ -4154,10 +4153,10 @@
         <v>86</v>
       </c>
       <c r="F19" s="23"/>
-      <c r="G19" s="76"/>
+      <c r="G19" s="74"/>
     </row>
     <row r="20" spans="1:7" ht="39" thickBot="1">
-      <c r="A20" s="60"/>
+      <c r="A20" s="58"/>
       <c r="B20" s="27" t="s">
         <v>107</v>
       </c>
@@ -4167,30 +4166,30 @@
         <v>86</v>
       </c>
       <c r="F20" s="23"/>
-      <c r="G20" s="76"/>
+      <c r="G20" s="74"/>
     </row>
     <row r="21" spans="1:7" ht="51.75" customHeight="1" thickBot="1">
-      <c r="A21" s="60"/>
+      <c r="A21" s="58"/>
       <c r="B21" s="27" t="s">
         <v>109</v>
       </c>
       <c r="E21" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G21" s="76"/>
+      <c r="G21" s="74"/>
     </row>
     <row r="22" spans="1:7" ht="90" thickBot="1">
-      <c r="A22" s="60"/>
+      <c r="A22" s="58"/>
       <c r="B22" s="27" t="s">
         <v>110</v>
       </c>
       <c r="E22" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G22" s="77"/>
+      <c r="G22" s="75"/>
     </row>
     <row r="23" spans="1:7" ht="39" thickBot="1">
-      <c r="A23" s="60" t="s">
+      <c r="A23" s="58" t="s">
         <v>112</v>
       </c>
       <c r="B23" s="27" t="s">
@@ -4199,49 +4198,49 @@
       <c r="E23" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="75" t="s">
+      <c r="G23" s="73" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="39" thickBot="1">
-      <c r="A24" s="60"/>
+      <c r="A24" s="58"/>
       <c r="B24" s="27" t="s">
         <v>115</v>
       </c>
       <c r="E24" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G24" s="76"/>
+      <c r="G24" s="74"/>
     </row>
     <row r="25" spans="1:7" ht="39" thickBot="1">
-      <c r="A25" s="60"/>
+      <c r="A25" s="58"/>
       <c r="B25" s="27" t="s">
         <v>116</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G25" s="76"/>
+      <c r="G25" s="74"/>
     </row>
     <row r="26" spans="1:7" ht="39" thickBot="1">
-      <c r="A26" s="60"/>
+      <c r="A26" s="58"/>
       <c r="B26" s="27" t="s">
         <v>111</v>
       </c>
       <c r="E26" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G26" s="76"/>
+      <c r="G26" s="74"/>
     </row>
     <row r="27" spans="1:7" ht="90" thickBot="1">
-      <c r="A27" s="60"/>
+      <c r="A27" s="58"/>
       <c r="B27" s="27" t="s">
         <v>110</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="G27" s="77"/>
+      <c r="G27" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -4270,8 +4269,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:B27"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4284,29 +4283,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="79"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="81"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="79"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
       </c>
@@ -4321,93 +4320,93 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="36" customHeight="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="80" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="87" t="s">
+      <c r="B3" s="78" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="85" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="78" t="s">
-        <v>209</v>
-      </c>
-      <c r="G3" s="78"/>
+      <c r="F3" s="76" t="s">
+        <v>208</v>
+      </c>
+      <c r="G3" s="76"/>
       <c r="H3" s="42"/>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="55" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36" customHeight="1">
-      <c r="A4" s="85"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="87"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="85"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="78" t="s">
-        <v>210</v>
-      </c>
-      <c r="G4" s="78"/>
+      <c r="F4" s="76" t="s">
+        <v>209</v>
+      </c>
+      <c r="G4" s="76"/>
       <c r="H4" s="42"/>
-      <c r="I4" s="57" t="s">
+      <c r="I4" s="55" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="36" customHeight="1">
-      <c r="A5" s="85"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="87"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="78" t="s">
-        <v>211</v>
-      </c>
-      <c r="G5" s="78"/>
+      <c r="F5" s="76" t="s">
+        <v>210</v>
+      </c>
+      <c r="G5" s="76"/>
       <c r="H5" s="42"/>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="55" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="87"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="78" t="s">
-        <v>212</v>
-      </c>
-      <c r="G6" s="78"/>
+      <c r="F6" s="76" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" s="76"/>
       <c r="H6" s="42"/>
-      <c r="I6" s="57" t="s">
+      <c r="I6" s="55" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36" customHeight="1">
-      <c r="A7" s="85"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="87"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="78" t="s">
-        <v>213</v>
-      </c>
-      <c r="G7" s="78"/>
+      <c r="F7" s="76" t="s">
+        <v>212</v>
+      </c>
+      <c r="G7" s="76"/>
       <c r="H7" s="42"/>
-      <c r="I7" s="57" t="s">
+      <c r="I7" s="55" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4418,82 +4417,82 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="36" customHeight="1">
-      <c r="A9" s="85" t="s">
+    <row r="9" spans="1:9" ht="45">
+      <c r="A9" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="57" t="s">
         <v>120</v>
       </c>
       <c r="D9" s="2">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="88" t="s">
+      <c r="F9" s="86" t="s">
         <v>139</v>
       </c>
-      <c r="G9" s="88" t="s">
+      <c r="G9" s="86" t="s">
         <v>139</v>
       </c>
-      <c r="H9" s="56" t="s">
-        <v>129</v>
+      <c r="H9" s="52" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="36" customHeight="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="59"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
       <c r="H10" s="47" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="36" customHeight="1">
-      <c r="A11" s="85"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="59"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
       <c r="H11" s="47" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="36" customHeight="1">
-      <c r="A12" s="85"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="59"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="57"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
       <c r="H12" s="47" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="36" customHeight="1">
-      <c r="A13" s="85"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="59"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="57"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
       <c r="H13" s="47" t="s">
         <v>129</v>
       </c>
@@ -4509,87 +4508,87 @@
       <c r="H14" s="50"/>
     </row>
     <row r="15" spans="1:9" ht="54" customHeight="1">
-      <c r="A15" s="85" t="s">
+      <c r="A15" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="80" t="s">
-        <v>201</v>
-      </c>
-      <c r="C15" s="87" t="s">
+      <c r="B15" s="78" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" s="85" t="s">
         <v>55</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="88" t="s">
-        <v>193</v>
-      </c>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="89" t="s">
+      <c r="F15" s="86" t="s">
+        <v>192</v>
+      </c>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="87" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="54" customHeight="1">
-      <c r="A16" s="85"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="87"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="85"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="88" t="s">
-        <v>194</v>
-      </c>
-      <c r="G16" s="88"/>
-      <c r="H16" s="88"/>
-      <c r="I16" s="89"/>
+      <c r="F16" s="86" t="s">
+        <v>193</v>
+      </c>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="87"/>
     </row>
     <row r="17" spans="1:9" ht="54" customHeight="1">
-      <c r="A17" s="85"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="87"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="85"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="88" t="s">
-        <v>195</v>
-      </c>
-      <c r="G17" s="88"/>
-      <c r="H17" s="88"/>
-      <c r="I17" s="89"/>
+      <c r="F17" s="86" t="s">
+        <v>194</v>
+      </c>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="87"/>
     </row>
     <row r="18" spans="1:9" ht="54" customHeight="1">
-      <c r="A18" s="85"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="87"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="85"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="88" t="s">
-        <v>196</v>
-      </c>
-      <c r="G18" s="88"/>
-      <c r="H18" s="88"/>
-      <c r="I18" s="89"/>
+      <c r="F18" s="86" t="s">
+        <v>195</v>
+      </c>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="87"/>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1">
-      <c r="A19" s="85"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="87"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="85"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="88" t="s">
-        <v>197</v>
-      </c>
-      <c r="G19" s="88"/>
-      <c r="H19" s="88"/>
-      <c r="I19" s="89"/>
+      <c r="F19" s="86" t="s">
+        <v>196</v>
+      </c>
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="87"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2"/>
@@ -4638,13 +4637,13 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="45">
-      <c r="A23" s="85" t="s">
+      <c r="A23" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="90" t="s">
+      <c r="B23" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="85" t="s">
+      <c r="C23" s="83" t="s">
         <v>57</v>
       </c>
       <c r="D23" s="5">
@@ -4654,14 +4653,14 @@
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23" s="43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9" ht="45">
-      <c r="A24" s="85"/>
-      <c r="B24" s="90"/>
-      <c r="C24" s="85"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="83"/>
       <c r="D24" s="5">
         <v>200437</v>
       </c>
@@ -4669,14 +4668,14 @@
       <c r="F24"/>
       <c r="G24"/>
       <c r="H24" s="43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9" ht="45" customHeight="1">
-      <c r="A25" s="85"/>
-      <c r="B25" s="90"/>
-      <c r="C25" s="85"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="83"/>
       <c r="D25" s="5">
         <v>310111</v>
       </c>
@@ -4684,36 +4683,36 @@
       <c r="F25"/>
       <c r="G25"/>
       <c r="H25" s="43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I25"/>
     </row>
     <row r="26" spans="1:9" ht="45" customHeight="1">
-      <c r="A26" s="85"/>
-      <c r="B26" s="90"/>
-      <c r="C26" s="85"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="5">
         <v>528401</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26"/>
       <c r="G26"/>
-      <c r="H26" s="78" t="s">
-        <v>214</v>
+      <c r="H26" s="76" t="s">
+        <v>213</v>
       </c>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="85"/>
-      <c r="B27" s="90"/>
-      <c r="C27" s="85"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="83"/>
       <c r="D27" s="5">
         <v>1076753</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27" s="78"/>
+      <c r="H27" s="76"/>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
@@ -4727,13 +4726,13 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:9" ht="54" customHeight="1">
-      <c r="A29" s="84" t="s">
+      <c r="A29" s="82" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="80" t="s">
+      <c r="B29" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="82" t="s">
+      <c r="C29" s="80" t="s">
         <v>67</v>
       </c>
       <c r="D29" s="5">
@@ -4747,9 +4746,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="54" customHeight="1">
-      <c r="A30" s="84"/>
-      <c r="B30" s="80"/>
-      <c r="C30" s="83"/>
+      <c r="A30" s="82"/>
+      <c r="B30" s="78"/>
+      <c r="C30" s="81"/>
       <c r="D30" s="5">
         <v>200437</v>
       </c>
@@ -4761,9 +4760,9 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="54" customHeight="1">
-      <c r="A31" s="84"/>
-      <c r="B31" s="80"/>
-      <c r="C31" s="83"/>
+      <c r="A31" s="82"/>
+      <c r="B31" s="78"/>
+      <c r="C31" s="81"/>
       <c r="D31" s="5">
         <v>310111</v>
       </c>
@@ -4775,9 +4774,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="54" customHeight="1">
-      <c r="A32" s="84"/>
-      <c r="B32" s="80"/>
-      <c r="C32" s="83"/>
+      <c r="A32" s="82"/>
+      <c r="B32" s="78"/>
+      <c r="C32" s="81"/>
       <c r="D32" s="5">
         <v>528401</v>
       </c>
@@ -4789,9 +4788,9 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="54" customHeight="1">
-      <c r="A33" s="84"/>
-      <c r="B33" s="80"/>
-      <c r="C33" s="83"/>
+      <c r="A33" s="82"/>
+      <c r="B33" s="78"/>
+      <c r="C33" s="81"/>
       <c r="D33" s="5">
         <v>1076753</v>
       </c>
@@ -4804,7 +4803,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" s="5"/>
-      <c r="B34" s="80"/>
+      <c r="B34" s="78"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
@@ -4816,7 +4815,7 @@
       <c r="A35" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="80"/>
+      <c r="B35" s="78"/>
       <c r="C35" s="19" t="s">
         <v>119</v>
       </c>
@@ -4851,14 +4850,14 @@
       <c r="H37" s="10"/>
     </row>
     <row r="38" spans="1:8" ht="94.5" customHeight="1">
-      <c r="A38" s="59" t="s">
+      <c r="A38" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="B38" s="59"/>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="57"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
@@ -4872,7 +4871,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -4938,40 +4937,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="50.1" customHeight="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="79" t="s">
         <v>174</v>
       </c>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="M1" s="81" t="s">
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="M1" s="79" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="79"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="81"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="79"/>
       <c r="F2" s="9">
         <v>5</v>
       </c>
@@ -5010,13 +5009,13 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="68.25" customHeight="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="57" t="s">
         <v>120</v>
       </c>
       <c r="D3" s="10">
@@ -5038,121 +5037,121 @@
       <c r="J3" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="K3" s="91" t="s">
+      <c r="K3" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="M3" s="91" t="s">
+      <c r="M3" s="89" t="s">
         <v>178</v>
       </c>
-      <c r="N3" s="91" t="s">
+      <c r="N3" s="89" t="s">
         <v>176</v>
       </c>
-      <c r="O3" s="91" t="s">
+      <c r="O3" s="89" t="s">
         <v>177</v>
       </c>
-      <c r="P3" s="91" t="s">
+      <c r="P3" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="Q3" s="91" t="s">
+      <c r="Q3" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="R3" s="91" t="s">
+      <c r="R3" s="89" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
-      <c r="A4" s="85"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="59"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="84"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="89" t="s">
         <v>162</v>
       </c>
-      <c r="G4" s="91" t="s">
+      <c r="G4" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="89" t="s">
         <v>170</v>
       </c>
-      <c r="I4" s="91" t="s">
+      <c r="I4" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="J4" s="91" t="s">
+      <c r="J4" s="89" t="s">
         <v>172</v>
       </c>
-      <c r="K4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
-      <c r="O4" s="91"/>
-      <c r="P4" s="91"/>
-      <c r="Q4" s="91"/>
-      <c r="R4" s="91"/>
+      <c r="K4" s="89"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="89"/>
+      <c r="O4" s="89"/>
+      <c r="P4" s="89"/>
+      <c r="Q4" s="89"/>
+      <c r="R4" s="89"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
-      <c r="A5" s="85"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="59"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
-      <c r="K5" s="91"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="91"/>
-      <c r="Q5" s="91"/>
-      <c r="R5" s="91"/>
+      <c r="F5" s="89"/>
+      <c r="G5" s="89"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="89"/>
+      <c r="O5" s="89"/>
+      <c r="P5" s="89"/>
+      <c r="Q5" s="89"/>
+      <c r="R5" s="89"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="59"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="91"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="91"/>
+      <c r="F6" s="89"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="89"/>
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
+      <c r="P6" s="89"/>
+      <c r="Q6" s="89"/>
+      <c r="R6" s="89"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
-      <c r="A7" s="85"/>
-      <c r="B7" s="86"/>
-      <c r="C7" s="59"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="91"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="91"/>
-      <c r="I7" s="91"/>
-      <c r="J7" s="91"/>
-      <c r="K7" s="91"/>
-      <c r="M7" s="91"/>
-      <c r="N7" s="91"/>
-      <c r="O7" s="91"/>
-      <c r="P7" s="91"/>
-      <c r="Q7" s="91"/>
-      <c r="R7" s="91"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="89"/>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+      <c r="M7" s="89"/>
+      <c r="N7" s="89"/>
+      <c r="O7" s="89"/>
+      <c r="P7" s="89"/>
+      <c r="Q7" s="89"/>
+      <c r="R7" s="89"/>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" s="2"/>
@@ -5163,139 +5162,139 @@
       <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:18" ht="54" customHeight="1">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="80" t="s">
+      <c r="B9" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="87" t="s">
+      <c r="C9" s="85" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="10">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="88" t="s">
+      <c r="F9" s="86" t="s">
         <v>145</v>
       </c>
-      <c r="G9" s="88" t="s">
+      <c r="G9" s="86" t="s">
         <v>146</v>
       </c>
-      <c r="H9" s="88" t="s">
+      <c r="H9" s="86" t="s">
         <v>147</v>
       </c>
-      <c r="I9" s="88" t="s">
+      <c r="I9" s="86" t="s">
         <v>160</v>
       </c>
-      <c r="J9" s="88" t="s">
+      <c r="J9" s="86" t="s">
         <v>161</v>
       </c>
-      <c r="K9" s="88" t="s">
+      <c r="K9" s="86" t="s">
         <v>168</v>
       </c>
-      <c r="M9" s="88" t="s">
+      <c r="M9" s="86" t="s">
         <v>182</v>
       </c>
-      <c r="N9" s="88" t="s">
+      <c r="N9" s="86" t="s">
         <v>183</v>
       </c>
-      <c r="O9" s="88" t="s">
+      <c r="O9" s="86" t="s">
         <v>184</v>
       </c>
-      <c r="P9" s="88" t="s">
+      <c r="P9" s="86" t="s">
         <v>185</v>
       </c>
-      <c r="Q9" s="88" t="s">
+      <c r="Q9" s="86" t="s">
         <v>186</v>
       </c>
-      <c r="R9" s="88" t="s">
+      <c r="R9" s="86" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="86"/>
-      <c r="C10" s="87"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="10">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
-      <c r="K10" s="88"/>
-      <c r="M10" s="88"/>
-      <c r="N10" s="88"/>
-      <c r="O10" s="88"/>
-      <c r="P10" s="88"/>
-      <c r="Q10" s="88"/>
-      <c r="R10" s="88"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="86"/>
+      <c r="M10" s="86"/>
+      <c r="N10" s="86"/>
+      <c r="O10" s="86"/>
+      <c r="P10" s="86"/>
+      <c r="Q10" s="86"/>
+      <c r="R10" s="86"/>
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
-      <c r="A11" s="85"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="87"/>
+      <c r="A11" s="83"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="85"/>
       <c r="D11" s="10">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
-      <c r="K11" s="88"/>
-      <c r="M11" s="88"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="88"/>
-      <c r="Q11" s="88"/>
-      <c r="R11" s="88"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="M11" s="86"/>
+      <c r="N11" s="86"/>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
-      <c r="A12" s="85"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="87"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="85"/>
       <c r="D12" s="10">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="88"/>
-      <c r="M12" s="88"/>
-      <c r="N12" s="88"/>
-      <c r="O12" s="88"/>
-      <c r="P12" s="88"/>
-      <c r="Q12" s="88"/>
-      <c r="R12" s="88"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
-      <c r="A13" s="85"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="87"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="84"/>
+      <c r="C13" s="85"/>
       <c r="D13" s="10">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="88"/>
-      <c r="M13" s="88"/>
-      <c r="N13" s="88"/>
-      <c r="O13" s="88"/>
-      <c r="P13" s="88"/>
-      <c r="Q13" s="88"/>
-      <c r="R13" s="88"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="M13" s="86"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="86"/>
+      <c r="P13" s="86"/>
+      <c r="Q13" s="86"/>
+      <c r="R13" s="86"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="5"/>
@@ -5308,14 +5307,14 @@
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:18" ht="94.5" customHeight="1">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
+      <c r="B15" s="57"/>
+      <c r="C15" s="57"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
@@ -5380,7 +5379,7 @@
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13:B17"/>
     </sheetView>
   </sheetViews>
@@ -5393,32 +5392,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="79"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="81"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="79"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
       </c>
@@ -5433,92 +5432,92 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="80" t="s">
-        <v>198</v>
-      </c>
-      <c r="C3" s="59" t="s">
+      <c r="B3" s="78" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="57" t="s">
         <v>53</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="88" t="s">
-        <v>202</v>
-      </c>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
+      <c r="F3" s="86" t="s">
+        <v>201</v>
+      </c>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1">
-      <c r="A4" s="85"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="59"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="88" t="s">
-        <v>203</v>
-      </c>
-      <c r="G4" s="88"/>
-      <c r="H4" s="88"/>
+      <c r="F4" s="86" t="s">
+        <v>202</v>
+      </c>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="45" customHeight="1">
-      <c r="A5" s="85"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="59"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="88" t="s">
-        <v>204</v>
-      </c>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
+      <c r="F5" s="86" t="s">
+        <v>203</v>
+      </c>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="59"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="88" t="s">
-        <v>205</v>
-      </c>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88"/>
+      <c r="F6" s="86" t="s">
+        <v>204</v>
+      </c>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="45" customHeight="1">
-      <c r="A7" s="85"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="59"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="88" t="s">
-        <v>206</v>
-      </c>
-      <c r="G7" s="88"/>
-      <c r="H7" s="88"/>
+      <c r="F7" s="86" t="s">
+        <v>205</v>
+      </c>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
@@ -5540,8 +5539,8 @@
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="58" t="s">
-        <v>200</v>
+      <c r="B9" s="56" t="s">
+        <v>199</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>47</v>
@@ -5550,11 +5549,11 @@
         <v>35</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="88" t="s">
-        <v>199</v>
-      </c>
-      <c r="G9" s="88"/>
-      <c r="H9" s="88"/>
+      <c r="F9" s="86" t="s">
+        <v>198</v>
+      </c>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
@@ -5569,7 +5568,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5"/>
-      <c r="O10" s="58"/>
+      <c r="O10" s="56"/>
     </row>
     <row r="11" spans="1:15" ht="30">
       <c r="A11" s="10" t="s">
@@ -5597,7 +5596,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
-      <c r="O11" s="58"/>
+      <c r="O11" s="56"/>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="10"/>
@@ -5611,16 +5610,16 @@
       <c r="I12" s="2"/>
       <c r="J12" s="4"/>
       <c r="K12" s="5"/>
-      <c r="O12" s="58"/>
+      <c r="O12" s="56"/>
     </row>
     <row r="13" spans="1:15" ht="60" customHeight="1">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="83" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="80" t="s">
-        <v>220</v>
-      </c>
-      <c r="C13" s="84" t="s">
+      <c r="B13" s="78" t="s">
+        <v>219</v>
+      </c>
+      <c r="C13" s="82" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="2">
@@ -5628,61 +5627,61 @@
       </c>
       <c r="E13" s="5"/>
       <c r="H13" s="42" t="s">
-        <v>215</v>
-      </c>
-      <c r="O13" s="58"/>
+        <v>214</v>
+      </c>
+      <c r="O13" s="56"/>
     </row>
     <row r="14" spans="1:15" ht="60" customHeight="1">
-      <c r="A14" s="85"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="84"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="82"/>
       <c r="D14" s="2">
         <v>200437</v>
       </c>
       <c r="E14" s="5"/>
       <c r="H14" s="42" t="s">
-        <v>216</v>
-      </c>
-      <c r="O14" s="58"/>
+        <v>215</v>
+      </c>
+      <c r="O14" s="56"/>
     </row>
     <row r="15" spans="1:15" ht="60" customHeight="1">
-      <c r="A15" s="85"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="84"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="78"/>
+      <c r="C15" s="82"/>
       <c r="D15" s="2">
         <v>310111</v>
       </c>
       <c r="E15" s="5"/>
       <c r="H15" s="42" t="s">
-        <v>217</v>
-      </c>
-      <c r="O15" s="58"/>
+        <v>216</v>
+      </c>
+      <c r="O15" s="56"/>
     </row>
     <row r="16" spans="1:15" ht="60" customHeight="1">
-      <c r="A16" s="85"/>
-      <c r="B16" s="80"/>
-      <c r="C16" s="84"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="82"/>
       <c r="D16" s="2">
         <v>528401</v>
       </c>
       <c r="E16" s="5"/>
       <c r="H16" s="42" t="s">
-        <v>218</v>
-      </c>
-      <c r="O16" s="58"/>
+        <v>217</v>
+      </c>
+      <c r="O16" s="56"/>
     </row>
     <row r="17" spans="1:15" ht="60" customHeight="1">
-      <c r="A17" s="85"/>
-      <c r="B17" s="80"/>
-      <c r="C17" s="84"/>
+      <c r="A17" s="83"/>
+      <c r="B17" s="78"/>
+      <c r="C17" s="82"/>
       <c r="D17" s="2">
         <v>1076753</v>
       </c>
       <c r="E17" s="5"/>
       <c r="H17" s="42" t="s">
-        <v>219</v>
-      </c>
-      <c r="O17" s="58"/>
+        <v>218</v>
+      </c>
+      <c r="O17" s="56"/>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="10"/>
@@ -5701,7 +5700,7 @@
       <c r="A19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="80" t="s">
+      <c r="B19" s="78" t="s">
         <v>43</v>
       </c>
       <c r="C19" s="18" t="s">
@@ -5722,7 +5721,7 @@
     </row>
     <row r="20" spans="1:15" ht="30" customHeight="1">
       <c r="A20" s="10"/>
-      <c r="B20" s="80"/>
+      <c r="B20" s="78"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
@@ -5735,7 +5734,7 @@
       <c r="A21" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="80"/>
+      <c r="B21" s="78"/>
       <c r="C21" s="18" t="s">
         <v>68</v>
       </c>
@@ -5764,14 +5763,14 @@
       <c r="K22" s="5"/>
     </row>
     <row r="23" spans="1:15" ht="75" customHeight="1">
-      <c r="A23" s="59" t="s">
+      <c r="A23" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="57"/>
+      <c r="F23" s="57"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
@@ -5822,8 +5821,8 @@
   </sheetPr>
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F9"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5845,13 +5844,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
       <c r="J1" s="9"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -5899,34 +5898,26 @@
       </c>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="75">
-      <c r="A3" s="85" t="s">
+    <row r="3" spans="1:14" ht="45">
+      <c r="A3" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="55" t="s">
-        <v>190</v>
-      </c>
-      <c r="C3" s="83" t="s">
+      <c r="B3" s="53" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="81" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="10">
         <v>145879</v>
       </c>
-      <c r="E3" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="F3" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="I3" s="48" t="s">
-        <v>131</v>
-      </c>
+      <c r="E3" s="76" t="s">
+        <v>221</v>
+      </c>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="41"/>
       <c r="J3" s="41"/>
       <c r="K3" s="2" t="s">
         <v>2</v>
@@ -5939,11 +5930,11 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1">
-      <c r="A4" s="85"/>
-      <c r="B4" s="80" t="s">
+      <c r="A4" s="83"/>
+      <c r="B4" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="C4" s="92"/>
+      <c r="C4" s="90"/>
       <c r="D4" s="10">
         <v>200437</v>
       </c>
@@ -5968,9 +5959,9 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1">
-      <c r="A5" s="85"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="92"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="90"/>
       <c r="D5" s="10">
         <v>310111</v>
       </c>
@@ -5995,9 +5986,9 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="92"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="90"/>
       <c r="D6" s="10">
         <v>528401</v>
       </c>
@@ -6022,9 +6013,9 @@
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1">
-      <c r="A7" s="85"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="92"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="90"/>
       <c r="D7" s="10">
         <v>1076753</v>
       </c>
@@ -6053,14 +6044,14 @@
       <c r="M8" s="5"/>
     </row>
     <row r="9" spans="1:14" ht="90" customHeight="1">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
@@ -6078,12 +6069,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C3:C7"/>
+    <mergeCell ref="E3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -6124,13 +6116,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
       <c r="J1" s="9"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -6235,30 +6227,30 @@
       <c r="M4" s="2"/>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="57"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
     </row>
     <row r="7" spans="1:14" ht="90" customHeight="1">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="59"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -6311,29 +6303,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="49.5" customHeight="1">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="79" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="81"/>
+      <c r="G1" s="79"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="79"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="81"/>
+      <c r="A2" s="77"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="79"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>40</v>
@@ -6343,13 +6335,13 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="36" customHeight="1">
-      <c r="A3" s="85" t="s">
+      <c r="A3" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="78" t="s">
         <v>189</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="57" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="2">
@@ -6361,9 +6353,9 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="36" customHeight="1">
-      <c r="A4" s="85"/>
-      <c r="B4" s="80"/>
-      <c r="C4" s="59"/>
+      <c r="A4" s="83"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="57"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
@@ -6373,9 +6365,9 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="36" customHeight="1">
-      <c r="A5" s="85"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="59"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="57"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
@@ -6385,9 +6377,9 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="36" customHeight="1">
-      <c r="A6" s="85"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="59"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
@@ -6397,9 +6389,9 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="36" customHeight="1">
-      <c r="A7" s="85"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="59"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="57"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
@@ -6419,7 +6411,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="53" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>49</v>
@@ -6513,13 +6505,13 @@
       <c r="N16" s="12"/>
     </row>
     <row r="17" spans="1:14" ht="54" customHeight="1">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="80" t="s">
         <v>148</v>
       </c>
       <c r="D17" s="5">
@@ -6532,9 +6524,9 @@
       <c r="N17" s="12"/>
     </row>
     <row r="18" spans="1:14" ht="54" customHeight="1">
-      <c r="A18" s="85"/>
-      <c r="B18" s="80"/>
-      <c r="C18" s="83"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="81"/>
       <c r="D18" s="5">
         <v>200437</v>
       </c>
@@ -6545,9 +6537,9 @@
       <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:14" ht="54" customHeight="1">
-      <c r="A19" s="85"/>
-      <c r="B19" s="80"/>
-      <c r="C19" s="83"/>
+      <c r="A19" s="83"/>
+      <c r="B19" s="78"/>
+      <c r="C19" s="81"/>
       <c r="D19" s="5">
         <v>310111</v>
       </c>
@@ -6558,9 +6550,9 @@
       <c r="N19" s="12"/>
     </row>
     <row r="20" spans="1:14" ht="54" customHeight="1">
-      <c r="A20" s="85"/>
-      <c r="B20" s="80"/>
-      <c r="C20" s="83"/>
+      <c r="A20" s="83"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="5">
         <v>528401</v>
       </c>
@@ -6571,9 +6563,9 @@
       <c r="N20" s="12"/>
     </row>
     <row r="21" spans="1:14" ht="54" customHeight="1">
-      <c r="A21" s="85"/>
-      <c r="B21" s="80"/>
-      <c r="C21" s="83"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="78"/>
+      <c r="C21" s="81"/>
       <c r="D21" s="5">
         <v>1076753</v>
       </c>
@@ -6592,13 +6584,13 @@
       <c r="N22" s="12"/>
     </row>
     <row r="23" spans="1:14" ht="54" customHeight="1">
-      <c r="A23" s="85" t="s">
+      <c r="A23" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="80" t="s">
+      <c r="B23" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="82" t="s">
+      <c r="C23" s="80" t="s">
         <v>118</v>
       </c>
       <c r="D23" s="5">
@@ -6611,9 +6603,9 @@
       <c r="N23" s="12"/>
     </row>
     <row r="24" spans="1:14" ht="54" customHeight="1">
-      <c r="A24" s="85"/>
-      <c r="B24" s="80"/>
-      <c r="C24" s="83"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="78"/>
+      <c r="C24" s="81"/>
       <c r="D24" s="5">
         <v>200437</v>
       </c>
@@ -6624,9 +6616,9 @@
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" ht="54" customHeight="1">
-      <c r="A25" s="85"/>
-      <c r="B25" s="80"/>
-      <c r="C25" s="83"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="78"/>
+      <c r="C25" s="81"/>
       <c r="D25" s="5">
         <v>310111</v>
       </c>
@@ -6636,9 +6628,9 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="54" customHeight="1">
-      <c r="A26" s="85"/>
-      <c r="B26" s="80"/>
-      <c r="C26" s="83"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="78"/>
+      <c r="C26" s="81"/>
       <c r="D26" s="5">
         <v>528401</v>
       </c>
@@ -6648,9 +6640,9 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="54" customHeight="1">
-      <c r="A27" s="85"/>
-      <c r="B27" s="80"/>
-      <c r="C27" s="83"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="78"/>
+      <c r="C27" s="81"/>
       <c r="D27" s="5">
         <v>1076753</v>
       </c>
@@ -6669,15 +6661,15 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:14" ht="99.95" customHeight="1">
-      <c r="A29" s="59" t="s">
+      <c r="A29" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="59"/>
+      <c r="B29" s="57"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="57"/>
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">

</xml_diff>

<commit_message>
More jobs finished, more questions addressed.
</commit_message>
<xml_diff>
--- a/mSigHdp-paper-tracking.xlsx
+++ b/mSigHdp-paper-tracking.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Lab\Rozen_Lab\practice\6_Mo_mSigHdp\mSigHdp_paper_sup_files_x1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F658FFD-99F0-4485-9071-E82A19926DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988A4617-E6A6-46D6-8999-E119BAE1716F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2010" yWindow="1005" windowWidth="15375" windowHeight="12855" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7755" yWindow="1215" windowWidth="20580" windowHeight="12855" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tool_info" sheetId="7" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="222">
   <si>
     <t>Google scholar citations</t>
   </si>
@@ -1944,15 +1944,30 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1965,23 +1980,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2514,8 +2514,8 @@
   </sheetPr>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2530,23 +2530,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="46.5" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="79" t="s">
+      <c r="C1" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="84" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="79"/>
+      <c r="G1" s="84"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
@@ -2555,10 +2555,10 @@
       <c r="M1" s="5"/>
     </row>
     <row r="2" spans="1:13" ht="30.75" customHeight="1">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
       <c r="E2" s="1"/>
       <c r="F2" s="8" t="s">
         <v>40</v>
@@ -2750,7 +2750,7 @@
       <c r="M12" s="5"/>
     </row>
     <row r="13" spans="1:13" ht="54" customHeight="1">
-      <c r="A13" s="83" t="s">
+      <c r="A13" s="76" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="78"/>
@@ -2761,7 +2761,7 @@
         <v>145879</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="86" t="s">
+      <c r="F13" s="81" t="s">
         <v>122</v>
       </c>
       <c r="G13" s="43" t="s">
@@ -2773,14 +2773,14 @@
       <c r="M13" s="5"/>
     </row>
     <row r="14" spans="1:13" ht="54" customHeight="1">
-      <c r="A14" s="83"/>
+      <c r="A14" s="76"/>
       <c r="B14" s="78"/>
       <c r="C14" s="91"/>
       <c r="D14" s="5">
         <v>200437</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="86"/>
+      <c r="F14" s="81"/>
       <c r="G14" s="43" t="s">
         <v>127</v>
       </c>
@@ -2790,14 +2790,14 @@
       <c r="M14" s="5"/>
     </row>
     <row r="15" spans="1:13" ht="54" customHeight="1">
-      <c r="A15" s="83"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="78"/>
       <c r="C15" s="91"/>
       <c r="D15" s="5">
         <v>310111</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="86"/>
+      <c r="F15" s="81"/>
       <c r="G15" s="44" t="s">
         <v>132</v>
       </c>
@@ -2807,14 +2807,14 @@
       <c r="M15" s="5"/>
     </row>
     <row r="16" spans="1:13" ht="54" customHeight="1">
-      <c r="A16" s="83"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="78"/>
       <c r="C16" s="91"/>
       <c r="D16" s="5">
         <v>528401</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="86"/>
+      <c r="F16" s="81"/>
       <c r="G16" s="44" t="s">
         <v>132</v>
       </c>
@@ -2824,14 +2824,14 @@
       <c r="M16" s="5"/>
     </row>
     <row r="17" spans="1:13" ht="54" customHeight="1">
-      <c r="A17" s="83"/>
+      <c r="A17" s="76"/>
       <c r="B17" s="78"/>
       <c r="C17" s="91"/>
       <c r="D17" s="5">
         <v>1076753</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="F17" s="86"/>
+      <c r="F17" s="81"/>
       <c r="G17" s="44" t="s">
         <v>132</v>
       </c>
@@ -2893,16 +2893,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="A20:G20"/>
     <mergeCell ref="F13:F17"/>
     <mergeCell ref="B11:B17"/>
     <mergeCell ref="C13:C17"/>
     <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2940,13 +2940,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
       <c r="J1" s="10"/>
       <c r="K1" s="11"/>
       <c r="L1" s="10"/>
@@ -2990,7 +2990,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="76" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="78" t="s">
@@ -3014,21 +3014,21 @@
       <c r="H3" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="I3" s="87" t="s">
+      <c r="I3" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="J3" s="83" t="s">
+      <c r="J3" s="76" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="83" t="s">
+      <c r="L3" s="76" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A4" s="83"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="78"/>
       <c r="C4" s="57"/>
       <c r="D4" s="2">
@@ -3043,13 +3043,13 @@
       <c r="G4" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I4" s="87"/>
-      <c r="J4" s="83"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="92"/>
-      <c r="L4" s="83"/>
+      <c r="L4" s="76"/>
     </row>
     <row r="5" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A5" s="83"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="78"/>
       <c r="C5" s="57"/>
       <c r="D5" s="2">
@@ -3064,13 +3064,13 @@
       <c r="G5" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I5" s="87"/>
-      <c r="J5" s="83"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="76"/>
       <c r="K5" s="92"/>
-      <c r="L5" s="83"/>
+      <c r="L5" s="76"/>
     </row>
     <row r="6" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A6" s="83"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="78"/>
       <c r="C6" s="57"/>
       <c r="D6" s="2">
@@ -3085,13 +3085,13 @@
       <c r="G6" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="83"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="76"/>
       <c r="K6" s="92"/>
-      <c r="L6" s="83"/>
+      <c r="L6" s="76"/>
     </row>
     <row r="7" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A7" s="83"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="78"/>
       <c r="C7" s="57"/>
       <c r="D7" s="2">
@@ -3106,10 +3106,10 @@
       <c r="G7" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="I7" s="87"/>
-      <c r="J7" s="83"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="76"/>
       <c r="K7" s="92"/>
-      <c r="L7" s="83"/>
+      <c r="L7" s="76"/>
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="10"/>
@@ -3259,13 +3259,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
       <c r="J1" s="10"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -3310,7 +3310,7 @@
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="76" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="78" t="s">
@@ -3322,94 +3322,94 @@
       <c r="D3" s="2">
         <v>145879</v>
       </c>
-      <c r="E3" s="86" t="s">
+      <c r="E3" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="F3" s="86" t="s">
+      <c r="F3" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="86" t="s">
+      <c r="G3" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="H3" s="86" t="s">
+      <c r="H3" s="81" t="s">
         <v>127</v>
       </c>
       <c r="I3" s="93" t="s">
         <v>127</v>
       </c>
-      <c r="J3" s="83" t="s">
+      <c r="J3" s="76" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="83" t="s">
+      <c r="L3" s="76" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A4" s="83"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="78"/>
       <c r="C4" s="57"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="93"/>
-      <c r="J4" s="83"/>
+      <c r="J4" s="76"/>
       <c r="K4" s="92"/>
-      <c r="L4" s="83"/>
+      <c r="L4" s="76"/>
     </row>
     <row r="5" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A5" s="83"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="78"/>
       <c r="C5" s="57"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
-      <c r="E5" s="86"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
       <c r="I5" s="93"/>
-      <c r="J5" s="83"/>
+      <c r="J5" s="76"/>
       <c r="K5" s="92"/>
-      <c r="L5" s="83"/>
+      <c r="L5" s="76"/>
     </row>
     <row r="6" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A6" s="83"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="78"/>
       <c r="C6" s="57"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
       <c r="I6" s="93"/>
-      <c r="J6" s="83"/>
+      <c r="J6" s="76"/>
       <c r="K6" s="92"/>
-      <c r="L6" s="83"/>
+      <c r="L6" s="76"/>
     </row>
     <row r="7" spans="1:13" ht="35.1" customHeight="1">
-      <c r="A7" s="83"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="78"/>
       <c r="C7" s="57"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
       <c r="I7" s="93"/>
-      <c r="J7" s="83"/>
+      <c r="J7" s="76"/>
       <c r="K7" s="92"/>
-      <c r="L7" s="83"/>
+      <c r="L7" s="76"/>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="10"/>
@@ -4244,6 +4244,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="C8:G8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="G23:G27"/>
     <mergeCell ref="G18:G22"/>
@@ -4251,11 +4256,6 @@
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="C12:E15"/>
     <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="C8:G8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:G10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4269,8 +4269,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25:H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4283,29 +4283,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="79"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="84"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
       </c>
@@ -4320,91 +4320,91 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="36" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="76" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="78" t="s">
         <v>197</v>
       </c>
-      <c r="C3" s="85" t="s">
+      <c r="C3" s="79" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="2">
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="76" t="s">
+      <c r="F3" s="82" t="s">
         <v>208</v>
       </c>
-      <c r="G3" s="76"/>
+      <c r="G3" s="82"/>
       <c r="H3" s="42"/>
       <c r="I3" s="55" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36" customHeight="1">
-      <c r="A4" s="83"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="78"/>
-      <c r="C4" s="85"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="76" t="s">
+      <c r="F4" s="82" t="s">
         <v>209</v>
       </c>
-      <c r="G4" s="76"/>
+      <c r="G4" s="82"/>
       <c r="H4" s="42"/>
       <c r="I4" s="55" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="36" customHeight="1">
-      <c r="A5" s="83"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="78"/>
-      <c r="C5" s="85"/>
+      <c r="C5" s="79"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="76" t="s">
+      <c r="F5" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="G5" s="76"/>
+      <c r="G5" s="82"/>
       <c r="H5" s="42"/>
       <c r="I5" s="55" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1">
-      <c r="A6" s="83"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="78"/>
-      <c r="C6" s="85"/>
+      <c r="C6" s="79"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="76" t="s">
+      <c r="F6" s="82" t="s">
         <v>211</v>
       </c>
-      <c r="G6" s="76"/>
+      <c r="G6" s="82"/>
       <c r="H6" s="42"/>
       <c r="I6" s="55" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36" customHeight="1">
-      <c r="A7" s="83"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="78"/>
-      <c r="C7" s="85"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="76" t="s">
+      <c r="F7" s="82" t="s">
         <v>212</v>
       </c>
-      <c r="G7" s="76"/>
+      <c r="G7" s="82"/>
       <c r="H7" s="42"/>
       <c r="I7" s="55" t="s">
         <v>129</v>
@@ -4418,7 +4418,7 @@
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="45">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="76" t="s">
         <v>121</v>
       </c>
       <c r="B9" s="78" t="s">
@@ -4431,10 +4431,10 @@
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="86" t="s">
+      <c r="F9" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="G9" s="86" t="s">
+      <c r="G9" s="81" t="s">
         <v>139</v>
       </c>
       <c r="H9" s="52" t="s">
@@ -4442,57 +4442,57 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="36" customHeight="1">
-      <c r="A10" s="83"/>
-      <c r="B10" s="84"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="88"/>
       <c r="C10" s="57"/>
       <c r="D10" s="2">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
       <c r="H10" s="47" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="36" customHeight="1">
-      <c r="A11" s="83"/>
-      <c r="B11" s="84"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="88"/>
       <c r="C11" s="57"/>
       <c r="D11" s="2">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
       <c r="H11" s="47" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="36" customHeight="1">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="88"/>
       <c r="C12" s="57"/>
       <c r="D12" s="2">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
       <c r="H12" s="47" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="36" customHeight="1">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="88"/>
       <c r="C13" s="57"/>
       <c r="D13" s="2">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
       <c r="H13" s="47" t="s">
         <v>129</v>
       </c>
@@ -4508,87 +4508,87 @@
       <c r="H14" s="50"/>
     </row>
     <row r="15" spans="1:9" ht="54" customHeight="1">
-      <c r="A15" s="83" t="s">
+      <c r="A15" s="76" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="78" t="s">
         <v>200</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="79" t="s">
         <v>55</v>
       </c>
       <c r="D15" s="2">
         <v>145879</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="86" t="s">
+      <c r="F15" s="81" t="s">
         <v>192</v>
       </c>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86"/>
-      <c r="I15" s="87" t="s">
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="80" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="54" customHeight="1">
-      <c r="A16" s="83"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="78"/>
-      <c r="C16" s="85"/>
+      <c r="C16" s="79"/>
       <c r="D16" s="2">
         <v>200437</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="86" t="s">
+      <c r="F16" s="81" t="s">
         <v>193</v>
       </c>
-      <c r="G16" s="86"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="87"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="80"/>
     </row>
     <row r="17" spans="1:9" ht="54" customHeight="1">
-      <c r="A17" s="83"/>
+      <c r="A17" s="76"/>
       <c r="B17" s="78"/>
-      <c r="C17" s="85"/>
+      <c r="C17" s="79"/>
       <c r="D17" s="2">
         <v>310111</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="86" t="s">
+      <c r="F17" s="81" t="s">
         <v>194</v>
       </c>
-      <c r="G17" s="86"/>
-      <c r="H17" s="86"/>
-      <c r="I17" s="87"/>
+      <c r="G17" s="81"/>
+      <c r="H17" s="81"/>
+      <c r="I17" s="80"/>
     </row>
     <row r="18" spans="1:9" ht="54" customHeight="1">
-      <c r="A18" s="83"/>
+      <c r="A18" s="76"/>
       <c r="B18" s="78"/>
-      <c r="C18" s="85"/>
+      <c r="C18" s="79"/>
       <c r="D18" s="2">
         <v>528401</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="86" t="s">
+      <c r="F18" s="81" t="s">
         <v>195</v>
       </c>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="87"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="80"/>
     </row>
     <row r="19" spans="1:9" ht="54" customHeight="1">
-      <c r="A19" s="83"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="78"/>
-      <c r="C19" s="85"/>
+      <c r="C19" s="79"/>
       <c r="D19" s="2">
         <v>1076753</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="86" t="s">
+      <c r="F19" s="81" t="s">
         <v>196</v>
       </c>
-      <c r="G19" s="86"/>
-      <c r="H19" s="86"/>
-      <c r="I19" s="87"/>
+      <c r="G19" s="81"/>
+      <c r="H19" s="81"/>
+      <c r="I19" s="80"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2"/>
@@ -4637,13 +4637,13 @@
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:9" ht="45">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="76" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="83" t="s">
+      <c r="C23" s="76" t="s">
         <v>57</v>
       </c>
       <c r="D23" s="5">
@@ -4658,9 +4658,9 @@
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9" ht="45">
-      <c r="A24" s="83"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="83"/>
+      <c r="A24" s="76"/>
+      <c r="B24" s="77"/>
+      <c r="C24" s="76"/>
       <c r="D24" s="5">
         <v>200437</v>
       </c>
@@ -4673,46 +4673,46 @@
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9" ht="45" customHeight="1">
-      <c r="A25" s="83"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="83"/>
+      <c r="A25" s="76"/>
+      <c r="B25" s="77"/>
+      <c r="C25" s="76"/>
       <c r="D25" s="5">
         <v>310111</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25"/>
       <c r="G25"/>
-      <c r="H25" s="43" t="s">
+      <c r="H25" s="89" t="s">
         <v>213</v>
       </c>
       <c r="I25"/>
     </row>
     <row r="26" spans="1:9" ht="45" customHeight="1">
-      <c r="A26" s="83"/>
-      <c r="B26" s="88"/>
-      <c r="C26" s="83"/>
+      <c r="A26" s="76"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="76"/>
       <c r="D26" s="5">
         <v>528401</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26"/>
       <c r="G26"/>
-      <c r="H26" s="76" t="s">
-        <v>213</v>
-      </c>
+      <c r="H26" s="89"/>
       <c r="I26"/>
     </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="83"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="83"/>
+    <row r="27" spans="1:9" ht="45">
+      <c r="A27" s="76"/>
+      <c r="B27" s="77"/>
+      <c r="C27" s="76"/>
       <c r="D27" s="5">
         <v>1076753</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27"/>
       <c r="G27"/>
-      <c r="H27" s="76"/>
+      <c r="H27" s="52" t="s">
+        <v>213</v>
+      </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
@@ -4726,13 +4726,13 @@
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:9" ht="54" customHeight="1">
-      <c r="A29" s="82" t="s">
+      <c r="A29" s="87" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="80" t="s">
+      <c r="C29" s="85" t="s">
         <v>67</v>
       </c>
       <c r="D29" s="5">
@@ -4746,9 +4746,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" ht="54" customHeight="1">
-      <c r="A30" s="82"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="78"/>
-      <c r="C30" s="81"/>
+      <c r="C30" s="86"/>
       <c r="D30" s="5">
         <v>200437</v>
       </c>
@@ -4760,9 +4760,9 @@
       </c>
     </row>
     <row r="31" spans="1:9" ht="54" customHeight="1">
-      <c r="A31" s="82"/>
+      <c r="A31" s="87"/>
       <c r="B31" s="78"/>
-      <c r="C31" s="81"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="5">
         <v>310111</v>
       </c>
@@ -4774,9 +4774,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" ht="54" customHeight="1">
-      <c r="A32" s="82"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="78"/>
-      <c r="C32" s="81"/>
+      <c r="C32" s="86"/>
       <c r="D32" s="5">
         <v>528401</v>
       </c>
@@ -4788,9 +4788,9 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="54" customHeight="1">
-      <c r="A33" s="82"/>
+      <c r="A33" s="87"/>
       <c r="B33" s="78"/>
-      <c r="C33" s="81"/>
+      <c r="C33" s="86"/>
       <c r="D33" s="5">
         <v>1076753</v>
       </c>
@@ -4876,26 +4876,7 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="I15:I19"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F9:F13"/>
-    <mergeCell ref="G9:G13"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="H25:H26"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="B29:B35"/>
@@ -4911,6 +4892,25 @@
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="A3:A7"/>
+    <mergeCell ref="F9:F13"/>
+    <mergeCell ref="G9:G13"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="I15:I19"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="A15:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4937,40 +4937,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="50.1" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="84" t="s">
         <v>174</v>
       </c>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="M1" s="79" t="s">
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="M1" s="84" t="s">
         <v>175</v>
       </c>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="79"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="84"/>
       <c r="F2" s="9">
         <v>5</v>
       </c>
@@ -5009,7 +5009,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" ht="68.25" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="76" t="s">
         <v>121</v>
       </c>
       <c r="B3" s="78" t="s">
@@ -5060,8 +5060,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" ht="75" customHeight="1">
-      <c r="A4" s="83"/>
-      <c r="B4" s="84"/>
+      <c r="A4" s="76"/>
+      <c r="B4" s="88"/>
       <c r="C4" s="57"/>
       <c r="D4" s="10">
         <v>200437</v>
@@ -5091,8 +5091,8 @@
       <c r="R4" s="89"/>
     </row>
     <row r="5" spans="1:18" ht="36" customHeight="1">
-      <c r="A5" s="83"/>
-      <c r="B5" s="84"/>
+      <c r="A5" s="76"/>
+      <c r="B5" s="88"/>
       <c r="C5" s="57"/>
       <c r="D5" s="10">
         <v>310111</v>
@@ -5112,8 +5112,8 @@
       <c r="R5" s="89"/>
     </row>
     <row r="6" spans="1:18" ht="36" customHeight="1">
-      <c r="A6" s="83"/>
-      <c r="B6" s="84"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="88"/>
       <c r="C6" s="57"/>
       <c r="D6" s="10">
         <v>528401</v>
@@ -5133,8 +5133,8 @@
       <c r="R6" s="89"/>
     </row>
     <row r="7" spans="1:18" ht="36" customHeight="1">
-      <c r="A7" s="83"/>
-      <c r="B7" s="84"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="88"/>
       <c r="C7" s="57"/>
       <c r="D7" s="10">
         <v>1076753</v>
@@ -5162,139 +5162,139 @@
       <c r="H8" s="41"/>
     </row>
     <row r="9" spans="1:18" ht="54" customHeight="1">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="76" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="85" t="s">
+      <c r="C9" s="79" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="10">
         <v>145879</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="86" t="s">
+      <c r="F9" s="81" t="s">
         <v>145</v>
       </c>
-      <c r="G9" s="86" t="s">
+      <c r="G9" s="81" t="s">
         <v>146</v>
       </c>
-      <c r="H9" s="86" t="s">
+      <c r="H9" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="I9" s="86" t="s">
+      <c r="I9" s="81" t="s">
         <v>160</v>
       </c>
-      <c r="J9" s="86" t="s">
+      <c r="J9" s="81" t="s">
         <v>161</v>
       </c>
-      <c r="K9" s="86" t="s">
+      <c r="K9" s="81" t="s">
         <v>168</v>
       </c>
-      <c r="M9" s="86" t="s">
+      <c r="M9" s="81" t="s">
         <v>182</v>
       </c>
-      <c r="N9" s="86" t="s">
+      <c r="N9" s="81" t="s">
         <v>183</v>
       </c>
-      <c r="O9" s="86" t="s">
+      <c r="O9" s="81" t="s">
         <v>184</v>
       </c>
-      <c r="P9" s="86" t="s">
+      <c r="P9" s="81" t="s">
         <v>185</v>
       </c>
-      <c r="Q9" s="86" t="s">
+      <c r="Q9" s="81" t="s">
         <v>186</v>
       </c>
-      <c r="R9" s="86" t="s">
+      <c r="R9" s="81" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="54" customHeight="1">
-      <c r="A10" s="83"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="85"/>
+      <c r="A10" s="76"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="79"/>
       <c r="D10" s="10">
         <v>200437</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="86"/>
-      <c r="Q10" s="86"/>
-      <c r="R10" s="86"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="81"/>
+      <c r="K10" s="81"/>
+      <c r="M10" s="81"/>
+      <c r="N10" s="81"/>
+      <c r="O10" s="81"/>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="81"/>
+      <c r="R10" s="81"/>
     </row>
     <row r="11" spans="1:18" ht="54" customHeight="1">
-      <c r="A11" s="83"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="85"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="10">
         <v>310111</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="86"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="86"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="86"/>
-      <c r="M11" s="86"/>
-      <c r="N11" s="86"/>
-      <c r="O11" s="86"/>
-      <c r="P11" s="86"/>
-      <c r="Q11" s="86"/>
-      <c r="R11" s="86"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="81"/>
+      <c r="K11" s="81"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="81"/>
+      <c r="R11" s="81"/>
     </row>
     <row r="12" spans="1:18" ht="54" customHeight="1">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="85"/>
+      <c r="A12" s="76"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="79"/>
       <c r="D12" s="10">
         <v>528401</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="86"/>
-      <c r="G12" s="86"/>
-      <c r="H12" s="86"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="86"/>
-      <c r="M12" s="86"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="86"/>
-      <c r="P12" s="86"/>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="86"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="81"/>
+      <c r="K12" s="81"/>
+      <c r="M12" s="81"/>
+      <c r="N12" s="81"/>
+      <c r="O12" s="81"/>
+      <c r="P12" s="81"/>
+      <c r="Q12" s="81"/>
+      <c r="R12" s="81"/>
     </row>
     <row r="13" spans="1:18" ht="54" customHeight="1">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="85"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="10">
         <v>1076753</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="86"/>
-      <c r="H13" s="86"/>
-      <c r="I13" s="86"/>
-      <c r="J13" s="86"/>
-      <c r="K13" s="86"/>
-      <c r="M13" s="86"/>
-      <c r="N13" s="86"/>
-      <c r="O13" s="86"/>
-      <c r="P13" s="86"/>
-      <c r="Q13" s="86"/>
-      <c r="R13" s="86"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="81"/>
+      <c r="K13" s="81"/>
+      <c r="M13" s="81"/>
+      <c r="N13" s="81"/>
+      <c r="O13" s="81"/>
+      <c r="P13" s="81"/>
+      <c r="Q13" s="81"/>
+      <c r="R13" s="81"/>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" s="5"/>
@@ -5328,28 +5328,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="M3:M7"/>
-    <mergeCell ref="N3:N7"/>
-    <mergeCell ref="O3:O7"/>
-    <mergeCell ref="P3:P7"/>
-    <mergeCell ref="M9:M13"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="N9:N13"/>
-    <mergeCell ref="O9:O13"/>
-    <mergeCell ref="P9:P13"/>
-    <mergeCell ref="Q9:Q13"/>
-    <mergeCell ref="R9:R13"/>
-    <mergeCell ref="Q3:Q7"/>
-    <mergeCell ref="R3:R7"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B7"/>
-    <mergeCell ref="C3:C7"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="K9:K13"/>
     <mergeCell ref="J9:J13"/>
@@ -5365,6 +5343,28 @@
     <mergeCell ref="K3:K7"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="H4:H7"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="C3:C7"/>
+    <mergeCell ref="P3:P7"/>
+    <mergeCell ref="M9:M13"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="N9:N13"/>
+    <mergeCell ref="O9:O13"/>
+    <mergeCell ref="P9:P13"/>
+    <mergeCell ref="Q9:Q13"/>
+    <mergeCell ref="R9:R13"/>
+    <mergeCell ref="Q3:Q7"/>
+    <mergeCell ref="R3:R7"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="M3:M7"/>
+    <mergeCell ref="N3:N7"/>
+    <mergeCell ref="O3:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5379,8 +5379,8 @@
   </sheetPr>
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5392,32 +5392,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="84" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:15">
-      <c r="A2" s="77"/>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="79"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="84"/>
       <c r="F2" s="9" t="s">
         <v>39</v>
       </c>
@@ -5432,7 +5432,7 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="76" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="78" t="s">
@@ -5445,79 +5445,79 @@
         <v>145879</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="86" t="s">
+      <c r="F3" s="81" t="s">
         <v>201</v>
       </c>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
       <c r="I3" s="2"/>
       <c r="J3" s="3"/>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:15" ht="45" customHeight="1">
-      <c r="A4" s="83"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="78"/>
       <c r="C4" s="57"/>
       <c r="D4" s="2">
         <v>200437</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="86" t="s">
+      <c r="F4" s="81" t="s">
         <v>202</v>
       </c>
-      <c r="G4" s="86"/>
-      <c r="H4" s="86"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="I4" s="2"/>
       <c r="J4" s="3"/>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:15" ht="45" customHeight="1">
-      <c r="A5" s="83"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="78"/>
       <c r="C5" s="57"/>
       <c r="D5" s="2">
         <v>310111</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="86" t="s">
+      <c r="F5" s="81" t="s">
         <v>203</v>
       </c>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
       <c r="I5" s="2"/>
       <c r="J5" s="3"/>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:15" ht="45" customHeight="1">
-      <c r="A6" s="83"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="78"/>
       <c r="C6" s="57"/>
       <c r="D6" s="2">
         <v>528401</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="86" t="s">
+      <c r="F6" s="81" t="s">
         <v>204</v>
       </c>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
+      <c r="G6" s="81"/>
+      <c r="H6" s="81"/>
       <c r="I6" s="2"/>
       <c r="J6" s="3"/>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:15" ht="45" customHeight="1">
-      <c r="A7" s="83"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="78"/>
       <c r="C7" s="57"/>
       <c r="D7" s="2">
         <v>1076753</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="86" t="s">
+      <c r="F7" s="81" t="s">
         <v>205</v>
       </c>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="81"/>
       <c r="I7" s="2"/>
       <c r="J7" s="3"/>
       <c r="K7" s="2"/>
@@ -5549,11 +5549,11 @@
         <v>35</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="86" t="s">
+      <c r="F9" s="81" t="s">
         <v>198</v>
       </c>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
       <c r="J9" s="4"/>
       <c r="K9" s="5"/>
     </row>
@@ -5613,74 +5613,84 @@
       <c r="O12" s="56"/>
     </row>
     <row r="13" spans="1:15" ht="60" customHeight="1">
-      <c r="A13" s="83" t="s">
+      <c r="A13" s="76" t="s">
         <v>26</v>
       </c>
       <c r="B13" s="78" t="s">
         <v>219</v>
       </c>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="87" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="2">
         <v>145879</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="H13" s="42" t="s">
+      <c r="F13" s="89" t="s">
         <v>214</v>
       </c>
+      <c r="G13" s="89"/>
+      <c r="H13" s="89"/>
       <c r="O13" s="56"/>
     </row>
     <row r="14" spans="1:15" ht="60" customHeight="1">
-      <c r="A14" s="83"/>
+      <c r="A14" s="76"/>
       <c r="B14" s="78"/>
-      <c r="C14" s="82"/>
+      <c r="C14" s="87"/>
       <c r="D14" s="2">
         <v>200437</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="H14" s="42" t="s">
+      <c r="F14" s="89" t="s">
         <v>215</v>
       </c>
+      <c r="G14" s="89"/>
+      <c r="H14" s="89"/>
       <c r="O14" s="56"/>
     </row>
     <row r="15" spans="1:15" ht="60" customHeight="1">
-      <c r="A15" s="83"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="78"/>
-      <c r="C15" s="82"/>
+      <c r="C15" s="87"/>
       <c r="D15" s="2">
         <v>310111</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="H15" s="42" t="s">
+      <c r="F15" s="89" t="s">
         <v>216</v>
       </c>
+      <c r="G15" s="89"/>
+      <c r="H15" s="89"/>
       <c r="O15" s="56"/>
     </row>
     <row r="16" spans="1:15" ht="60" customHeight="1">
-      <c r="A16" s="83"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="78"/>
-      <c r="C16" s="82"/>
+      <c r="C16" s="87"/>
       <c r="D16" s="2">
         <v>528401</v>
       </c>
       <c r="E16" s="5"/>
-      <c r="H16" s="42" t="s">
+      <c r="F16" s="89" t="s">
         <v>217</v>
       </c>
+      <c r="G16" s="89"/>
+      <c r="H16" s="89"/>
       <c r="O16" s="56"/>
     </row>
     <row r="17" spans="1:15" ht="60" customHeight="1">
-      <c r="A17" s="83"/>
+      <c r="A17" s="76"/>
       <c r="B17" s="78"/>
-      <c r="C17" s="82"/>
+      <c r="C17" s="87"/>
       <c r="D17" s="2">
         <v>1076753</v>
       </c>
       <c r="E17" s="5"/>
-      <c r="H17" s="42" t="s">
+      <c r="F17" s="89" t="s">
         <v>218</v>
       </c>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
       <c r="O17" s="56"/>
     </row>
     <row r="18" spans="1:15">
@@ -5788,7 +5798,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="24">
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="F16:H16"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="C13:C17"/>
@@ -5805,9 +5823,6 @@
     <mergeCell ref="C3:C7"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5822,7 +5837,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:H3"/>
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5844,13 +5859,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
       <c r="J1" s="9"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -5899,24 +5914,26 @@
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="45">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="76" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="53" t="s">
         <v>220</v>
       </c>
-      <c r="C3" s="81" t="s">
+      <c r="C3" s="86" t="s">
         <v>51</v>
       </c>
       <c r="D3" s="10">
         <v>145879</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
+      <c r="F3" s="82" t="s">
+        <v>221</v>
+      </c>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
       <c r="I3" s="41"/>
       <c r="J3" s="41"/>
       <c r="K3" s="2" t="s">
@@ -5930,7 +5947,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="30" customHeight="1">
-      <c r="A4" s="83"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="78" t="s">
         <v>189</v>
       </c>
@@ -5959,7 +5976,7 @@
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1">
-      <c r="A5" s="83"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="78"/>
       <c r="C5" s="90"/>
       <c r="D5" s="10">
@@ -5986,7 +6003,7 @@
       <c r="M5" s="2"/>
     </row>
     <row r="6" spans="1:14" ht="30" customHeight="1">
-      <c r="A6" s="83"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="78"/>
       <c r="C6" s="90"/>
       <c r="D6" s="10">
@@ -6013,7 +6030,7 @@
       <c r="M6" s="2"/>
     </row>
     <row r="7" spans="1:14" ht="30" customHeight="1">
-      <c r="A7" s="83"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="78"/>
       <c r="C7" s="90"/>
       <c r="D7" s="10">
@@ -6075,7 +6092,7 @@
     <mergeCell ref="E1:I1"/>
     <mergeCell ref="B4:B7"/>
     <mergeCell ref="C3:C7"/>
-    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
@@ -6116,13 +6133,13 @@
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
-      <c r="E1" s="77" t="s">
+      <c r="E1" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
       <c r="J1" s="9"/>
       <c r="K1" s="10"/>
       <c r="L1" s="10"/>
@@ -6289,8 +6306,8 @@
   </sheetPr>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6303,29 +6320,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="49.5" customHeight="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="79" t="s">
+      <c r="B1" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="83" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="79" t="s">
+      <c r="D1" s="84" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="79"/>
+      <c r="G1" s="84"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="77"/>
-      <c r="B2" s="79"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="79"/>
+      <c r="A2" s="83"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="84"/>
       <c r="E2" s="1"/>
       <c r="F2" s="9" t="s">
         <v>40</v>
@@ -6335,7 +6352,7 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="36" customHeight="1">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="76" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="78" t="s">
@@ -6353,7 +6370,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="36" customHeight="1">
-      <c r="A4" s="83"/>
+      <c r="A4" s="76"/>
       <c r="B4" s="78"/>
       <c r="C4" s="57"/>
       <c r="D4" s="2">
@@ -6365,7 +6382,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="36" customHeight="1">
-      <c r="A5" s="83"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="78"/>
       <c r="C5" s="57"/>
       <c r="D5" s="2">
@@ -6377,7 +6394,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="36" customHeight="1">
-      <c r="A6" s="83"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="78"/>
       <c r="C6" s="57"/>
       <c r="D6" s="2">
@@ -6389,7 +6406,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="36" customHeight="1">
-      <c r="A7" s="83"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="78"/>
       <c r="C7" s="57"/>
       <c r="D7" s="2">
@@ -6505,13 +6522,13 @@
       <c r="N16" s="12"/>
     </row>
     <row r="17" spans="1:14" ht="54" customHeight="1">
-      <c r="A17" s="83" t="s">
+      <c r="A17" s="76" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="80" t="s">
+      <c r="C17" s="85" t="s">
         <v>148</v>
       </c>
       <c r="D17" s="5">
@@ -6524,9 +6541,9 @@
       <c r="N17" s="12"/>
     </row>
     <row r="18" spans="1:14" ht="54" customHeight="1">
-      <c r="A18" s="83"/>
+      <c r="A18" s="76"/>
       <c r="B18" s="78"/>
-      <c r="C18" s="81"/>
+      <c r="C18" s="86"/>
       <c r="D18" s="5">
         <v>200437</v>
       </c>
@@ -6537,9 +6554,9 @@
       <c r="N18" s="12"/>
     </row>
     <row r="19" spans="1:14" ht="54" customHeight="1">
-      <c r="A19" s="83"/>
+      <c r="A19" s="76"/>
       <c r="B19" s="78"/>
-      <c r="C19" s="81"/>
+      <c r="C19" s="86"/>
       <c r="D19" s="5">
         <v>310111</v>
       </c>
@@ -6550,9 +6567,9 @@
       <c r="N19" s="12"/>
     </row>
     <row r="20" spans="1:14" ht="54" customHeight="1">
-      <c r="A20" s="83"/>
+      <c r="A20" s="76"/>
       <c r="B20" s="78"/>
-      <c r="C20" s="81"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="5">
         <v>528401</v>
       </c>
@@ -6563,9 +6580,9 @@
       <c r="N20" s="12"/>
     </row>
     <row r="21" spans="1:14" ht="54" customHeight="1">
-      <c r="A21" s="83"/>
+      <c r="A21" s="76"/>
       <c r="B21" s="78"/>
-      <c r="C21" s="81"/>
+      <c r="C21" s="86"/>
       <c r="D21" s="5">
         <v>1076753</v>
       </c>
@@ -6584,13 +6601,13 @@
       <c r="N22" s="12"/>
     </row>
     <row r="23" spans="1:14" ht="54" customHeight="1">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="76" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="80" t="s">
+      <c r="C23" s="85" t="s">
         <v>118</v>
       </c>
       <c r="D23" s="5">
@@ -6603,9 +6620,9 @@
       <c r="N23" s="12"/>
     </row>
     <row r="24" spans="1:14" ht="54" customHeight="1">
-      <c r="A24" s="83"/>
+      <c r="A24" s="76"/>
       <c r="B24" s="78"/>
-      <c r="C24" s="81"/>
+      <c r="C24" s="86"/>
       <c r="D24" s="5">
         <v>200437</v>
       </c>
@@ -6616,9 +6633,9 @@
       <c r="N24" s="12"/>
     </row>
     <row r="25" spans="1:14" ht="54" customHeight="1">
-      <c r="A25" s="83"/>
+      <c r="A25" s="76"/>
       <c r="B25" s="78"/>
-      <c r="C25" s="81"/>
+      <c r="C25" s="86"/>
       <c r="D25" s="5">
         <v>310111</v>
       </c>
@@ -6628,9 +6645,9 @@
       </c>
     </row>
     <row r="26" spans="1:14" ht="54" customHeight="1">
-      <c r="A26" s="83"/>
+      <c r="A26" s="76"/>
       <c r="B26" s="78"/>
-      <c r="C26" s="81"/>
+      <c r="C26" s="86"/>
       <c r="D26" s="5">
         <v>528401</v>
       </c>
@@ -6640,9 +6657,9 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="54" customHeight="1">
-      <c r="A27" s="83"/>
+      <c r="A27" s="76"/>
       <c r="B27" s="78"/>
-      <c r="C27" s="81"/>
+      <c r="C27" s="86"/>
       <c r="D27" s="5">
         <v>1076753</v>
       </c>

</xml_diff>